<commit_message>
WIP: Enhanced testsuite so that it now checks that a threadteam can be destroyed even if there are waiting and computing threads.  Ported the ThreadTeamState methods startTask and enqueue over to the NotThreadsafe version.
</commit_message>
<xml_diff>
--- a/docs/RuntimeDesign.xlsx
+++ b/docs/RuntimeDesign.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jared/Projects/OrchestrationRuntime/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C446294E-6687-6C4B-826F-E40D6F0E6DA3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF5F2A6A-909D-394C-AD4D-3B2D750DCCBB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="17560" xr2:uid="{9B8D0C4A-3FF1-A04E-B8F8-B86CE3BC2D78}"/>
   </bookViews>
@@ -2092,8 +2092,8 @@
   <dimension ref="A1:R111"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E3" sqref="E3:N3"/>
+      <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
WIP: Finished adding unittests of EFSM transtions.  The testsuite requires a thorough review and cleaning.
</commit_message>
<xml_diff>
--- a/docs/RuntimeDesign.xlsx
+++ b/docs/RuntimeDesign.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jared/Projects/OrchestrationRuntime/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B62EA42B-FF50-6D4A-A35F-A3B9E0610B8D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{063FDD71-FF99-2540-936F-6CA40A2F4252}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="17560" xr2:uid="{9B8D0C4A-3FF1-A04E-B8F8-B86CE3BC2D78}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="873" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="887" uniqueCount="146">
   <si>
     <t>Machine Mode</t>
   </si>
@@ -1171,8 +1171,28 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Call </t>
+    <t>N_c-1 &gt; 0</t>
+  </si>
+  <si>
+    <t>N_w &gt; 1</t>
+  </si>
+  <si>
+    <t>N_w-1 &gt;= 1</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Broadcast </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="8" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>unblock</t>
     </r>
     <r>
       <rPr>
@@ -1181,7 +1201,7 @@
         <color theme="8" tint="-0.249977111117893"/>
         <rFont val="Calibri (Body)_x0000_"/>
       </rPr>
-      <t>increaseThreadCount</t>
+      <t>WaitThread</t>
     </r>
     <r>
       <rPr>
@@ -1191,17 +1211,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>(i) of Thread Subscriber if exists</t>
-    </r>
-  </si>
-  <si>
-    <t>N_c-1 &gt; 0</t>
-  </si>
-  <si>
-    <t>N_w &gt; 1</t>
-  </si>
-  <si>
-    <t>N_w-1 &gt;= 1</t>
+      <t xml:space="preserve"> signal to wake all threads that called wait() if any</t>
+    </r>
   </si>
   <si>
     <r>
@@ -1225,7 +1236,7 @@
         <color theme="8" tint="-0.249977111117893"/>
         <rFont val="Calibri (Body)_x0000_"/>
       </rPr>
-      <t>WaitThread</t>
+      <t xml:space="preserve">WaitThread </t>
     </r>
     <r>
       <rPr>
@@ -1235,23 +1246,12 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> signal to wake all threads that called wait() if any</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Broadcast </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="8" tint="-0.249977111117893"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>unblock</t>
+      <t>signal to wake all threads that called wait() if any</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Transition Mode and then broadcast to all waiting threads the </t>
     </r>
     <r>
       <rPr>
@@ -1260,7 +1260,7 @@
         <color theme="8" tint="-0.249977111117893"/>
         <rFont val="Calibri (Body)_x0000_"/>
       </rPr>
-      <t xml:space="preserve">WaitThread </t>
+      <t>transitionThread</t>
     </r>
     <r>
       <rPr>
@@ -1270,12 +1270,88 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>signal to wake all threads that called wait() if any</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Transition Mode and then broadcast to all waiting threads the </t>
+      <t xml:space="preserve"> signal</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Only </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>startTask</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>increaseThreadCount</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> can emit </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF2F75B5"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>activateThread.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">  Both only emit if i &lt;= N_i - N_to_activate</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>0 &lt; N_i &lt; N_max</t>
+  </si>
+  <si>
+    <t>0 &lt;= N_i &lt; N_max</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">We are assuming that any threads that are Waiting have yet to receive the </t>
     </r>
     <r>
       <rPr>
@@ -1294,12 +1370,117 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t xml:space="preserve"> signal, but will.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Receiving thread transitions Mode and then broadcasts to all waiting threads the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="8" tint="-0.249977111117893"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>transitionThread</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve"> signal</t>
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Only </t>
+    <t>N_i+1 &lt; N_max</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Increment N_to_activate by i and emit </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="8" tint="-0.249977111117893"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>activateThread</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> event i times</t>
+    </r>
+  </si>
+  <si>
+    <t>Test name</t>
+  </si>
+  <si>
+    <t>TestInitialState</t>
+  </si>
+  <si>
+    <t>Internally</t>
+  </si>
+  <si>
+    <t>TestNoWorkNoThreads</t>
+  </si>
+  <si>
+    <t>TestIdleErrors</t>
+  </si>
+  <si>
+    <t>Many</t>
+  </si>
+  <si>
+    <t>TestIdleForwardsThreads</t>
+  </si>
+  <si>
+    <t>TestNoWork</t>
+  </si>
+  <si>
+    <t>TestRunningOpenErrors</t>
+  </si>
+  <si>
+    <t>TestRunningOpenIncreaseThreads</t>
+  </si>
+  <si>
+    <t>Nothing to test</t>
+  </si>
+  <si>
+    <t>TestRunningOpenEnqueue</t>
+  </si>
+  <si>
+    <t>TestRunningClosedErrors</t>
+  </si>
+  <si>
+    <t>TestRunningNoMoreWorkErrors</t>
+  </si>
+  <si>
+    <t>TestRunningClosedActivation</t>
+  </si>
+  <si>
+    <t>TestRunningClosedWorkPub</t>
+  </si>
+  <si>
+    <t>TestRunningNoMoreWorkForward</t>
+  </si>
+  <si>
+    <t>Do not know how to test directly</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Call </t>
     </r>
     <r>
       <rPr>
@@ -1308,212 +1489,37 @@
         <color theme="9" tint="-0.249977111117893"/>
         <rFont val="Calibri (Body)_x0000_"/>
       </rPr>
-      <t>startTask</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> and </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="9" tint="-0.249977111117893"/>
-        <rFont val="Calibri (Body)_x0000_"/>
-      </rPr>
       <t>increaseThreadCount</t>
     </r>
     <r>
       <rPr>
         <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> can emit </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FF2F75B5"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>activateThread.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t xml:space="preserve">  Both only emit if i &lt;= N_i - N_to_activate</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <t>0 &lt; N_i &lt; N_max</t>
-  </si>
-  <si>
-    <t>0 &lt;= N_i &lt; N_max</t>
-  </si>
-  <si>
-    <t>As for N_i=N_max-1 / N_w=1 transition</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">We are assuming that any threads that are Waiting have yet to receive the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="8" tint="-0.249977111117893"/>
-        <rFont val="Calibri (Body)_x0000_"/>
-      </rPr>
-      <t>transitionThread</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> signal, but will.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Receiving thread transitions Mode and then broadcasts to all waiting threads the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="8" tint="-0.249977111117893"/>
-        <rFont val="Calibri (Body)_x0000_"/>
-      </rPr>
-      <t>transitionThread</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> signal</t>
-    </r>
-  </si>
-  <si>
-    <t>N_i+1 &lt; N_max</t>
-  </si>
-  <si>
-    <t>As for N_i=N_max-1 / N_c=1 transition, except there is no work to enqueue first</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Increment N_to_activate by i and emit </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="8" tint="-0.249977111117893"/>
-        <rFont val="Calibri (Body)_x0000_"/>
-      </rPr>
-      <t>activateThread</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> event i times</t>
-    </r>
-  </si>
-  <si>
-    <t>Test name</t>
-  </si>
-  <si>
-    <t>TestInitialState</t>
-  </si>
-  <si>
-    <t>Internally</t>
-  </si>
-  <si>
-    <t>TestNoWorkNoThreads</t>
-  </si>
-  <si>
-    <t>TestIdleErrors</t>
-  </si>
-  <si>
-    <t>Many</t>
-  </si>
-  <si>
-    <t>???</t>
-  </si>
-  <si>
-    <t>TestIdleForwardsThreads</t>
-  </si>
-  <si>
-    <t>TestNoWork</t>
-  </si>
-  <si>
-    <t>TestRunningOpenErrors</t>
-  </si>
-  <si>
-    <t>TestRunningOpenIncreaseThreads</t>
-  </si>
-  <si>
-    <t>Nothing to test</t>
-  </si>
-  <si>
-    <t>TestRunningOpenEnqueue</t>
-  </si>
-  <si>
-    <t>TestRunningClosedErrors</t>
-  </si>
-  <si>
-    <t>TestRunningNoMoreWorkErrors</t>
-  </si>
-  <si>
-    <t>TestRunningClosedActivation</t>
-  </si>
-  <si>
-    <t>TestRunningClosedWorkPub</t>
-  </si>
-  <si>
-    <t>TestRunningNoMoreWorkForward</t>
+      <t>(i) of Thread Subscriber if exists</t>
+    </r>
+  </si>
+  <si>
+    <t>TestRunningNoMoreWorkTransition</t>
+  </si>
+  <si>
+    <t>N_i &lt; N_max-1</t>
+  </si>
+  <si>
+    <t>THERE ARE NO WAITING THREADS TO RECEIVE THIS EVENT.  THE EFSM WOULD GET STUCK IN THIS MODE.</t>
+  </si>
+  <si>
+    <t>TODO: We cannot enter into NoMoreWork unless we have at least one thread that is computing.  The last thread (Computing or Waiting) to transition to Idle always sets the EFSM mode to Idle.  Therefore there is no transition to this error state</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16">
+  <fonts count="15">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1614,16 +1620,8 @@
       <name val="Menlo"/>
       <family val="2"/>
     </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1634,12 +1632,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -1790,7 +1782,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1843,30 +1835,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1909,8 +1877,33 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2226,11 +2219,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98772F20-44FC-FE45-839B-70D0417F8C61}">
-  <dimension ref="A1:Q109"/>
+  <dimension ref="A1:Q108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A73" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A81" sqref="A81"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2256,57 +2249,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="16" customHeight="1">
-      <c r="B1" s="38"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
+      <c r="L1" s="39"/>
     </row>
     <row r="2" spans="1:17" ht="17" thickBot="1">
-      <c r="B2" s="38"/>
+      <c r="B2" s="30"/>
     </row>
     <row r="3" spans="1:17" ht="17" thickBot="1">
-      <c r="B3" s="38"/>
-      <c r="C3" s="18" t="s">
+      <c r="B3" s="30"/>
+      <c r="C3" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="21"/>
-      <c r="J3" s="18" t="s">
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="35"/>
+      <c r="J3" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="K3" s="19"/>
-      <c r="L3" s="19"/>
-      <c r="M3" s="20"/>
-      <c r="N3" s="21"/>
+      <c r="K3" s="33"/>
+      <c r="L3" s="33"/>
+      <c r="M3" s="34"/>
+      <c r="N3" s="35"/>
     </row>
     <row r="4" spans="1:17" ht="17" thickBot="1">
-      <c r="B4" s="38"/>
+      <c r="B4" s="30"/>
       <c r="C4" s="5"/>
-      <c r="D4" s="22" t="s">
+      <c r="D4" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="24"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="38"/>
       <c r="J4" s="5"/>
-      <c r="K4" s="22" t="s">
+      <c r="K4" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="L4" s="23"/>
-      <c r="M4" s="23"/>
-      <c r="N4" s="24"/>
+      <c r="L4" s="37"/>
+      <c r="M4" s="37"/>
+      <c r="N4" s="38"/>
     </row>
     <row r="5" spans="1:17" ht="17" thickBot="1">
-      <c r="B5" s="38"/>
+      <c r="B5" s="30"/>
       <c r="C5" s="5" t="s">
         <v>0</v>
       </c>
@@ -2346,30 +2339,30 @@
       <c r="O5" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="P5" s="31" t="s">
-        <v>126</v>
+      <c r="P5" s="23" t="s">
+        <v>123</v>
       </c>
       <c r="Q5" s="12" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:17">
-      <c r="B6" s="37" t="s">
+      <c r="B6" s="29" t="s">
         <v>84</v>
       </c>
-      <c r="C6" s="31" t="s">
+      <c r="C6" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="31" t="s">
+      <c r="D6" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="E6" s="31">
-        <v>0</v>
-      </c>
-      <c r="F6" s="31">
-        <v>0</v>
-      </c>
-      <c r="G6" s="31">
+      <c r="E6" s="23">
+        <v>0</v>
+      </c>
+      <c r="F6" s="23">
+        <v>0</v>
+      </c>
+      <c r="G6" s="23">
         <v>0</v>
       </c>
       <c r="H6" s="1" t="s">
@@ -2393,16 +2386,16 @@
       <c r="N6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="O6" s="32" t="s">
+      <c r="O6" s="24" t="s">
         <v>85</v>
       </c>
-      <c r="P6" s="36" t="s">
-        <v>127</v>
+      <c r="P6" s="28" t="s">
+        <v>124</v>
       </c>
       <c r="Q6" s="12"/>
     </row>
     <row r="7" spans="1:17">
-      <c r="B7" s="29"/>
+      <c r="B7" s="21"/>
       <c r="C7" s="1" t="s">
         <v>4</v>
       </c>
@@ -2443,14 +2436,14 @@
         <v>94</v>
       </c>
       <c r="P7" s="15" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="Q7" s="3" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:17">
-      <c r="B8" s="29"/>
+      <c r="B8" s="21"/>
       <c r="C8" s="1" t="s">
         <v>4</v>
       </c>
@@ -2491,7 +2484,7 @@
         <v>94</v>
       </c>
       <c r="P8" s="15" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="Q8" s="13" t="s">
         <v>86</v>
@@ -2499,7 +2492,7 @@
     </row>
     <row r="9" spans="1:17">
       <c r="A9" s="2"/>
-      <c r="B9" s="27"/>
+      <c r="B9" s="19"/>
       <c r="C9" s="1" t="s">
         <v>4</v>
       </c>
@@ -2539,12 +2532,12 @@
       <c r="O9" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="P9" s="36" t="s">
-        <v>130</v>
+      <c r="P9" s="28" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="10" spans="1:17">
-      <c r="B10" s="26"/>
+      <c r="B10" s="18"/>
       <c r="C10" s="1" t="s">
         <v>4</v>
       </c>
@@ -2585,11 +2578,11 @@
         <v>95</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="11" spans="1:17">
-      <c r="B11" s="26"/>
+      <c r="B11" s="18"/>
       <c r="C11" s="1" t="s">
         <v>4</v>
       </c>
@@ -2629,13 +2622,13 @@
       <c r="O11" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="P11" s="36" t="s">
-        <v>130</v>
+      <c r="P11" s="28" t="s">
+        <v>127</v>
       </c>
       <c r="Q11" s="13"/>
     </row>
     <row r="12" spans="1:17">
-      <c r="B12" s="26"/>
+      <c r="B12" s="18"/>
       <c r="C12" s="1" t="s">
         <v>4</v>
       </c>
@@ -2675,13 +2668,13 @@
       <c r="O12" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="P12" s="36" t="s">
-        <v>130</v>
+      <c r="P12" s="28" t="s">
+        <v>127</v>
       </c>
       <c r="Q12" s="13"/>
     </row>
     <row r="13" spans="1:17">
-      <c r="B13" s="30"/>
+      <c r="B13" s="22"/>
       <c r="C13" s="1" t="s">
         <v>4</v>
       </c>
@@ -2721,12 +2714,12 @@
       <c r="O13" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="P13" s="36" t="s">
-        <v>133</v>
+      <c r="P13" s="28" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="14" spans="1:17">
-      <c r="B14" s="30"/>
+      <c r="B14" s="22"/>
       <c r="C14" s="1" t="s">
         <v>4</v>
       </c>
@@ -2766,13 +2759,13 @@
       <c r="O14" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="P14" s="36" t="s">
-        <v>130</v>
+      <c r="P14" s="28" t="s">
+        <v>127</v>
       </c>
       <c r="Q14" s="13"/>
     </row>
     <row r="15" spans="1:17">
-      <c r="B15" s="30"/>
+      <c r="B15" s="22"/>
       <c r="C15" s="1" t="s">
         <v>4</v>
       </c>
@@ -2812,12 +2805,12 @@
       <c r="O15" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="P15" s="36" t="s">
-        <v>130</v>
+      <c r="P15" s="28" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="16" spans="1:17">
-      <c r="B16" s="30"/>
+      <c r="B16" s="22"/>
       <c r="C16" s="1" t="s">
         <v>4</v>
       </c>
@@ -2857,12 +2850,12 @@
       <c r="O16" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="P16" s="39" t="s">
-        <v>132</v>
+      <c r="P16" s="31" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="17" spans="2:17">
-      <c r="B17" s="30"/>
+      <c r="B17" s="22"/>
       <c r="C17" s="1" t="s">
         <v>4</v>
       </c>
@@ -2902,12 +2895,12 @@
       <c r="O17" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="P17" s="39" t="s">
-        <v>132</v>
+      <c r="P17" s="31" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="18" spans="2:17">
-      <c r="B18" s="30"/>
+      <c r="B18" s="22"/>
       <c r="C18" s="1" t="s">
         <v>4</v>
       </c>
@@ -2947,13 +2940,13 @@
       <c r="O18" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="P18" s="39" t="s">
-        <v>132</v>
+      <c r="P18" s="31" t="s">
+        <v>140</v>
       </c>
       <c r="Q18" s="13"/>
     </row>
     <row r="19" spans="2:17">
-      <c r="B19" s="26"/>
+      <c r="B19" s="18"/>
       <c r="C19" s="1" t="s">
         <v>5</v>
       </c>
@@ -2993,12 +2986,12 @@
       <c r="O19" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="P19" s="36" t="s">
-        <v>135</v>
+      <c r="P19" s="28" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="20" spans="2:17">
-      <c r="B20" s="26"/>
+      <c r="B20" s="18"/>
       <c r="C20" s="1" t="s">
         <v>5</v>
       </c>
@@ -3038,12 +3031,12 @@
       <c r="O20" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="P20" s="36" t="s">
-        <v>135</v>
+      <c r="P20" s="28" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="21" spans="2:17">
-      <c r="B21" s="26"/>
+      <c r="B21" s="18"/>
       <c r="C21" s="1" t="s">
         <v>5</v>
       </c>
@@ -3083,12 +3076,12 @@
       <c r="O21" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="P21" s="36" t="s">
-        <v>135</v>
+      <c r="P21" s="28" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="22" spans="2:17">
-      <c r="B22" s="26"/>
+      <c r="B22" s="18"/>
       <c r="C22" s="1" t="s">
         <v>5</v>
       </c>
@@ -3126,14 +3119,14 @@
         <v>98</v>
       </c>
       <c r="O22" s="13" t="s">
-        <v>125</v>
-      </c>
-      <c r="P22" s="36" t="s">
-        <v>136</v>
+        <v>122</v>
+      </c>
+      <c r="P22" s="28" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="23" spans="2:17">
-      <c r="B23" s="26"/>
+      <c r="B23" s="18"/>
       <c r="C23" s="1" t="s">
         <v>5</v>
       </c>
@@ -3173,12 +3166,12 @@
       <c r="O23" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="P23" s="36" t="s">
-        <v>138</v>
+      <c r="P23" s="28" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="24" spans="2:17">
-      <c r="B24" s="26"/>
+      <c r="B24" s="18"/>
       <c r="C24" s="1" t="s">
         <v>5</v>
       </c>
@@ -3218,18 +3211,18 @@
       <c r="O24" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="P24" s="36" t="s">
-        <v>129</v>
+      <c r="P24" s="28" t="s">
+        <v>126</v>
       </c>
       <c r="Q24" s="13"/>
     </row>
     <row r="25" spans="2:17">
-      <c r="B25" s="26"/>
+      <c r="B25" s="18"/>
       <c r="C25" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>17</v>
@@ -3262,14 +3255,14 @@
         <v>0</v>
       </c>
       <c r="O25" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="P25" s="36" t="s">
-        <v>134</v>
+        <v>115</v>
+      </c>
+      <c r="P25" s="28" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="26" spans="2:17">
-      <c r="B26" s="26"/>
+      <c r="B26" s="18"/>
       <c r="C26" s="1" t="s">
         <v>5</v>
       </c>
@@ -3310,12 +3303,12 @@
         <v>20</v>
       </c>
       <c r="P26" s="15" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="Q26" s="13"/>
     </row>
     <row r="27" spans="2:17">
-      <c r="B27" s="26"/>
+      <c r="B27" s="18"/>
       <c r="C27" s="1" t="s">
         <v>5</v>
       </c>
@@ -3355,15 +3348,15 @@
       <c r="O27" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="P27" s="39" t="s">
-        <v>132</v>
+      <c r="P27" s="31" t="s">
+        <v>140</v>
       </c>
       <c r="Q27" s="3" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="28" spans="2:17">
-      <c r="B28" s="26"/>
+      <c r="B28" s="18"/>
       <c r="C28" s="1" t="s">
         <v>5</v>
       </c>
@@ -3403,12 +3396,12 @@
       <c r="O28" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="P28" s="36" t="s">
-        <v>136</v>
+      <c r="P28" s="28" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="29" spans="2:17">
-      <c r="B29" s="26"/>
+      <c r="B29" s="18"/>
       <c r="C29" s="1" t="s">
         <v>5</v>
       </c>
@@ -3448,21 +3441,21 @@
       <c r="O29" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="P29" s="36" t="s">
-        <v>136</v>
+      <c r="P29" s="28" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="30" spans="2:17">
-      <c r="B30" s="28"/>
+      <c r="B30" s="20"/>
       <c r="O30" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="P30" s="36" t="s">
-        <v>136</v>
+      <c r="P30" s="28" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="31" spans="2:17">
-      <c r="B31" s="26"/>
+      <c r="B31" s="18"/>
       <c r="C31" s="1" t="s">
         <v>5</v>
       </c>
@@ -3503,11 +3496,11 @@
         <v>20</v>
       </c>
       <c r="P31" s="1" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="32" spans="2:17">
-      <c r="B32" s="26"/>
+      <c r="B32" s="18"/>
       <c r="C32" s="1" t="s">
         <v>5</v>
       </c>
@@ -3547,12 +3540,12 @@
       <c r="O32" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="P32" s="39" t="s">
-        <v>132</v>
+      <c r="P32" s="31" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="33" spans="1:17">
-      <c r="B33" s="26"/>
+      <c r="B33" s="18"/>
       <c r="C33" s="1" t="s">
         <v>5</v>
       </c>
@@ -3592,22 +3585,22 @@
       <c r="O33" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="P33" s="36" t="s">
-        <v>138</v>
+      <c r="P33" s="28" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="34" spans="1:17">
-      <c r="B34" s="28"/>
+      <c r="B34" s="20"/>
       <c r="H34" s="14"/>
       <c r="O34" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="P34" s="36" t="s">
-        <v>138</v>
+      <c r="P34" s="28" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="35" spans="1:17">
-      <c r="B35" s="26"/>
+      <c r="B35" s="18"/>
       <c r="C35" s="1" t="s">
         <v>5</v>
       </c>
@@ -3648,11 +3641,11 @@
         <v>104</v>
       </c>
       <c r="P35" s="1" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="36" spans="1:17">
-      <c r="B36" s="26"/>
+      <c r="B36" s="18"/>
       <c r="C36" s="1" t="s">
         <v>5</v>
       </c>
@@ -3692,23 +3685,23 @@
       <c r="O36" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="P36" s="36" t="s">
-        <v>138</v>
+      <c r="P36" s="28" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="37" spans="1:17">
       <c r="A37" s="13"/>
-      <c r="B37" s="28"/>
+      <c r="B37" s="20"/>
       <c r="H37" s="17"/>
       <c r="O37" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="P37" s="36" t="s">
-        <v>138</v>
+      <c r="P37" s="28" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="38" spans="1:17">
-      <c r="B38" s="26"/>
+      <c r="B38" s="18"/>
       <c r="C38" s="1" t="s">
         <v>5</v>
       </c>
@@ -3748,32 +3741,32 @@
       <c r="O38" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="P38" s="36" t="s">
-        <v>138</v>
+      <c r="P38" s="28" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="39" spans="1:17">
-      <c r="B39" s="28"/>
+      <c r="B39" s="20"/>
       <c r="H39" s="15"/>
       <c r="O39" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="P39" s="36" t="s">
-        <v>138</v>
+      <c r="P39" s="28" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="40" spans="1:17">
-      <c r="B40" s="28"/>
+      <c r="B40" s="20"/>
       <c r="H40" s="15"/>
       <c r="O40" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="P40" s="36" t="s">
-        <v>138</v>
+      <c r="P40" s="28" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="41" spans="1:17">
-      <c r="B41" s="26"/>
+      <c r="B41" s="18"/>
       <c r="C41" s="1" t="s">
         <v>49</v>
       </c>
@@ -3813,12 +3806,12 @@
       <c r="O41" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="P41" s="36" t="s">
-        <v>139</v>
+      <c r="P41" s="28" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="42" spans="1:17">
-      <c r="B42" s="26"/>
+      <c r="B42" s="18"/>
       <c r="C42" s="1" t="s">
         <v>49</v>
       </c>
@@ -3858,12 +3851,12 @@
       <c r="O42" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="P42" s="36" t="s">
-        <v>139</v>
+      <c r="P42" s="28" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="43" spans="1:17">
-      <c r="B43" s="26"/>
+      <c r="B43" s="18"/>
       <c r="C43" s="1" t="s">
         <v>49</v>
       </c>
@@ -3903,12 +3896,12 @@
       <c r="O43" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="P43" s="36" t="s">
-        <v>139</v>
+      <c r="P43" s="28" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="44" spans="1:17">
-      <c r="B44" s="26"/>
+      <c r="B44" s="18"/>
       <c r="C44" s="1" t="s">
         <v>49</v>
       </c>
@@ -3948,12 +3941,12 @@
       <c r="O44" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="P44" s="36" t="s">
-        <v>133</v>
+      <c r="P44" s="28" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="45" spans="1:17">
-      <c r="B45" s="26"/>
+      <c r="B45" s="18"/>
       <c r="C45" s="1" t="s">
         <v>49</v>
       </c>
@@ -3993,12 +3986,12 @@
       <c r="O45" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="P45" s="36" t="s">
-        <v>139</v>
+      <c r="P45" s="28" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="46" spans="1:17">
-      <c r="B46" s="26"/>
+      <c r="B46" s="18"/>
       <c r="C46" s="1" t="s">
         <v>49</v>
       </c>
@@ -4038,12 +4031,12 @@
       <c r="O46" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="P46" s="36" t="s">
-        <v>139</v>
+      <c r="P46" s="28" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="47" spans="1:17">
-      <c r="B47" s="26"/>
+      <c r="B47" s="18"/>
       <c r="C47" s="1" t="s">
         <v>49</v>
       </c>
@@ -4083,15 +4076,15 @@
       <c r="O47" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="P47" s="39" t="s">
-        <v>132</v>
+      <c r="P47" s="31" t="s">
+        <v>140</v>
       </c>
       <c r="Q47" s="13" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="48" spans="1:17">
-      <c r="B48" s="26"/>
+      <c r="B48" s="18"/>
       <c r="C48" s="1" t="s">
         <v>49</v>
       </c>
@@ -4131,23 +4124,23 @@
       <c r="O48" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="P48" s="39" t="s">
-        <v>132</v>
+      <c r="P48" s="31" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="49" spans="2:17">
-      <c r="B49" s="28"/>
+      <c r="B49" s="20"/>
       <c r="H49" s="14"/>
       <c r="O49" s="13" t="s">
-        <v>122</v>
-      </c>
-      <c r="P49" s="39" t="s">
-        <v>132</v>
+        <v>120</v>
+      </c>
+      <c r="P49" s="31" t="s">
+        <v>140</v>
       </c>
       <c r="Q49" s="13"/>
     </row>
     <row r="50" spans="2:17">
-      <c r="B50" s="26"/>
+      <c r="B50" s="18"/>
       <c r="C50" s="1" t="s">
         <v>49</v>
       </c>
@@ -4187,30 +4180,30 @@
       <c r="O50" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="P50" s="36" t="s">
-        <v>141</v>
+      <c r="P50" s="28" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="51" spans="2:17">
-      <c r="B51" s="28"/>
+      <c r="B51" s="20"/>
       <c r="O51" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="P51" s="39" t="s">
-        <v>132</v>
+      <c r="P51" s="31" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="52" spans="2:17">
-      <c r="B52" s="28"/>
+      <c r="B52" s="20"/>
       <c r="O52" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="P52" s="36" t="s">
-        <v>141</v>
+      <c r="P52" s="28" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="53" spans="2:17">
-      <c r="B53" s="26"/>
+      <c r="B53" s="18"/>
       <c r="C53" s="1" t="s">
         <v>49</v>
       </c>
@@ -4250,22 +4243,22 @@
       <c r="O53" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="P53" s="36" t="s">
-        <v>141</v>
+      <c r="P53" s="28" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="54" spans="2:17">
-      <c r="B54" s="28"/>
+      <c r="B54" s="20"/>
       <c r="H54" s="14"/>
       <c r="O54" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="P54" s="36" t="s">
-        <v>141</v>
+      <c r="P54" s="28" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="55" spans="2:17">
-      <c r="B55" s="26"/>
+      <c r="B55" s="18"/>
       <c r="C55" s="1" t="s">
         <v>49</v>
       </c>
@@ -4306,11 +4299,11 @@
         <v>20</v>
       </c>
       <c r="P55" s="1" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="56" spans="2:17">
-      <c r="B56" s="26"/>
+      <c r="B56" s="18"/>
       <c r="C56" s="1" t="s">
         <v>49</v>
       </c>
@@ -4350,12 +4343,12 @@
       <c r="O56" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="P56" s="39" t="s">
-        <v>132</v>
+      <c r="P56" s="31" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="57" spans="2:17">
-      <c r="B57" s="26"/>
+      <c r="B57" s="18"/>
       <c r="C57" s="1" t="s">
         <v>49</v>
       </c>
@@ -4395,32 +4388,32 @@
       <c r="O57" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="P57" s="39" t="s">
-        <v>132</v>
+      <c r="P57" s="31" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="58" spans="2:17">
-      <c r="B58" s="28"/>
+      <c r="B58" s="20"/>
       <c r="H58" s="14"/>
       <c r="O58" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="P58" s="39" t="s">
-        <v>132</v>
+      <c r="P58" s="31" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="59" spans="2:17">
-      <c r="B59" s="28"/>
+      <c r="B59" s="20"/>
       <c r="H59" s="14"/>
       <c r="O59" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="P59" s="40" t="s">
-        <v>132</v>
+      <c r="P59" s="31" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="60" spans="2:17">
-      <c r="B60" s="26"/>
+      <c r="B60" s="18"/>
       <c r="C60" s="1" t="s">
         <v>49</v>
       </c>
@@ -4460,22 +4453,22 @@
       <c r="O60" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="P60" s="40" t="s">
-        <v>132</v>
+      <c r="P60" s="31" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="61" spans="2:17">
-      <c r="B61" s="28"/>
+      <c r="B61" s="20"/>
       <c r="H61" s="14"/>
       <c r="O61" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="P61" s="39" t="s">
-        <v>132</v>
+      <c r="P61" s="31" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="62" spans="2:17">
-      <c r="B62" s="26"/>
+      <c r="B62" s="18"/>
       <c r="C62" s="1" t="s">
         <v>49</v>
       </c>
@@ -4516,11 +4509,11 @@
         <v>104</v>
       </c>
       <c r="P62" s="1" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="63" spans="2:17">
-      <c r="B63" s="26"/>
+      <c r="B63" s="18"/>
       <c r="C63" s="1" t="s">
         <v>49</v>
       </c>
@@ -4560,33 +4553,33 @@
       <c r="O63" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="P63" s="39" t="s">
-        <v>132</v>
+      <c r="P63" s="31" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="64" spans="2:17">
-      <c r="B64" s="26"/>
+      <c r="B64" s="18"/>
       <c r="H64" s="14"/>
       <c r="O64" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="P64" s="39" t="s">
-        <v>132</v>
+      <c r="P64" s="31" t="s">
+        <v>140</v>
       </c>
       <c r="Q64" s="13"/>
     </row>
     <row r="65" spans="2:17">
-      <c r="B65" s="28"/>
+      <c r="B65" s="20"/>
       <c r="H65" s="17"/>
       <c r="O65" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="P65" s="39" t="s">
-        <v>132</v>
+      <c r="P65" s="31" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="66" spans="2:17">
-      <c r="B66" s="26"/>
+      <c r="B66" s="18"/>
       <c r="C66" s="1" t="s">
         <v>49</v>
       </c>
@@ -4626,42 +4619,42 @@
       <c r="O66" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="P66" s="36" t="s">
-        <v>142</v>
+      <c r="P66" s="28" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="67" spans="2:17">
-      <c r="B67" s="28"/>
+      <c r="B67" s="20"/>
       <c r="H67" s="15"/>
       <c r="O67" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="P67" s="36" t="s">
-        <v>142</v>
+      <c r="P67" s="28" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="68" spans="2:17">
-      <c r="B68" s="28"/>
+      <c r="B68" s="20"/>
       <c r="H68" s="15"/>
       <c r="O68" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="P68" s="39" t="s">
-        <v>132</v>
+      <c r="P68" s="31" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="69" spans="2:17">
-      <c r="B69" s="28"/>
+      <c r="B69" s="20"/>
       <c r="H69" s="15"/>
       <c r="O69" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="P69" s="36" t="s">
-        <v>142</v>
+      <c r="P69" s="28" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="70" spans="2:17">
-      <c r="B70" s="26"/>
+      <c r="B70" s="18"/>
       <c r="C70" s="1" t="s">
         <v>49</v>
       </c>
@@ -4701,32 +4694,32 @@
       <c r="O70" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="P70" s="36" t="s">
-        <v>142</v>
+      <c r="P70" s="28" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="71" spans="2:17">
-      <c r="B71" s="34"/>
+      <c r="B71" s="26"/>
       <c r="H71" s="17"/>
       <c r="O71" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="P71" s="36" t="s">
-        <v>142</v>
+      <c r="P71" s="28" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="72" spans="2:17">
-      <c r="B72" s="35"/>
+      <c r="B72" s="27"/>
       <c r="H72" s="17"/>
       <c r="O72" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="P72" s="36" t="s">
-        <v>142</v>
+      <c r="P72" s="28" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="73" spans="2:17">
-      <c r="B73" s="26"/>
+      <c r="B73" s="18"/>
       <c r="C73" s="1" t="s">
         <v>38</v>
       </c>
@@ -4767,11 +4760,11 @@
         <v>109</v>
       </c>
       <c r="P73" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="74" spans="2:17">
-      <c r="B74" s="26"/>
+      <c r="B74" s="18"/>
       <c r="C74" s="1" t="s">
         <v>38</v>
       </c>
@@ -4811,12 +4804,12 @@
       <c r="O74" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="P74" s="36" t="s">
-        <v>140</v>
+      <c r="P74" s="28" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="75" spans="2:17">
-      <c r="B75" s="26"/>
+      <c r="B75" s="18"/>
       <c r="C75" s="1" t="s">
         <v>38</v>
       </c>
@@ -4856,13 +4849,13 @@
       <c r="O75" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="P75" s="36" t="s">
-        <v>140</v>
+      <c r="P75" s="28" t="s">
+        <v>136</v>
       </c>
       <c r="Q75" s="13"/>
     </row>
     <row r="76" spans="2:17">
-      <c r="B76" s="26"/>
+      <c r="B76" s="18"/>
       <c r="C76" s="1" t="s">
         <v>38</v>
       </c>
@@ -4902,12 +4895,12 @@
       <c r="O76" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="P76" s="36" t="s">
-        <v>140</v>
+      <c r="P76" s="28" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="77" spans="2:17">
-      <c r="B77" s="26"/>
+      <c r="B77" s="18"/>
       <c r="C77" s="1" t="s">
         <v>38</v>
       </c>
@@ -4945,15 +4938,15 @@
         <v>0</v>
       </c>
       <c r="O77" s="13" t="s">
-        <v>110</v>
-      </c>
-      <c r="P77" s="36" t="s">
-        <v>143</v>
+        <v>141</v>
+      </c>
+      <c r="P77" s="28" t="s">
+        <v>139</v>
       </c>
       <c r="Q77" s="13"/>
     </row>
     <row r="78" spans="2:17">
-      <c r="B78" s="26"/>
+      <c r="B78" s="18"/>
       <c r="C78" s="1" t="s">
         <v>38</v>
       </c>
@@ -4993,12 +4986,12 @@
       <c r="O78" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="P78" s="36" t="s">
-        <v>140</v>
+      <c r="P78" s="28" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="79" spans="2:17">
-      <c r="B79" s="26"/>
+      <c r="B79" s="18"/>
       <c r="C79" s="1" t="s">
         <v>38</v>
       </c>
@@ -5038,12 +5031,12 @@
       <c r="O79" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="P79" s="36" t="s">
-        <v>140</v>
+      <c r="P79" s="28" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="80" spans="2:17">
-      <c r="B80" s="26"/>
+      <c r="B80" s="18"/>
       <c r="C80" s="1" t="s">
         <v>38</v>
       </c>
@@ -5083,15 +5076,15 @@
       <c r="O80" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="P80" s="39" t="s">
-        <v>132</v>
-      </c>
-      <c r="Q80" s="33" t="s">
-        <v>117</v>
+      <c r="P80" s="31" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q80" s="25" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="81" spans="2:17">
-      <c r="B81" s="26"/>
+      <c r="B81" s="18"/>
       <c r="C81" s="1" t="s">
         <v>38</v>
       </c>
@@ -5131,40 +5124,51 @@
       <c r="O81" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="P81" s="15"/>
+      <c r="P81" s="31" t="s">
+        <v>140</v>
+      </c>
       <c r="Q81" s="13"/>
     </row>
     <row r="82" spans="2:17">
-      <c r="B82" s="28"/>
+      <c r="B82" s="20"/>
       <c r="H82" s="14"/>
       <c r="O82" s="13" t="s">
         <v>88</v>
       </c>
+      <c r="P82" s="31" t="s">
+        <v>140</v>
+      </c>
       <c r="Q82" s="13"/>
     </row>
     <row r="83" spans="2:17">
-      <c r="B83" s="28"/>
+      <c r="B83" s="20"/>
       <c r="H83" s="14"/>
       <c r="O83" s="13" t="s">
-        <v>115</v>
+        <v>114</v>
+      </c>
+      <c r="P83" s="31" t="s">
+        <v>140</v>
       </c>
       <c r="Q83" s="13"/>
     </row>
     <row r="84" spans="2:17">
-      <c r="B84" s="28"/>
+      <c r="B84" s="20"/>
       <c r="H84" s="14"/>
       <c r="O84" s="13" t="s">
         <v>83</v>
       </c>
+      <c r="P84" s="31" t="s">
+        <v>140</v>
+      </c>
       <c r="Q84" s="13"/>
     </row>
     <row r="85" spans="2:17">
-      <c r="B85" s="26"/>
+      <c r="B85" s="18"/>
       <c r="C85" s="1" t="s">
         <v>38</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E85" s="1" t="s">
         <v>17</v>
@@ -5199,23 +5203,26 @@
       <c r="O85" s="3" t="s">
         <v>73</v>
       </c>
+      <c r="P85" s="31" t="s">
+        <v>140</v>
+      </c>
       <c r="Q85" s="3" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="86" spans="2:17">
-      <c r="B86" s="26"/>
+        <v>119</v>
+      </c>
+    </row>
+    <row r="86" spans="2:17" ht="17" customHeight="1">
+      <c r="B86" s="18"/>
       <c r="C86" s="1" t="s">
         <v>38</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E86" s="1">
         <v>0</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="G86" s="1">
         <v>0</v>
@@ -5244,20 +5251,23 @@
       <c r="O86" s="3" t="s">
         <v>20</v>
       </c>
+      <c r="P86" s="1" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="87" spans="2:17">
-      <c r="B87" s="26"/>
+      <c r="B87" s="18"/>
       <c r="C87" s="1" t="s">
         <v>38</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E87" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="F87" s="1" t="s">
-        <v>18</v>
+        <v>39</v>
+      </c>
+      <c r="E87" s="1">
+        <v>0</v>
+      </c>
+      <c r="F87" s="1">
+        <v>0</v>
       </c>
       <c r="G87" s="1">
         <v>0</v>
@@ -5269,31 +5279,37 @@
         <v>8</v>
       </c>
       <c r="J87" s="1" t="s">
-        <v>38</v>
+        <v>4</v>
       </c>
       <c r="K87" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="L87" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="M87" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
+      </c>
+      <c r="L87" s="1">
+        <v>0</v>
+      </c>
+      <c r="M87" s="1">
+        <v>0</v>
       </c>
       <c r="N87" s="1">
         <v>0</v>
       </c>
-      <c r="O87" s="3" t="s">
-        <v>63</v>
+      <c r="O87" s="41" t="s">
+        <v>144</v>
+      </c>
+      <c r="P87" s="31" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q87" s="13" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="88" spans="2:17">
-      <c r="B88" s="26"/>
+      <c r="B88" s="18"/>
       <c r="C88" s="1" t="s">
         <v>38</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>19</v>
+        <v>143</v>
       </c>
       <c r="E88" s="1">
         <v>1</v>
@@ -5314,7 +5330,7 @@
         <v>38</v>
       </c>
       <c r="K88" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="L88" s="1">
         <v>0</v>
@@ -5328,10 +5344,13 @@
       <c r="O88" s="13" t="s">
         <v>63</v>
       </c>
+      <c r="P88" s="40" t="s">
+        <v>142</v>
+      </c>
       <c r="Q88" s="13"/>
     </row>
     <row r="89" spans="2:17">
-      <c r="B89" s="26"/>
+      <c r="B89" s="18"/>
       <c r="C89" s="1" t="s">
         <v>38</v>
       </c>
@@ -5371,35 +5390,43 @@
       <c r="O89" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="P89" s="15"/>
+      <c r="P89" s="31" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="90" spans="2:17">
-      <c r="B90" s="28"/>
+      <c r="B90" s="20"/>
       <c r="H90" s="14"/>
       <c r="O90" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
+      </c>
+      <c r="P90" s="31" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="91" spans="2:17">
-      <c r="B91" s="28"/>
+      <c r="B91" s="20"/>
       <c r="H91" s="14"/>
       <c r="O91" s="3" t="s">
         <v>83</v>
       </c>
+      <c r="P91" s="31" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="92" spans="2:17">
-      <c r="B92" s="26"/>
+      <c r="B92" s="18"/>
       <c r="C92" s="1" t="s">
         <v>38</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E92" s="1">
-        <v>0</v>
-      </c>
-      <c r="F92" s="1">
-        <v>0</v>
+        <v>143</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F92" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="G92" s="1">
         <v>0</v>
@@ -5411,27 +5438,29 @@
         <v>8</v>
       </c>
       <c r="J92" s="1" t="s">
-        <v>4</v>
+        <v>38</v>
       </c>
       <c r="K92" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="L92" s="1">
-        <v>0</v>
-      </c>
-      <c r="M92" s="1">
-        <v>0</v>
+        <v>62</v>
+      </c>
+      <c r="L92" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="M92" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="N92" s="1">
         <v>0</v>
       </c>
-      <c r="O92" s="13" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q92" s="13"/>
+      <c r="O92" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="P92" s="40" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="93" spans="2:17">
-      <c r="B93" s="26"/>
+      <c r="B93" s="18"/>
       <c r="C93" s="1" t="s">
         <v>38</v>
       </c>
@@ -5472,16 +5501,16 @@
         <v>104</v>
       </c>
       <c r="P93" s="1" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="94" spans="2:17">
-      <c r="B94" s="26"/>
+      <c r="B94" s="18"/>
       <c r="C94" s="1" t="s">
         <v>38</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>19</v>
+        <v>143</v>
       </c>
       <c r="E94" s="1" t="s">
         <v>31</v>
@@ -5502,7 +5531,7 @@
         <v>38</v>
       </c>
       <c r="K94" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="L94" s="1" t="s">
         <v>42</v>
@@ -5516,22 +5545,28 @@
       <c r="O94" s="13" t="s">
         <v>80</v>
       </c>
+      <c r="P94" s="31" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="95" spans="2:17">
-      <c r="B95" s="28"/>
+      <c r="B95" s="20"/>
       <c r="H95" s="14"/>
       <c r="O95" s="13" t="s">
         <v>61</v>
       </c>
+      <c r="P95" s="31" t="s">
+        <v>140</v>
+      </c>
       <c r="Q95" s="13"/>
     </row>
     <row r="96" spans="2:17">
-      <c r="B96" s="26"/>
+      <c r="B96" s="18"/>
       <c r="C96" s="1" t="s">
         <v>38</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>19</v>
+        <v>143</v>
       </c>
       <c r="E96" s="1">
         <v>0</v>
@@ -5552,13 +5587,13 @@
         <v>38</v>
       </c>
       <c r="K96" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="L96" s="1">
         <v>0</v>
       </c>
       <c r="M96" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N96" s="1">
         <v>0</v>
@@ -5566,17 +5601,23 @@
       <c r="O96" s="13" t="s">
         <v>80</v>
       </c>
+      <c r="P96" s="40" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="97" spans="2:17">
-      <c r="B97" s="28"/>
+      <c r="B97" s="20"/>
       <c r="H97" s="14"/>
       <c r="O97" s="13" t="s">
         <v>61</v>
       </c>
+      <c r="P97" s="40" t="s">
+        <v>142</v>
+      </c>
       <c r="Q97" s="13"/>
     </row>
     <row r="98" spans="2:17">
-      <c r="B98" s="26"/>
+      <c r="B98" s="18"/>
       <c r="C98" s="1" t="s">
         <v>38</v>
       </c>
@@ -5616,71 +5657,44 @@
       <c r="O98" s="13" t="s">
         <v>80</v>
       </c>
+      <c r="P98" s="40" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="99" spans="2:17">
-      <c r="B99" s="28"/>
+      <c r="B99" s="20"/>
       <c r="H99" s="17"/>
       <c r="O99" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="P99" s="15"/>
+      <c r="P99" s="40" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="100" spans="2:17">
-      <c r="B100" s="28"/>
+      <c r="B100" s="20"/>
       <c r="H100" s="17"/>
       <c r="O100" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
+      </c>
+      <c r="P100" s="40" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="101" spans="2:17">
-      <c r="B101" s="28"/>
+      <c r="B101" s="20"/>
       <c r="H101" s="17"/>
       <c r="O101" s="13" t="s">
         <v>83</v>
       </c>
+      <c r="P101" s="40" t="s">
+        <v>142</v>
+      </c>
       <c r="Q101" s="13"/>
     </row>
     <row r="102" spans="2:17">
-      <c r="B102" s="26"/>
-      <c r="C102" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D102" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E102" s="1">
-        <v>0</v>
-      </c>
-      <c r="F102" s="1">
-        <v>0</v>
-      </c>
-      <c r="G102" s="1">
-        <v>0</v>
-      </c>
-      <c r="H102" s="14" t="s">
-        <v>91</v>
-      </c>
-      <c r="I102" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J102" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="K102" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="L102" s="1">
-        <v>0</v>
-      </c>
-      <c r="M102" s="1">
-        <v>0</v>
-      </c>
-      <c r="N102" s="1">
-        <v>0</v>
-      </c>
-      <c r="O102" s="13" t="s">
-        <v>124</v>
-      </c>
+      <c r="H102" s="15"/>
+      <c r="O102"/>
       <c r="Q102"/>
     </row>
     <row r="103" spans="2:17">
@@ -5689,9 +5703,7 @@
       <c r="Q103"/>
     </row>
     <row r="104" spans="2:17">
-      <c r="H104" s="15"/>
-      <c r="O104"/>
-      <c r="Q104"/>
+      <c r="H104" s="14"/>
     </row>
     <row r="105" spans="2:17">
       <c r="H105" s="14"/>
@@ -5703,10 +5715,7 @@
       <c r="H107" s="14"/>
     </row>
     <row r="108" spans="2:17">
-      <c r="H108" s="14"/>
-    </row>
-    <row r="109" spans="2:17">
-      <c r="H109" s="15"/>
+      <c r="H108" s="15"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0"/>

</xml_diff>

<commit_message>
WIP: Cleaned the main design document and grew it so that it now includes important technical specifications for the Running/Closed and Running/NoMoreWork modes.  As part of writing these specifications, the design spreadsheet and code were improved as well.
</commit_message>
<xml_diff>
--- a/docs/RuntimeDesign.xlsx
+++ b/docs/RuntimeDesign.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jared/Projects/OrchestrationRuntime/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{063FDD71-FF99-2540-936F-6CA40A2F4252}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAC11267-6030-1E4B-805A-60F78B4EA177}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="17560" xr2:uid="{9B8D0C4A-3FF1-A04E-B8F8-B86CE3BC2D78}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="887" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="846" uniqueCount="142">
   <si>
     <t>Machine Mode</t>
   </si>
@@ -427,9 +427,6 @@
     </r>
   </si>
   <si>
-    <t>N_i+1</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Receiving thread waits on </t>
     </r>
@@ -690,7 +687,31 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Thread that just finished work waits on </t>
+      <t xml:space="preserve">Thread that just finished work transitions Mode and then broadcast to all threads the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="8" tint="-0.249977111117893"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>transitionThread</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> signal</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Waits on </t>
     </r>
     <r>
       <rPr>
@@ -724,18 +745,9 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Thread that just finished work transitions Mode and then broadcast to all threads the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="8" tint="-0.249977111117893"/>
-        <rFont val="Calibri (Body)_x0000_"/>
-      </rPr>
-      <t>transitionThread</t>
-    </r>
+    <t>Initial</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="12"/>
@@ -744,12 +756,284 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> signal</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Waits on </t>
+      <t>All threads waiting on</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="8" tint="-0.249977111117893"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>activateThread</t>
+    </r>
+  </si>
+  <si>
+    <t>Satisfaction of Req proven</t>
+  </si>
+  <si>
+    <t>N_Q &gt; 0</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Call </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>increaseThreadCount</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">(1) of Thread Subscriber if exists and wait for </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="8" tint="-0.249977111117893"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>activateThread</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Wait for </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="8" tint="-0.249977111117893"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>activateThread</t>
+    </r>
+  </si>
+  <si>
+    <t>computationFinished</t>
+  </si>
+  <si>
+    <t>0 &lt;= i &lt;= N_max</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Throw error</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - adding more threads than in team</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Throw error</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - By requirement</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Set N_to_activate = i and emit </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="8" tint="-0.249977111117893"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t xml:space="preserve">activateThread </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>event i times</t>
+    </r>
+  </si>
+  <si>
+    <t>N Idle</t>
+  </si>
+  <si>
+    <t>N_Q &gt;= 0</t>
+  </si>
+  <si>
+    <t>N_Q</t>
+  </si>
+  <si>
+    <t>N_Q-1 &gt;= 0</t>
+  </si>
+  <si>
+    <t>i &gt; 0 and i &gt; N_i</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Enqueue given unit of work W and emit </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="8" tint="-0.249977111117893"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>transitionThread</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> once</t>
+    </r>
+  </si>
+  <si>
+    <t>N_Q+1 &gt; 0</t>
+  </si>
+  <si>
+    <t>N_Q &gt; 1</t>
+  </si>
+  <si>
+    <t>N_Q-1 &gt; 0</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Emit </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="8" tint="-0.249977111117893"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t xml:space="preserve">activateThread </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">event min(i, N_Q) times and if i &gt; N_Q call </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>increaseThreadCount(i - N_Q)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> of ThreadSubscriber if exists</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Throw error </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- there should be no pending work</t>
+    </r>
+  </si>
+  <si>
+    <t>N_c-1 &gt; 0</t>
+  </si>
+  <si>
+    <t>N_w &gt; 1</t>
+  </si>
+  <si>
+    <t>N_w-1 &gt;= 1</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Broadcast </t>
     </r>
     <r>
       <rPr>
@@ -760,7 +1044,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>activate</t>
+      <t>unblock</t>
     </r>
     <r>
       <rPr>
@@ -769,7 +1053,7 @@
         <color theme="8" tint="-0.249977111117893"/>
         <rFont val="Calibri (Body)_x0000_"/>
       </rPr>
-      <t>Thread</t>
+      <t>WaitThread</t>
     </r>
     <r>
       <rPr>
@@ -779,13 +1063,33 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> signal</t>
-    </r>
-  </si>
-  <si>
-    <t>Initial</t>
-  </si>
-  <si>
+      <t xml:space="preserve"> signal to wake all threads that called wait() if any</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Broadcast </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="8" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>unblock</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="8" tint="-0.249977111117893"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t xml:space="preserve">WaitThread </t>
+    </r>
     <r>
       <rPr>
         <sz val="12"/>
@@ -794,18 +1098,42 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>All threads waiting on</t>
+      <t>signal to wake all threads that called wait() if any</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Transition Mode and then broadcast to all waiting threads the </t>
     </r>
     <r>
       <rPr>
         <b/>
+        <sz val="12"/>
+        <color theme="8" tint="-0.249977111117893"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>transitionThread</t>
+    </r>
+    <r>
+      <rPr>
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> </t>
+      <t xml:space="preserve"> signal</t>
+    </r>
+  </si>
+  <si>
+    <t>0 &lt; N_i &lt; N_max</t>
+  </si>
+  <si>
+    <t>0 &lt;= N_i &lt; N_max</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">We are assuming that any threads that are Waiting have yet to receive the </t>
     </r>
     <r>
       <rPr>
@@ -814,27 +1142,7 @@
         <color theme="8" tint="-0.249977111117893"/>
         <rFont val="Calibri (Body)_x0000_"/>
       </rPr>
-      <t>activateThread</t>
-    </r>
-  </si>
-  <si>
-    <t>Satisfaction of Req proven</t>
-  </si>
-  <si>
-    <t>N_Q &gt; 0</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Call </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="9" tint="-0.249977111117893"/>
-        <rFont val="Calibri (Body)_x0000_"/>
-      </rPr>
-      <t>increaseThreadCount(1)</t>
+      <t>transitionThread</t>
     </r>
     <r>
       <rPr>
@@ -844,21 +1152,24 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> of Thread Subscriber if exists</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Call </t>
+      <t xml:space="preserve"> signal, but will.</t>
+    </r>
+  </si>
+  <si>
+    <t>N_i+1 &lt; N_max</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Increment N_to_activate by i and emit </t>
     </r>
     <r>
       <rPr>
         <b/>
         <sz val="12"/>
-        <color theme="9" tint="-0.249977111117893"/>
+        <color theme="8" tint="-0.249977111117893"/>
         <rFont val="Calibri (Body)_x0000_"/>
       </rPr>
-      <t>increaseThreadCount</t>
+      <t>activateThread</t>
     </r>
     <r>
       <rPr>
@@ -868,658 +1179,137 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">(1) of Thread Subscriber if exists and wait for </t>
+      <t xml:space="preserve"> event i times</t>
+    </r>
+  </si>
+  <si>
+    <t>Test name</t>
+  </si>
+  <si>
+    <t>TestInitialState</t>
+  </si>
+  <si>
+    <t>Internally</t>
+  </si>
+  <si>
+    <t>TestNoWorkNoThreads</t>
+  </si>
+  <si>
+    <t>TestIdleErrors</t>
+  </si>
+  <si>
+    <t>Many</t>
+  </si>
+  <si>
+    <t>TestIdleForwardsThreads</t>
+  </si>
+  <si>
+    <t>TestNoWork</t>
+  </si>
+  <si>
+    <t>TestRunningOpenErrors</t>
+  </si>
+  <si>
+    <t>TestRunningOpenIncreaseThreads</t>
+  </si>
+  <si>
+    <t>Nothing to test</t>
+  </si>
+  <si>
+    <t>TestRunningOpenEnqueue</t>
+  </si>
+  <si>
+    <t>TestRunningClosedErrors</t>
+  </si>
+  <si>
+    <t>TestRunningNoMoreWorkErrors</t>
+  </si>
+  <si>
+    <t>TestRunningClosedActivation</t>
+  </si>
+  <si>
+    <t>TestRunningClosedWorkPub</t>
+  </si>
+  <si>
+    <t>TestRunningNoMoreWorkForward</t>
+  </si>
+  <si>
+    <t>Do not know how to test directly</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Call </t>
     </r>
     <r>
       <rPr>
         <b/>
         <sz val="12"/>
-        <color theme="8" tint="-0.249977111117893"/>
+        <color theme="9" tint="-0.249977111117893"/>
         <rFont val="Calibri (Body)_x0000_"/>
       </rPr>
-      <t>activateThread</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Wait for </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="8" tint="-0.249977111117893"/>
-        <rFont val="Calibri (Body)_x0000_"/>
-      </rPr>
-      <t>activateThread</t>
-    </r>
-  </si>
-  <si>
-    <t>computationFinished</t>
-  </si>
-  <si>
-    <t>0 &lt;= i &lt;= N_max</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
+      <t>increaseThreadCount</t>
+    </r>
+    <r>
+      <rPr>
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Throw error</t>
-    </r>
-    <r>
-      <rPr>
+      <t>(i) of Thread Subscriber if exists</t>
+    </r>
+  </si>
+  <si>
+    <t>TestRunningNoMoreWorkTransition</t>
+  </si>
+  <si>
+    <t>N_i &lt; N_max-1</t>
+  </si>
+  <si>
+    <t>N_i = N_max</t>
+  </si>
+  <si>
+    <t>THIS WOULD LEAD TO DEADLOCK.  Not allowed by specifications.</t>
+  </si>
+  <si>
+    <t>THIS WOULD LEAD TO THREAD RESOURCE LOSS!  Not allowed by specifications.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> - adding more threads than in team</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
+      <t>IMPOSSIBLE:</t>
+    </r>
+    <r>
+      <rPr>
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Throw error</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - By requirement</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Set N_to_activate = i and emit </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="8" tint="-0.249977111117893"/>
-        <rFont val="Calibri (Body)_x0000_"/>
-      </rPr>
-      <t xml:space="preserve">activateThread </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>event i times</t>
-    </r>
-  </si>
-  <si>
-    <t>N Idle</t>
-  </si>
-  <si>
-    <t>N_Q &gt;= 0</t>
-  </si>
-  <si>
-    <t>N_Q</t>
-  </si>
-  <si>
-    <t>N_Q-1 &gt;= 0</t>
-  </si>
-  <si>
-    <t>i &gt; 0 and i &gt; N_i</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Enqueue given unit of work W and emit </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="8" tint="-0.249977111117893"/>
-        <rFont val="Calibri (Body)_x0000_"/>
-      </rPr>
-      <t>transitionThread</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> once</t>
-    </r>
-  </si>
-  <si>
-    <t>N_Q+1 &gt; 0</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Throw error</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - no threads to receive event.  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri (Body)_x0000_"/>
-      </rPr>
-      <t>THIS WOULD LEAD TO THREAD RESOURCE LOSS!</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Throw error </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>- this event is triggered by a computing thread =&gt; N_c &gt; 0</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Only startTask and increaseThreadCount can emit </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="8" tint="-0.249977111117893"/>
-        <rFont val="Calibri (Body)_x0000_"/>
-      </rPr>
-      <t>activateThread.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri (Body)_x0000_"/>
-      </rPr>
-      <t xml:space="preserve">  Both only emit if i &lt;= N_i - N_to_activate</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <t>N_Q &gt; 1</t>
-  </si>
-  <si>
-    <t>N_Q-1 &gt; 0</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Emit </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="8" tint="-0.249977111117893"/>
-        <rFont val="Calibri (Body)_x0000_"/>
-      </rPr>
-      <t xml:space="preserve">activateThread </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">event min(i, N_Q) times and if i &gt; N_Q call </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="9" tint="-0.249977111117893"/>
-        <rFont val="Calibri (Body)_x0000_"/>
-      </rPr>
-      <t>increaseThreadCount(i - N_Q)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> of ThreadSubscriber if exists</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Throw error </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>- there should be no pending work</t>
-    </r>
-  </si>
-  <si>
-    <t>N_c-1 &gt; 0</t>
-  </si>
-  <si>
-    <t>N_w &gt; 1</t>
-  </si>
-  <si>
-    <t>N_w-1 &gt;= 1</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Broadcast </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="8" tint="-0.249977111117893"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>unblock</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="8" tint="-0.249977111117893"/>
-        <rFont val="Calibri (Body)_x0000_"/>
-      </rPr>
-      <t>WaitThread</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> signal to wake all threads that called wait() if any</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Broadcast </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="8" tint="-0.249977111117893"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>unblock</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="8" tint="-0.249977111117893"/>
-        <rFont val="Calibri (Body)_x0000_"/>
-      </rPr>
-      <t xml:space="preserve">WaitThread </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>signal to wake all threads that called wait() if any</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Transition Mode and then broadcast to all waiting threads the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="8" tint="-0.249977111117893"/>
-        <rFont val="Calibri (Body)_x0000_"/>
-      </rPr>
-      <t>transitionThread</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> signal</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Only </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="9" tint="-0.249977111117893"/>
-        <rFont val="Calibri (Body)_x0000_"/>
-      </rPr>
-      <t>startTask</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> and </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="9" tint="-0.249977111117893"/>
-        <rFont val="Calibri (Body)_x0000_"/>
-      </rPr>
-      <t>increaseThreadCount</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> can emit </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FF2F75B5"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>activateThread.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t xml:space="preserve">  Both only emit if i &lt;= N_i - N_to_activate</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <t>0 &lt; N_i &lt; N_max</t>
-  </si>
-  <si>
-    <t>0 &lt;= N_i &lt; N_max</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">We are assuming that any threads that are Waiting have yet to receive the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="8" tint="-0.249977111117893"/>
-        <rFont val="Calibri (Body)_x0000_"/>
-      </rPr>
-      <t>transitionThread</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> signal, but will.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Receiving thread transitions Mode and then broadcasts to all waiting threads the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="8" tint="-0.249977111117893"/>
-        <rFont val="Calibri (Body)_x0000_"/>
-      </rPr>
-      <t>transitionThread</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> signal</t>
-    </r>
-  </si>
-  <si>
-    <t>N_i+1 &lt; N_max</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Increment N_to_activate by i and emit </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="8" tint="-0.249977111117893"/>
-        <rFont val="Calibri (Body)_x0000_"/>
-      </rPr>
-      <t>activateThread</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> event i times</t>
-    </r>
-  </si>
-  <si>
-    <t>Test name</t>
-  </si>
-  <si>
-    <t>TestInitialState</t>
-  </si>
-  <si>
-    <t>Internally</t>
-  </si>
-  <si>
-    <t>TestNoWorkNoThreads</t>
-  </si>
-  <si>
-    <t>TestIdleErrors</t>
-  </si>
-  <si>
-    <t>Many</t>
-  </si>
-  <si>
-    <t>TestIdleForwardsThreads</t>
-  </si>
-  <si>
-    <t>TestNoWork</t>
-  </si>
-  <si>
-    <t>TestRunningOpenErrors</t>
-  </si>
-  <si>
-    <t>TestRunningOpenIncreaseThreads</t>
-  </si>
-  <si>
-    <t>Nothing to test</t>
-  </si>
-  <si>
-    <t>TestRunningOpenEnqueue</t>
-  </si>
-  <si>
-    <t>TestRunningClosedErrors</t>
-  </si>
-  <si>
-    <t>TestRunningNoMoreWorkErrors</t>
-  </si>
-  <si>
-    <t>TestRunningClosedActivation</t>
-  </si>
-  <si>
-    <t>TestRunningClosedWorkPub</t>
-  </si>
-  <si>
-    <t>TestRunningNoMoreWorkForward</t>
-  </si>
-  <si>
-    <t>Do not know how to test directly</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Call </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="9" tint="-0.249977111117893"/>
-        <rFont val="Calibri (Body)_x0000_"/>
-      </rPr>
-      <t>increaseThreadCount</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(i) of Thread Subscriber if exists</t>
-    </r>
-  </si>
-  <si>
-    <t>TestRunningNoMoreWorkTransition</t>
-  </si>
-  <si>
-    <t>N_i &lt; N_max-1</t>
-  </si>
-  <si>
-    <t>THERE ARE NO WAITING THREADS TO RECEIVE THIS EVENT.  THE EFSM WOULD GET STUCK IN THIS MODE.</t>
-  </si>
-  <si>
-    <t>TODO: We cannot enter into NoMoreWork unless we have at least one thread that is computing.  The last thread (Computing or Waiting) to transition to Idle always sets the EFSM mode to Idle.  Therefore there is no transition to this error state</t>
+      <t xml:space="preserve"> this event is triggered by a computing thread =&gt; N_c &gt; 0</t>
+    </r>
+  </si>
+  <si>
+    <t>N_c+1 &gt; 0</t>
+  </si>
+  <si>
+    <t>NEED AT LEAST ONE THREAD TO TRANSITION TO IDLE. Not allowed by specifications.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15">
+  <fonts count="13">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1602,17 +1392,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FF2F75B5"/>
-      <name val="Calibri (Body)"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri (Body)"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1782,7 +1561,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1865,7 +1644,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1876,6 +1655,13 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1901,9 +1687,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2219,11 +2004,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98772F20-44FC-FE45-839B-70D0417F8C61}">
-  <dimension ref="A1:Q108"/>
+  <dimension ref="A1:Q99"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O92" sqref="O92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2250,53 +2035,53 @@
   <sheetData>
     <row r="1" spans="1:17" ht="16" customHeight="1">
       <c r="B1" s="30"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="39"/>
-      <c r="K1" s="39"/>
-      <c r="L1" s="39"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
+      <c r="K1" s="42"/>
+      <c r="L1" s="42"/>
     </row>
     <row r="2" spans="1:17" ht="17" thickBot="1">
       <c r="B2" s="30"/>
     </row>
     <row r="3" spans="1:17" ht="17" thickBot="1">
       <c r="B3" s="30"/>
-      <c r="C3" s="32" t="s">
+      <c r="C3" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="35"/>
-      <c r="J3" s="32" t="s">
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="38"/>
+      <c r="J3" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="K3" s="33"/>
-      <c r="L3" s="33"/>
-      <c r="M3" s="34"/>
-      <c r="N3" s="35"/>
+      <c r="K3" s="36"/>
+      <c r="L3" s="36"/>
+      <c r="M3" s="37"/>
+      <c r="N3" s="38"/>
     </row>
     <row r="4" spans="1:17" ht="17" thickBot="1">
       <c r="B4" s="30"/>
       <c r="C4" s="5"/>
-      <c r="D4" s="36" t="s">
+      <c r="D4" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="38"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="41"/>
       <c r="J4" s="5"/>
-      <c r="K4" s="36" t="s">
+      <c r="K4" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="L4" s="37"/>
-      <c r="M4" s="37"/>
-      <c r="N4" s="38"/>
+      <c r="L4" s="40"/>
+      <c r="M4" s="40"/>
+      <c r="N4" s="41"/>
     </row>
     <row r="5" spans="1:17" ht="17" thickBot="1">
       <c r="B5" s="30"/>
@@ -2304,7 +2089,7 @@
         <v>0</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E5" s="10" t="s">
         <v>13</v>
@@ -2325,7 +2110,7 @@
         <v>0</v>
       </c>
       <c r="K5" s="6" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="L5" s="10" t="s">
         <v>13</v>
@@ -2340,7 +2125,7 @@
         <v>3</v>
       </c>
       <c r="P5" s="23" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="Q5" s="12" t="s">
         <v>35</v>
@@ -2348,7 +2133,7 @@
     </row>
     <row r="6" spans="1:17">
       <c r="B6" s="29" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C6" s="23" t="s">
         <v>4</v>
@@ -2387,10 +2172,10 @@
         <v>8</v>
       </c>
       <c r="O6" s="24" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="P6" s="28" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="Q6" s="12"/>
     </row>
@@ -2409,7 +2194,7 @@
         <v>27</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>27</v>
@@ -2433,13 +2218,13 @@
         <v>8</v>
       </c>
       <c r="O7" s="11" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="P7" s="15" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="Q7" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:17">
@@ -2481,13 +2266,13 @@
         <v>8</v>
       </c>
       <c r="O8" s="11" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="P8" s="15" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="Q8" s="13" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:17">
@@ -2533,7 +2318,7 @@
         <v>23</v>
       </c>
       <c r="P9" s="28" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="10" spans="1:17">
@@ -2557,7 +2342,7 @@
         <v>9</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>5</v>
@@ -2575,10 +2360,10 @@
         <v>0</v>
       </c>
       <c r="O10" s="3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:17">
@@ -2623,7 +2408,7 @@
         <v>23</v>
       </c>
       <c r="P11" s="28" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="Q11" s="13"/>
     </row>
@@ -2666,10 +2451,10 @@
         <v>8</v>
       </c>
       <c r="O12" s="13" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="P12" s="28" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="Q12" s="13"/>
     </row>
@@ -2712,10 +2497,10 @@
         <v>0</v>
       </c>
       <c r="O13" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="P13" s="28" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
     </row>
     <row r="14" spans="1:17">
@@ -2760,7 +2545,7 @@
         <v>24</v>
       </c>
       <c r="P14" s="28" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="Q14" s="13"/>
     </row>
@@ -2806,7 +2591,7 @@
         <v>26</v>
       </c>
       <c r="P15" s="28" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="16" spans="1:17">
@@ -2848,10 +2633,10 @@
         <v>0</v>
       </c>
       <c r="O16" s="13" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="P16" s="31" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
     </row>
     <row r="17" spans="2:17">
@@ -2893,10 +2678,10 @@
         <v>0</v>
       </c>
       <c r="O17" s="3" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="P17" s="31" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
     </row>
     <row r="18" spans="2:17">
@@ -2917,7 +2702,7 @@
         <v>0</v>
       </c>
       <c r="H18" s="14" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>8</v>
@@ -2938,10 +2723,10 @@
         <v>0</v>
       </c>
       <c r="O18" s="13" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="P18" s="31" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="Q18" s="13"/>
     </row>
@@ -2987,7 +2772,7 @@
         <v>46</v>
       </c>
       <c r="P19" s="28" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
     </row>
     <row r="20" spans="2:17">
@@ -3032,7 +2817,7 @@
         <v>25</v>
       </c>
       <c r="P20" s="28" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
     </row>
     <row r="21" spans="2:17">
@@ -3056,7 +2841,7 @@
         <v>11</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="J21" s="1" t="s">
         <v>8</v>
@@ -3077,7 +2862,7 @@
         <v>23</v>
       </c>
       <c r="P21" s="28" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
     </row>
     <row r="22" spans="2:17">
@@ -3095,7 +2880,7 @@
         <v>18</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="H22" s="16" t="s">
         <v>11</v>
@@ -3116,13 +2901,13 @@
         <v>41</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="O22" s="13" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="P22" s="28" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
     </row>
     <row r="23" spans="2:17">
@@ -3140,7 +2925,7 @@
         <v>18</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="H23" s="16" t="s">
         <v>22</v>
@@ -3161,13 +2946,13 @@
         <v>41</v>
       </c>
       <c r="N23" s="4" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="O23" s="11" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="P23" s="28" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="24" spans="2:17">
@@ -3209,10 +2994,10 @@
         <v>0</v>
       </c>
       <c r="O24" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="P24" s="28" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="Q24" s="13"/>
     </row>
@@ -3222,7 +3007,7 @@
         <v>5</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>17</v>
@@ -3255,10 +3040,10 @@
         <v>0</v>
       </c>
       <c r="O25" s="11" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="P25" s="28" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
     </row>
     <row r="26" spans="2:17">
@@ -3276,7 +3061,7 @@
         <v>18</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H26" s="16" t="s">
         <v>28</v>
@@ -3297,13 +3082,13 @@
         <v>41</v>
       </c>
       <c r="N26" s="4" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="O26" s="11" t="s">
         <v>20</v>
       </c>
       <c r="P26" s="15" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="Q26" s="13"/>
     </row>
@@ -3345,14 +3130,11 @@
       <c r="N27" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="O27" s="13" t="s">
-        <v>103</v>
+      <c r="O27" s="34" t="s">
+        <v>138</v>
       </c>
       <c r="P27" s="31" t="s">
-        <v>140</v>
-      </c>
-      <c r="Q27" s="3" t="s">
-        <v>105</v>
+        <v>132</v>
       </c>
     </row>
     <row r="28" spans="2:17">
@@ -3382,7 +3164,7 @@
         <v>5</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L28" s="1" t="s">
         <v>51</v>
@@ -3397,7 +3179,7 @@
         <v>52</v>
       </c>
       <c r="P28" s="28" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
     </row>
     <row r="29" spans="2:17">
@@ -3415,7 +3197,7 @@
         <v>18</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H29" s="14" t="s">
         <v>7</v>
@@ -3436,13 +3218,13 @@
         <v>59</v>
       </c>
       <c r="N29" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="O29" s="3" t="s">
         <v>53</v>
       </c>
       <c r="P29" s="28" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
     </row>
     <row r="30" spans="2:17">
@@ -3451,7 +3233,7 @@
         <v>57</v>
       </c>
       <c r="P30" s="28" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
     </row>
     <row r="31" spans="2:17">
@@ -3469,7 +3251,7 @@
         <v>18</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="H31" s="14" t="s">
         <v>54</v>
@@ -3490,13 +3272,13 @@
         <v>41</v>
       </c>
       <c r="N31" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="O31" s="3" t="s">
         <v>20</v>
       </c>
       <c r="P31" s="1" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
     </row>
     <row r="32" spans="2:17">
@@ -3541,7 +3323,7 @@
         <v>60</v>
       </c>
       <c r="P32" s="31" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
     </row>
     <row r="33" spans="1:17">
@@ -3559,7 +3341,7 @@
         <v>18</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H33" s="14" t="s">
         <v>54</v>
@@ -3580,23 +3362,23 @@
         <v>59</v>
       </c>
       <c r="N33" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="O33" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="P33" s="28" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="34" spans="1:17">
       <c r="B34" s="20"/>
       <c r="H34" s="14"/>
       <c r="O34" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="P34" s="28" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="35" spans="1:17">
@@ -3617,7 +3399,7 @@
         <v>27</v>
       </c>
       <c r="H35" s="14" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="I35" s="1" t="s">
         <v>8</v>
@@ -3637,11 +3419,11 @@
       <c r="N35" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="O35" s="13" t="s">
-        <v>104</v>
+      <c r="O35" s="32" t="s">
+        <v>139</v>
       </c>
       <c r="P35" s="1" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
     </row>
     <row r="36" spans="1:17">
@@ -3662,7 +3444,7 @@
         <v>0</v>
       </c>
       <c r="H36" s="14" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="I36" s="1" t="s">
         <v>8</v>
@@ -3683,10 +3465,10 @@
         <v>0</v>
       </c>
       <c r="O36" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="P36" s="28" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="37" spans="1:17">
@@ -3697,7 +3479,7 @@
         <v>60</v>
       </c>
       <c r="P37" s="28" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="38" spans="1:17">
@@ -3715,10 +3497,10 @@
         <v>32</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H38" s="14" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="I38" s="1" t="s">
         <v>8</v>
@@ -3736,33 +3518,33 @@
         <v>41</v>
       </c>
       <c r="N38" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="O38" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="P38" s="28" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="39" spans="1:17">
       <c r="B39" s="20"/>
       <c r="H39" s="15"/>
       <c r="O39" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="P39" s="28" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="40" spans="1:17">
       <c r="B40" s="20"/>
       <c r="H40" s="15"/>
       <c r="O40" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="P40" s="28" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="41" spans="1:17">
@@ -3779,11 +3561,11 @@
       <c r="F41" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G41" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H41" s="16" t="s">
-        <v>9</v>
+      <c r="G41" s="1">
+        <v>0</v>
+      </c>
+      <c r="H41" s="15" t="s">
+        <v>27</v>
       </c>
       <c r="I41" s="1" t="s">
         <v>33</v>
@@ -3803,12 +3585,13 @@
       <c r="N41" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="O41" s="3" t="s">
-        <v>46</v>
+      <c r="O41" s="34" t="s">
+        <v>137</v>
       </c>
       <c r="P41" s="28" t="s">
-        <v>135</v>
-      </c>
+        <v>117</v>
+      </c>
+      <c r="Q41" s="32"/>
     </row>
     <row r="42" spans="1:17">
       <c r="B42" s="18"/>
@@ -3825,13 +3608,13 @@
         <v>27</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>27</v>
+        <v>85</v>
       </c>
       <c r="H42" s="16" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="J42" s="1" t="s">
         <v>8</v>
@@ -3849,10 +3632,10 @@
         <v>8</v>
       </c>
       <c r="O42" s="3" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="P42" s="28" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="43" spans="1:17">
@@ -3861,7 +3644,7 @@
         <v>49</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>27</v>
@@ -3870,13 +3653,13 @@
         <v>27</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>27</v>
+        <v>85</v>
       </c>
       <c r="H43" s="16" t="s">
         <v>11</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="J43" s="1" t="s">
         <v>8</v>
@@ -3894,10 +3677,10 @@
         <v>8</v>
       </c>
       <c r="O43" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="P43" s="28" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="44" spans="1:17">
@@ -3909,40 +3692,40 @@
         <v>19</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="H44" s="16" t="s">
         <v>11</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>48</v>
+        <v>97</v>
       </c>
       <c r="J44" s="1" t="s">
-        <v>49</v>
+        <v>8</v>
       </c>
       <c r="K44" s="1" t="s">
-        <v>45</v>
+        <v>8</v>
       </c>
       <c r="L44" s="1" t="s">
-        <v>42</v>
+        <v>8</v>
       </c>
       <c r="M44" s="1" t="s">
-        <v>41</v>
+        <v>8</v>
       </c>
       <c r="N44" s="1" t="s">
-        <v>98</v>
+        <v>8</v>
       </c>
       <c r="O44" s="3" t="s">
-        <v>108</v>
+        <v>23</v>
       </c>
       <c r="P44" s="28" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="45" spans="1:17">
@@ -3951,43 +3734,43 @@
         <v>49</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>27</v>
+        <v>85</v>
       </c>
       <c r="H45" s="16" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="J45" s="1" t="s">
-        <v>8</v>
+        <v>49</v>
       </c>
       <c r="K45" s="1" t="s">
-        <v>8</v>
+        <v>45</v>
       </c>
       <c r="L45" s="1" t="s">
-        <v>8</v>
+        <v>42</v>
       </c>
       <c r="M45" s="1" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="N45" s="1" t="s">
-        <v>8</v>
+        <v>95</v>
       </c>
       <c r="O45" s="3" t="s">
-        <v>44</v>
+        <v>102</v>
       </c>
       <c r="P45" s="28" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
     </row>
     <row r="46" spans="1:17">
@@ -4005,13 +3788,13 @@
         <v>27</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>27</v>
+        <v>85</v>
       </c>
       <c r="H46" s="16" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="J46" s="1" t="s">
         <v>8</v>
@@ -4029,10 +3812,10 @@
         <v>8</v>
       </c>
       <c r="O46" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="P46" s="28" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="47" spans="1:17">
@@ -4040,8 +3823,8 @@
       <c r="C47" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D47" s="1">
-        <v>0</v>
+      <c r="D47" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>27</v>
@@ -4050,10 +3833,10 @@
         <v>27</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H47" s="14" t="s">
-        <v>7</v>
+        <v>85</v>
+      </c>
+      <c r="H47" s="16" t="s">
+        <v>28</v>
       </c>
       <c r="I47" s="1" t="s">
         <v>8</v>
@@ -4073,14 +3856,11 @@
       <c r="N47" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="O47" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="P47" s="31" t="s">
-        <v>140</v>
-      </c>
-      <c r="Q47" s="13" t="s">
-        <v>105</v>
+      <c r="O47" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="P47" s="28" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="48" spans="1:17">
@@ -4088,17 +3868,17 @@
       <c r="C48" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D48" s="1" t="s">
-        <v>16</v>
+      <c r="D48" s="1">
+        <v>0</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G48" s="1">
-        <v>0</v>
+        <v>27</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>85</v>
       </c>
       <c r="H48" s="14" t="s">
         <v>7</v>
@@ -4107,157 +3887,192 @@
         <v>8</v>
       </c>
       <c r="J48" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K48" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L48" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M48" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N48" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="O48" s="34" t="s">
+        <v>138</v>
+      </c>
+      <c r="P48" s="31" t="s">
+        <v>132</v>
+      </c>
+      <c r="Q48" s="13"/>
+    </row>
+    <row r="49" spans="2:16">
+      <c r="B49" s="18"/>
+      <c r="C49" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G49" s="1">
+        <v>1</v>
+      </c>
+      <c r="H49" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="I49" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J49" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="K48" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="L48" s="1" t="s">
+      <c r="K49" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L49" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="M48" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="N48" s="1">
-        <v>0</v>
-      </c>
-      <c r="O48" s="3" t="s">
+      <c r="M49" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="N49" s="1">
+        <v>0</v>
+      </c>
+      <c r="O49" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="P49" s="28" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="50" spans="2:16">
+      <c r="B50" s="20"/>
+      <c r="O50" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="P48" s="31" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="49" spans="2:17">
-      <c r="B49" s="20"/>
-      <c r="H49" s="14"/>
-      <c r="O49" s="13" t="s">
-        <v>120</v>
-      </c>
-      <c r="P49" s="31" t="s">
-        <v>140</v>
-      </c>
-      <c r="Q49" s="13"/>
-    </row>
-    <row r="50" spans="2:17">
-      <c r="B50" s="18"/>
-      <c r="C50" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G50" s="1">
-        <v>1</v>
-      </c>
-      <c r="H50" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="I50" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J50" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="K50" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="L50" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="M50" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="N50" s="1">
-        <v>0</v>
-      </c>
-      <c r="O50" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="P50" s="28" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="51" spans="2:17">
+      <c r="P50" s="31" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="51" spans="2:16">
       <c r="B51" s="20"/>
       <c r="O51" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="P51" s="31" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="52" spans="2:17">
-      <c r="B52" s="20"/>
+        <v>56</v>
+      </c>
+      <c r="P51" s="28" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="52" spans="2:16">
+      <c r="B52" s="18"/>
+      <c r="C52" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="H52" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="I52" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J52" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="K52" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L52" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M52" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="N52" s="1" t="s">
+        <v>101</v>
+      </c>
       <c r="O52" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="P52" s="28" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="53" spans="2:16">
+      <c r="B53" s="20"/>
+      <c r="H53" s="14"/>
+      <c r="O53" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="P52" s="28" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="53" spans="2:17">
-      <c r="B53" s="18"/>
-      <c r="C53" s="1" t="s">
+      <c r="P53" s="28" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="54" spans="2:16">
+      <c r="B54" s="18"/>
+      <c r="C54" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D53" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F53" s="1" t="s">
+      <c r="D54" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E54" s="1">
+        <v>0</v>
+      </c>
+      <c r="F54" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G53" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="H53" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="I53" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J53" s="1" t="s">
+      <c r="G54" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="H54" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="I54" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J54" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="K53" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="L53" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="M53" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="N53" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="O53" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="P53" s="28" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="54" spans="2:17">
-      <c r="B54" s="20"/>
-      <c r="H54" s="14"/>
+      <c r="K54" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L54" s="1">
+        <v>0</v>
+      </c>
+      <c r="M54" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="N54" s="1" t="s">
+        <v>95</v>
+      </c>
       <c r="O54" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="P54" s="28" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="55" spans="2:17">
+        <v>20</v>
+      </c>
+      <c r="P54" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="55" spans="2:16">
       <c r="B55" s="18"/>
       <c r="C55" s="1" t="s">
         <v>49</v>
@@ -4265,14 +4080,14 @@
       <c r="D55" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E55" s="1">
-        <v>0</v>
+      <c r="E55" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="F55" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G55" s="1" t="s">
-        <v>97</v>
+      <c r="G55" s="1">
+        <v>1</v>
       </c>
       <c r="H55" s="14" t="s">
         <v>54</v>
@@ -4281,441 +4096,512 @@
         <v>8</v>
       </c>
       <c r="J55" s="1" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="K55" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="L55" s="1">
-        <v>0</v>
+      <c r="L55" s="1" t="s">
+        <v>74</v>
       </c>
       <c r="M55" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="N55" s="1" t="s">
-        <v>98</v>
+        <v>140</v>
+      </c>
+      <c r="N55" s="1">
+        <v>0</v>
       </c>
       <c r="O55" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="P55" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="56" spans="2:17">
-      <c r="B56" s="18"/>
-      <c r="C56" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="P55" s="31" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="56" spans="2:16">
+      <c r="B56" s="20"/>
+      <c r="H56" s="14"/>
+      <c r="O56" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="P56" s="31" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="57" spans="2:16">
+      <c r="B57" s="20"/>
+      <c r="H57" s="14"/>
+      <c r="O57" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="P57" s="31" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="58" spans="2:16">
+      <c r="B58" s="18"/>
+      <c r="C58" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D56" s="1" t="s">
+      <c r="D58" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E56" s="1" t="s">
+      <c r="E58" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F56" s="1" t="s">
+      <c r="F58" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G56" s="1">
-        <v>0</v>
-      </c>
-      <c r="H56" s="14" t="s">
+      <c r="G58" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="H58" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="I56" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J56" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="K56" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="L56" s="1" t="s">
+      <c r="I58" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J58" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="K58" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L58" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="M58" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="N58" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="O58" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="M56" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="N56" s="1">
-        <v>0</v>
-      </c>
-      <c r="O56" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="P56" s="31" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="57" spans="2:17">
-      <c r="B57" s="18"/>
-      <c r="C57" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E57" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F57" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G57" s="1">
-        <v>1</v>
-      </c>
-      <c r="H57" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="I57" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J57" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="K57" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="L57" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="M57" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="N57" s="1">
-        <v>0</v>
-      </c>
-      <c r="O57" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="P57" s="31" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="58" spans="2:17">
-      <c r="B58" s="20"/>
-      <c r="H58" s="14"/>
-      <c r="O58" s="3" t="s">
-        <v>77</v>
-      </c>
       <c r="P58" s="31" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="59" spans="2:17">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="59" spans="2:16">
       <c r="B59" s="20"/>
       <c r="H59" s="14"/>
       <c r="O59" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="P59" s="31" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="60" spans="2:17">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="60" spans="2:16">
       <c r="B60" s="18"/>
       <c r="C60" s="1" t="s">
         <v>49</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F60" s="1" t="s">
-        <v>18</v>
+        <v>27</v>
+      </c>
+      <c r="F60" s="1">
+        <v>0</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>106</v>
+        <v>85</v>
       </c>
       <c r="H60" s="14" t="s">
-        <v>54</v>
+        <v>88</v>
       </c>
       <c r="I60" s="1" t="s">
         <v>8</v>
       </c>
       <c r="J60" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K60" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L60" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M60" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N60" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="O60" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="P60" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="61" spans="2:16">
+      <c r="B61" s="18"/>
+      <c r="C61" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="K60" s="1" t="s">
+      <c r="D61" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G61" s="1">
+        <v>1</v>
+      </c>
+      <c r="H61" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="I61" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J61" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K61" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="L60" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="M60" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="N60" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="O60" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="P60" s="31" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="61" spans="2:17">
-      <c r="B61" s="20"/>
-      <c r="H61" s="14"/>
+      <c r="L61" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M61" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N61" s="1">
+        <v>0</v>
+      </c>
       <c r="O61" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="P61" s="31" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="62" spans="2:17">
-      <c r="B62" s="18"/>
-      <c r="C62" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E62" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F62" s="1">
-        <v>0</v>
-      </c>
-      <c r="G62" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H62" s="14" t="s">
-        <v>91</v>
-      </c>
-      <c r="I62" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J62" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K62" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L62" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="M62" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="N62" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="O62" s="13" t="s">
-        <v>104</v>
-      </c>
-      <c r="P62" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="63" spans="2:17">
-      <c r="B63" s="18"/>
-      <c r="C63" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E63" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F63" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G63" s="1">
-        <v>0</v>
-      </c>
-      <c r="H63" s="14" t="s">
-        <v>91</v>
-      </c>
-      <c r="I63" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J63" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="K63" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="L63" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="M63" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="N63" s="1">
-        <v>0</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="P61" s="28" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="62" spans="2:16">
+      <c r="B62" s="20"/>
+      <c r="H62" s="15"/>
+      <c r="O62" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="P62" s="28" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="63" spans="2:16">
+      <c r="B63" s="20"/>
+      <c r="H63" s="15"/>
       <c r="O63" s="3" t="s">
         <v>80</v>
       </c>
       <c r="P63" s="31" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="64" spans="2:17">
-      <c r="B64" s="18"/>
-      <c r="H64" s="14"/>
-      <c r="O64" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="P64" s="31" t="s">
-        <v>140</v>
-      </c>
-      <c r="Q64" s="13"/>
+        <v>132</v>
+      </c>
+    </row>
+    <row r="64" spans="2:16">
+      <c r="B64" s="20"/>
+      <c r="H64" s="15"/>
+      <c r="O64" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="P64" s="28" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="65" spans="2:17">
-      <c r="B65" s="20"/>
-      <c r="H65" s="17"/>
+      <c r="B65" s="18"/>
+      <c r="C65" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="H65" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="I65" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J65" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="K65" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L65" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M65" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="N65" s="1" t="s">
+        <v>101</v>
+      </c>
       <c r="O65" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="P65" s="31" t="s">
-        <v>140</v>
+        <v>69</v>
+      </c>
+      <c r="P65" s="28" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="66" spans="2:17">
-      <c r="B66" s="18"/>
-      <c r="C66" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E66" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F66" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G66" s="1">
-        <v>1</v>
-      </c>
-      <c r="H66" s="14" t="s">
-        <v>91</v>
-      </c>
-      <c r="I66" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J66" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="K66" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="L66" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="M66" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="N66" s="1">
-        <v>0</v>
-      </c>
+      <c r="B66" s="26"/>
+      <c r="H66" s="17"/>
       <c r="O66" s="3" t="s">
         <v>70</v>
       </c>
       <c r="P66" s="28" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
     </row>
     <row r="67" spans="2:17">
-      <c r="B67" s="20"/>
-      <c r="H67" s="15"/>
+      <c r="B67" s="27"/>
+      <c r="H67" s="17"/>
       <c r="O67" s="3" t="s">
         <v>71</v>
       </c>
       <c r="P67" s="28" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
     </row>
     <row r="68" spans="2:17">
-      <c r="B68" s="20"/>
-      <c r="H68" s="15"/>
-      <c r="O68" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="P68" s="31" t="s">
-        <v>140</v>
-      </c>
+      <c r="B68" s="43"/>
+      <c r="C68" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G68" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H68" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I68" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J68" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K68" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L68" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M68" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N68" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="O68" s="34" t="s">
+        <v>141</v>
+      </c>
+      <c r="P68" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q68" s="32"/>
     </row>
     <row r="69" spans="2:17">
-      <c r="B69" s="20"/>
-      <c r="H69" s="15"/>
-      <c r="O69" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="P69" s="28" t="s">
-        <v>138</v>
+      <c r="B69" s="18"/>
+      <c r="C69" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D69" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G69" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="H69" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I69" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J69" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K69" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L69" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M69" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N69" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="O69" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="P69" s="1" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="70" spans="2:17">
       <c r="B70" s="18"/>
       <c r="C70" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D70" s="1" t="s">
-        <v>19</v>
+        <v>38</v>
+      </c>
+      <c r="D70" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G70" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="H70" s="14" t="s">
-        <v>91</v>
+        <v>27</v>
+      </c>
+      <c r="G70" s="1">
+        <v>0</v>
+      </c>
+      <c r="H70" s="16" t="s">
+        <v>9</v>
       </c>
       <c r="I70" s="1" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="J70" s="1" t="s">
-        <v>49</v>
+        <v>8</v>
       </c>
       <c r="K70" s="1" t="s">
-        <v>45</v>
+        <v>8</v>
       </c>
       <c r="L70" s="1" t="s">
-        <v>42</v>
+        <v>8</v>
       </c>
       <c r="M70" s="1" t="s">
-        <v>41</v>
+        <v>8</v>
       </c>
       <c r="N70" s="1" t="s">
-        <v>107</v>
+        <v>8</v>
       </c>
       <c r="O70" s="3" t="s">
-        <v>70</v>
+        <v>46</v>
       </c>
       <c r="P70" s="28" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
     </row>
     <row r="71" spans="2:17">
-      <c r="B71" s="26"/>
-      <c r="H71" s="17"/>
-      <c r="O71" s="3" t="s">
-        <v>71</v>
+      <c r="B71" s="18"/>
+      <c r="C71" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D71" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G71" s="1">
+        <v>0</v>
+      </c>
+      <c r="H71" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="I71" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J71" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K71" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L71" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M71" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N71" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="O71" s="13" t="s">
+        <v>25</v>
       </c>
       <c r="P71" s="28" t="s">
-        <v>138</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="Q71" s="13"/>
     </row>
     <row r="72" spans="2:17">
-      <c r="B72" s="27"/>
-      <c r="H72" s="17"/>
-      <c r="O72" s="3" t="s">
-        <v>72</v>
+      <c r="B72" s="18"/>
+      <c r="C72" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G72" s="1">
+        <v>0</v>
+      </c>
+      <c r="H72" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="I72" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="J72" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K72" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L72" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M72" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N72" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="O72" s="13" t="s">
+        <v>23</v>
       </c>
       <c r="P72" s="28" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
     </row>
     <row r="73" spans="2:17">
@@ -4724,52 +4610,53 @@
         <v>38</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G73" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="H73" s="1" t="s">
-        <v>27</v>
+        <v>18</v>
+      </c>
+      <c r="G73" s="1">
+        <v>0</v>
+      </c>
+      <c r="H73" s="16" t="s">
+        <v>11</v>
       </c>
       <c r="I73" s="1" t="s">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="J73" s="1" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="K73" s="1" t="s">
-        <v>8</v>
+        <v>45</v>
       </c>
       <c r="L73" s="1" t="s">
-        <v>8</v>
+        <v>42</v>
       </c>
       <c r="M73" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="N73" s="1" t="s">
-        <v>8</v>
+        <v>41</v>
+      </c>
+      <c r="N73" s="1">
+        <v>0</v>
       </c>
       <c r="O73" s="13" t="s">
-        <v>109</v>
-      </c>
-      <c r="P73" s="1" t="s">
-        <v>125</v>
-      </c>
+        <v>133</v>
+      </c>
+      <c r="P73" s="28" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q73" s="13"/>
     </row>
     <row r="74" spans="2:17">
       <c r="B74" s="18"/>
       <c r="C74" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D74" s="1" t="s">
-        <v>27</v>
+      <c r="D74" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="E74" s="1" t="s">
         <v>27</v>
@@ -4781,10 +4668,10 @@
         <v>0</v>
       </c>
       <c r="H74" s="16" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="I74" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="J74" s="1" t="s">
         <v>8</v>
@@ -4802,10 +4689,10 @@
         <v>8</v>
       </c>
       <c r="O74" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="P74" s="28" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
     </row>
     <row r="75" spans="2:17">
@@ -4813,8 +4700,8 @@
       <c r="C75" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D75" s="1" t="s">
-        <v>27</v>
+      <c r="D75" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="E75" s="1" t="s">
         <v>27</v>
@@ -4826,10 +4713,10 @@
         <v>0</v>
       </c>
       <c r="H75" s="16" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="I75" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="J75" s="1" t="s">
         <v>8</v>
@@ -4846,21 +4733,20 @@
       <c r="N75" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="O75" s="13" t="s">
-        <v>25</v>
+      <c r="O75" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="P75" s="28" t="s">
-        <v>136</v>
-      </c>
-      <c r="Q75" s="13"/>
+        <v>128</v>
+      </c>
     </row>
     <row r="76" spans="2:17">
       <c r="B76" s="18"/>
       <c r="C76" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D76" s="1" t="s">
-        <v>19</v>
+      <c r="D76" s="1">
+        <v>0</v>
       </c>
       <c r="E76" s="1" t="s">
         <v>27</v>
@@ -4871,11 +4757,11 @@
       <c r="G76" s="1">
         <v>0</v>
       </c>
-      <c r="H76" s="16" t="s">
-        <v>11</v>
+      <c r="H76" s="14" t="s">
+        <v>7</v>
       </c>
       <c r="I76" s="1" t="s">
-        <v>100</v>
+        <v>8</v>
       </c>
       <c r="J76" s="1" t="s">
         <v>8</v>
@@ -4892,12 +4778,13 @@
       <c r="N76" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="O76" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="P76" s="28" t="s">
-        <v>136</v>
-      </c>
+      <c r="O76" s="34" t="s">
+        <v>138</v>
+      </c>
+      <c r="P76" s="31" t="s">
+        <v>132</v>
+      </c>
+      <c r="Q76" s="25"/>
     </row>
     <row r="77" spans="2:17">
       <c r="B77" s="18"/>
@@ -4905,7 +4792,7 @@
         <v>38</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>19</v>
+        <v>110</v>
       </c>
       <c r="E77" s="1" t="s">
         <v>17</v>
@@ -4916,11 +4803,11 @@
       <c r="G77" s="1">
         <v>0</v>
       </c>
-      <c r="H77" s="16" t="s">
-        <v>11</v>
+      <c r="H77" s="14" t="s">
+        <v>7</v>
       </c>
       <c r="I77" s="1" t="s">
-        <v>48</v>
+        <v>8</v>
       </c>
       <c r="J77" s="1" t="s">
         <v>38</v>
@@ -4937,57 +4824,59 @@
       <c r="N77" s="1">
         <v>0</v>
       </c>
-      <c r="O77" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="P77" s="28" t="s">
-        <v>139</v>
-      </c>
-      <c r="Q77" s="13"/>
-    </row>
-    <row r="78" spans="2:17">
+      <c r="O77" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="P77" s="31" t="s">
+        <v>132</v>
+      </c>
+      <c r="Q77" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="78" spans="2:17" ht="17" customHeight="1">
       <c r="B78" s="18"/>
       <c r="C78" s="1" t="s">
         <v>38</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E78" s="1" t="s">
-        <v>27</v>
+        <v>15</v>
+      </c>
+      <c r="E78" s="1">
+        <v>0</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="G78" s="1">
         <v>0</v>
       </c>
-      <c r="H78" s="16" t="s">
-        <v>22</v>
+      <c r="H78" s="14" t="s">
+        <v>54</v>
       </c>
       <c r="I78" s="1" t="s">
-        <v>34</v>
+        <v>8</v>
       </c>
       <c r="J78" s="1" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="K78" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L78" s="1" t="s">
-        <v>8</v>
+        <v>45</v>
+      </c>
+      <c r="L78" s="1">
+        <v>0</v>
       </c>
       <c r="M78" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="N78" s="1" t="s">
-        <v>8</v>
+        <v>41</v>
+      </c>
+      <c r="N78" s="1">
+        <v>0</v>
       </c>
       <c r="O78" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="P78" s="28" t="s">
-        <v>136</v>
+        <v>20</v>
+      </c>
+      <c r="P78" s="1" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="79" spans="2:17">
@@ -4996,171 +4885,200 @@
         <v>38</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E79" s="1" t="s">
-        <v>27</v>
+        <v>135</v>
+      </c>
+      <c r="E79" s="1">
+        <v>1</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="G79" s="1">
         <v>0</v>
       </c>
-      <c r="H79" s="16" t="s">
-        <v>28</v>
+      <c r="H79" s="14" t="s">
+        <v>54</v>
       </c>
       <c r="I79" s="1" t="s">
         <v>8</v>
       </c>
       <c r="J79" s="1" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="K79" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L79" s="1" t="s">
-        <v>8</v>
+        <v>113</v>
+      </c>
+      <c r="L79" s="1">
+        <v>0</v>
       </c>
       <c r="M79" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="N79" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="O79" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="P79" s="28" t="s">
-        <v>136</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="N79" s="1">
+        <v>0</v>
+      </c>
+      <c r="O79" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="P79" s="33" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q79" s="13"/>
     </row>
     <row r="80" spans="2:17">
       <c r="B80" s="18"/>
       <c r="C80" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D80" s="1">
-        <v>0</v>
-      </c>
-      <c r="E80" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F80" s="1" t="s">
-        <v>27</v>
+      <c r="D80" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E80" s="1">
+        <v>1</v>
+      </c>
+      <c r="F80" s="1">
+        <v>0</v>
       </c>
       <c r="G80" s="1">
         <v>0</v>
       </c>
       <c r="H80" s="14" t="s">
-        <v>7</v>
+        <v>54</v>
       </c>
       <c r="I80" s="1" t="s">
         <v>8</v>
       </c>
       <c r="J80" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="K80" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L80" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="M80" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="N80" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="O80" s="13" t="s">
-        <v>103</v>
+        <v>39</v>
+      </c>
+      <c r="L80" s="1">
+        <v>0</v>
+      </c>
+      <c r="M80" s="1">
+        <v>0</v>
+      </c>
+      <c r="N80" s="1">
+        <v>0</v>
+      </c>
+      <c r="O80" s="11" t="s">
+        <v>63</v>
       </c>
       <c r="P80" s="31" t="s">
-        <v>140</v>
-      </c>
-      <c r="Q80" s="25" t="s">
-        <v>116</v>
+        <v>132</v>
       </c>
     </row>
     <row r="81" spans="2:17">
-      <c r="B81" s="18"/>
-      <c r="C81" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D81" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E81" s="1">
-        <v>0</v>
-      </c>
-      <c r="F81" s="1">
-        <v>0</v>
-      </c>
-      <c r="G81" s="1">
-        <v>0</v>
-      </c>
-      <c r="H81" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="I81" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J81" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="K81" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="L81" s="1">
-        <v>0</v>
-      </c>
-      <c r="M81" s="1">
-        <v>0</v>
-      </c>
-      <c r="N81" s="1">
-        <v>0</v>
-      </c>
-      <c r="O81" s="11" t="s">
-        <v>64</v>
+      <c r="B81" s="20"/>
+      <c r="H81" s="14"/>
+      <c r="O81" s="3" t="s">
+        <v>108</v>
       </c>
       <c r="P81" s="31" t="s">
-        <v>140</v>
-      </c>
-      <c r="Q81" s="13"/>
+        <v>132</v>
+      </c>
     </row>
     <row r="82" spans="2:17">
       <c r="B82" s="20"/>
       <c r="H82" s="14"/>
-      <c r="O82" s="13" t="s">
+      <c r="O82" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="P82" s="31" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="83" spans="2:17">
+      <c r="B83" s="18"/>
+      <c r="C83" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G83" s="1">
+        <v>0</v>
+      </c>
+      <c r="H83" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="I83" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J83" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K83" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="L83" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="M83" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="N83" s="1">
+        <v>0</v>
+      </c>
+      <c r="O83" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="P83" s="33" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="84" spans="2:17">
+      <c r="B84" s="18"/>
+      <c r="C84" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F84" s="1">
+        <v>0</v>
+      </c>
+      <c r="G84" s="1">
+        <v>0</v>
+      </c>
+      <c r="H84" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="P82" s="31" t="s">
-        <v>140</v>
-      </c>
-      <c r="Q82" s="13"/>
-    </row>
-    <row r="83" spans="2:17">
-      <c r="B83" s="20"/>
-      <c r="H83" s="14"/>
-      <c r="O83" s="13" t="s">
-        <v>114</v>
-      </c>
-      <c r="P83" s="31" t="s">
-        <v>140</v>
-      </c>
-      <c r="Q83" s="13"/>
-    </row>
-    <row r="84" spans="2:17">
-      <c r="B84" s="20"/>
-      <c r="H84" s="14"/>
-      <c r="O84" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="P84" s="31" t="s">
-        <v>140</v>
-      </c>
-      <c r="Q84" s="13"/>
+      <c r="I84" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J84" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K84" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L84" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M84" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N84" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="O84" s="32" t="s">
+        <v>139</v>
+      </c>
+      <c r="P84" s="1" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="85" spans="2:17">
       <c r="B85" s="18"/>
@@ -5168,19 +5086,19 @@
         <v>38</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>117</v>
+        <v>135</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="G85" s="1">
         <v>0</v>
       </c>
       <c r="H85" s="14" t="s">
-        <v>7</v>
+        <v>88</v>
       </c>
       <c r="I85" s="1" t="s">
         <v>8</v>
@@ -5189,71 +5107,34 @@
         <v>38</v>
       </c>
       <c r="K85" s="1" t="s">
-        <v>45</v>
+        <v>113</v>
       </c>
       <c r="L85" s="1" t="s">
         <v>42</v>
       </c>
       <c r="M85" s="1" t="s">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="N85" s="1">
         <v>0</v>
       </c>
-      <c r="O85" s="3" t="s">
-        <v>73</v>
+      <c r="O85" s="13" t="s">
+        <v>79</v>
       </c>
       <c r="P85" s="31" t="s">
-        <v>140</v>
-      </c>
-      <c r="Q85" s="3" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="86" spans="2:17" ht="17" customHeight="1">
-      <c r="B86" s="18"/>
-      <c r="C86" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D86" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E86" s="1">
-        <v>0</v>
-      </c>
-      <c r="F86" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G86" s="1">
-        <v>0</v>
-      </c>
-      <c r="H86" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="I86" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J86" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="K86" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="L86" s="1">
-        <v>0</v>
-      </c>
-      <c r="M86" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="N86" s="1">
-        <v>0</v>
-      </c>
-      <c r="O86" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="P86" s="1" t="s">
-        <v>133</v>
-      </c>
+        <v>132</v>
+      </c>
+    </row>
+    <row r="86" spans="2:17">
+      <c r="B86" s="20"/>
+      <c r="H86" s="14"/>
+      <c r="O86" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="P86" s="31" t="s">
+        <v>132</v>
+      </c>
+      <c r="Q86" s="13"/>
     </row>
     <row r="87" spans="2:17">
       <c r="B87" s="18"/>
@@ -5261,91 +5142,53 @@
         <v>38</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>39</v>
+        <v>135</v>
       </c>
       <c r="E87" s="1">
         <v>0</v>
       </c>
-      <c r="F87" s="1">
-        <v>0</v>
+      <c r="F87" s="1" t="s">
+        <v>58</v>
       </c>
       <c r="G87" s="1">
         <v>0</v>
       </c>
       <c r="H87" s="14" t="s">
-        <v>54</v>
+        <v>88</v>
       </c>
       <c r="I87" s="1" t="s">
         <v>8</v>
       </c>
       <c r="J87" s="1" t="s">
-        <v>4</v>
+        <v>38</v>
       </c>
       <c r="K87" s="1" t="s">
-        <v>39</v>
+        <v>113</v>
       </c>
       <c r="L87" s="1">
         <v>0</v>
       </c>
-      <c r="M87" s="1">
-        <v>0</v>
+      <c r="M87" s="1" t="s">
+        <v>104</v>
       </c>
       <c r="N87" s="1">
         <v>0</v>
       </c>
-      <c r="O87" s="41" t="s">
-        <v>144</v>
-      </c>
-      <c r="P87" s="31" t="s">
-        <v>140</v>
-      </c>
-      <c r="Q87" s="13" t="s">
-        <v>145</v>
+      <c r="O87" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="P87" s="33" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="88" spans="2:17">
-      <c r="B88" s="18"/>
-      <c r="C88" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D88" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="E88" s="1">
-        <v>1</v>
-      </c>
-      <c r="F88" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G88" s="1">
-        <v>0</v>
-      </c>
-      <c r="H88" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="I88" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J88" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="K88" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="L88" s="1">
-        <v>0</v>
-      </c>
-      <c r="M88" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="N88" s="1">
-        <v>0</v>
-      </c>
+      <c r="B88" s="20"/>
+      <c r="H88" s="14"/>
       <c r="O88" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="P88" s="40" t="s">
-        <v>142</v>
+        <v>61</v>
+      </c>
+      <c r="P88" s="33" t="s">
+        <v>134</v>
       </c>
       <c r="Q88" s="13"/>
     </row>
@@ -5358,16 +5201,16 @@
         <v>21</v>
       </c>
       <c r="E89" s="1">
+        <v>0</v>
+      </c>
+      <c r="F89" s="1">
         <v>1</v>
       </c>
-      <c r="F89" s="1">
-        <v>0</v>
-      </c>
       <c r="G89" s="1">
         <v>0</v>
       </c>
       <c r="H89" s="14" t="s">
-        <v>54</v>
+        <v>88</v>
       </c>
       <c r="I89" s="1" t="s">
         <v>8</v>
@@ -5387,335 +5230,68 @@
       <c r="N89" s="1">
         <v>0</v>
       </c>
-      <c r="O89" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="P89" s="31" t="s">
-        <v>140</v>
+      <c r="O89" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="P89" s="33" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="90" spans="2:17">
       <c r="B90" s="20"/>
-      <c r="H90" s="14"/>
-      <c r="O90" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="P90" s="31" t="s">
-        <v>140</v>
+      <c r="H90" s="17"/>
+      <c r="O90" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="P90" s="33" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="91" spans="2:17">
       <c r="B91" s="20"/>
-      <c r="H91" s="14"/>
-      <c r="O91" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="P91" s="31" t="s">
-        <v>140</v>
+      <c r="H91" s="17"/>
+      <c r="O91" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="P91" s="33" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="92" spans="2:17">
-      <c r="B92" s="18"/>
-      <c r="C92" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D92" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="E92" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="F92" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G92" s="1">
-        <v>0</v>
-      </c>
-      <c r="H92" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="I92" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J92" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="K92" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="L92" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="M92" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="N92" s="1">
-        <v>0</v>
-      </c>
-      <c r="O92" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="P92" s="40" t="s">
-        <v>142</v>
-      </c>
+      <c r="B92" s="20"/>
+      <c r="H92" s="17"/>
+      <c r="O92" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="P92" s="33" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q92" s="13"/>
     </row>
     <row r="93" spans="2:17">
-      <c r="B93" s="18"/>
-      <c r="C93" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D93" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E93" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F93" s="1">
-        <v>0</v>
-      </c>
-      <c r="G93" s="1">
-        <v>0</v>
-      </c>
-      <c r="H93" s="14" t="s">
-        <v>91</v>
-      </c>
-      <c r="I93" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J93" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K93" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L93" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="M93" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="N93" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="O93" s="13" t="s">
-        <v>104</v>
-      </c>
-      <c r="P93" s="1" t="s">
-        <v>133</v>
-      </c>
+      <c r="H93" s="15"/>
+      <c r="O93"/>
+      <c r="Q93"/>
     </row>
     <row r="94" spans="2:17">
-      <c r="B94" s="18"/>
-      <c r="C94" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D94" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="E94" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F94" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G94" s="1">
-        <v>0</v>
-      </c>
-      <c r="H94" s="14" t="s">
-        <v>91</v>
-      </c>
-      <c r="I94" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J94" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="K94" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="L94" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="M94" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="N94" s="1">
-        <v>0</v>
-      </c>
-      <c r="O94" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="P94" s="31" t="s">
-        <v>140</v>
-      </c>
+      <c r="H94" s="15"/>
+      <c r="O94"/>
+      <c r="Q94"/>
     </row>
     <row r="95" spans="2:17">
-      <c r="B95" s="20"/>
       <c r="H95" s="14"/>
-      <c r="O95" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="P95" s="31" t="s">
-        <v>140</v>
-      </c>
-      <c r="Q95" s="13"/>
     </row>
     <row r="96" spans="2:17">
-      <c r="B96" s="18"/>
-      <c r="C96" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D96" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="E96" s="1">
-        <v>0</v>
-      </c>
-      <c r="F96" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="G96" s="1">
-        <v>0</v>
-      </c>
-      <c r="H96" s="14" t="s">
-        <v>91</v>
-      </c>
-      <c r="I96" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J96" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="K96" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="L96" s="1">
-        <v>0</v>
-      </c>
-      <c r="M96" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="N96" s="1">
-        <v>0</v>
-      </c>
-      <c r="O96" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="P96" s="40" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="97" spans="2:17">
-      <c r="B97" s="20"/>
+      <c r="H96" s="14"/>
+    </row>
+    <row r="97" spans="8:8">
       <c r="H97" s="14"/>
-      <c r="O97" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="P97" s="40" t="s">
-        <v>142</v>
-      </c>
-      <c r="Q97" s="13"/>
-    </row>
-    <row r="98" spans="2:17">
-      <c r="B98" s="18"/>
-      <c r="C98" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D98" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E98" s="1">
-        <v>0</v>
-      </c>
-      <c r="F98" s="1">
-        <v>1</v>
-      </c>
-      <c r="G98" s="1">
-        <v>0</v>
-      </c>
-      <c r="H98" s="14" t="s">
-        <v>91</v>
-      </c>
-      <c r="I98" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J98" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="K98" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="L98" s="1">
-        <v>0</v>
-      </c>
-      <c r="M98" s="1">
-        <v>0</v>
-      </c>
-      <c r="N98" s="1">
-        <v>0</v>
-      </c>
-      <c r="O98" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="P98" s="40" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="99" spans="2:17">
-      <c r="B99" s="20"/>
-      <c r="H99" s="17"/>
-      <c r="O99" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="P99" s="40" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="100" spans="2:17">
-      <c r="B100" s="20"/>
-      <c r="H100" s="17"/>
-      <c r="O100" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="P100" s="40" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="101" spans="2:17">
-      <c r="B101" s="20"/>
-      <c r="H101" s="17"/>
-      <c r="O101" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="P101" s="40" t="s">
-        <v>142</v>
-      </c>
-      <c r="Q101" s="13"/>
-    </row>
-    <row r="102" spans="2:17">
-      <c r="H102" s="15"/>
-      <c r="O102"/>
-      <c r="Q102"/>
-    </row>
-    <row r="103" spans="2:17">
-      <c r="H103" s="15"/>
-      <c r="O103"/>
-      <c r="Q103"/>
-    </row>
-    <row r="104" spans="2:17">
-      <c r="H104" s="14"/>
-    </row>
-    <row r="105" spans="2:17">
-      <c r="H105" s="14"/>
-    </row>
-    <row r="106" spans="2:17">
-      <c r="H106" s="14"/>
-    </row>
-    <row r="107" spans="2:17">
-      <c r="H107" s="14"/>
-    </row>
-    <row r="108" spans="2:17">
-      <c r="H108" s="15"/>
+    </row>
+    <row r="98" spans="8:8">
+      <c r="H98" s="14"/>
+    </row>
+    <row r="99" spans="8:8">
+      <c r="H99" s="15"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0"/>

</xml_diff>

<commit_message>
Added a missing specification about forwarding thread resources.  Associated outputs were added to the design spreadsheet and a test expanded to test the functionality.  The tests all passed, which implies that the implementation was already correct.
</commit_message>
<xml_diff>
--- a/docs/RuntimeDesign.xlsx
+++ b/docs/RuntimeDesign.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jared/Projects/OrchestrationRuntime/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAC11267-6030-1E4B-805A-60F78B4EA177}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A155357C-8A01-0C44-B1EF-1D58B077B103}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="17560" xr2:uid="{9B8D0C4A-3FF1-A04E-B8F8-B86CE3BC2D78}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="846" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="854" uniqueCount="142">
   <si>
     <t>Machine Mode</t>
   </si>
@@ -212,9 +212,6 @@
     <t>any W</t>
   </si>
   <si>
-    <t>Notes</t>
-  </si>
-  <si>
     <t>Current State</t>
   </si>
   <si>
@@ -780,9 +777,6 @@
     </r>
   </si>
   <si>
-    <t>Satisfaction of Req proven</t>
-  </si>
-  <si>
     <t>N_Q &gt; 0</t>
   </si>
   <si>
@@ -863,15 +857,55 @@
   </si>
   <si>
     <r>
+      <t xml:space="preserve">Set N_to_activate = i and emit </t>
+    </r>
+    <r>
       <rPr>
         <b/>
+        <sz val="12"/>
+        <color theme="8" tint="-0.249977111117893"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t xml:space="preserve">activateThread </t>
+    </r>
+    <r>
+      <rPr>
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Throw error</t>
+      <t>event i times</t>
+    </r>
+  </si>
+  <si>
+    <t>N Idle</t>
+  </si>
+  <si>
+    <t>N_Q &gt;= 0</t>
+  </si>
+  <si>
+    <t>N_Q</t>
+  </si>
+  <si>
+    <t>N_Q-1 &gt;= 0</t>
+  </si>
+  <si>
+    <t>i &gt; 0 and i &gt; N_i</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Enqueue given unit of work W and emit </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="8" tint="-0.249977111117893"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>transitionThread</t>
     </r>
     <r>
       <rPr>
@@ -881,12 +915,21 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> - By requirement</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Set N_to_activate = i and emit </t>
+      <t xml:space="preserve"> once</t>
+    </r>
+  </si>
+  <si>
+    <t>N_Q+1 &gt; 0</t>
+  </si>
+  <si>
+    <t>N_Q &gt; 1</t>
+  </si>
+  <si>
+    <t>N_Q-1 &gt; 0</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Emit </t>
     </r>
     <r>
       <rPr>
@@ -905,36 +948,16 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>event i times</t>
-    </r>
-  </si>
-  <si>
-    <t>N Idle</t>
-  </si>
-  <si>
-    <t>N_Q &gt;= 0</t>
-  </si>
-  <si>
-    <t>N_Q</t>
-  </si>
-  <si>
-    <t>N_Q-1 &gt;= 0</t>
-  </si>
-  <si>
-    <t>i &gt; 0 and i &gt; N_i</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Enqueue given unit of work W and emit </t>
+      <t xml:space="preserve">event min(i, N_Q) times and if i &gt; N_Q call </t>
     </r>
     <r>
       <rPr>
         <b/>
         <sz val="12"/>
-        <color theme="8" tint="-0.249977111117893"/>
+        <color theme="9" tint="-0.249977111117893"/>
         <rFont val="Calibri (Body)_x0000_"/>
       </rPr>
-      <t>transitionThread</t>
+      <t>increaseThreadCount(i - N_Q)</t>
     </r>
     <r>
       <rPr>
@@ -944,49 +967,20 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> once</t>
-    </r>
-  </si>
-  <si>
-    <t>N_Q+1 &gt; 0</t>
-  </si>
-  <si>
-    <t>N_Q &gt; 1</t>
-  </si>
-  <si>
-    <t>N_Q-1 &gt; 0</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Emit </t>
-    </r>
+      <t xml:space="preserve"> of ThreadSubscriber if exists</t>
+    </r>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
-        <sz val="12"/>
-        <color theme="8" tint="-0.249977111117893"/>
-        <rFont val="Calibri (Body)_x0000_"/>
-      </rPr>
-      <t xml:space="preserve">activateThread </t>
-    </r>
-    <r>
-      <rPr>
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">event min(i, N_Q) times and if i &gt; N_Q call </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="9" tint="-0.249977111117893"/>
-        <rFont val="Calibri (Body)_x0000_"/>
-      </rPr>
-      <t>increaseThreadCount(i - N_Q)</t>
+      <t xml:space="preserve">Throw error </t>
     </r>
     <r>
       <rPr>
@@ -996,20 +990,76 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> of ThreadSubscriber if exists</t>
-    </r>
-  </si>
-  <si>
+      <t>- there should be no pending work</t>
+    </r>
+  </si>
+  <si>
+    <t>N_c-1 &gt; 0</t>
+  </si>
+  <si>
+    <t>N_w &gt; 1</t>
+  </si>
+  <si>
+    <t>N_w-1 &gt;= 1</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Broadcast </t>
+    </r>
     <r>
       <rPr>
         <b/>
+        <sz val="12"/>
+        <color theme="8" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>unblock</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="8" tint="-0.249977111117893"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>WaitThread</t>
+    </r>
+    <r>
+      <rPr>
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">Throw error </t>
+      <t xml:space="preserve"> signal to wake all threads that called wait() if any</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Broadcast </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="8" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>unblock</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="8" tint="-0.249977111117893"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t xml:space="preserve">WaitThread </t>
     </r>
     <r>
       <rPr>
@@ -1019,32 +1069,12 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>- there should be no pending work</t>
-    </r>
-  </si>
-  <si>
-    <t>N_c-1 &gt; 0</t>
-  </si>
-  <si>
-    <t>N_w &gt; 1</t>
-  </si>
-  <si>
-    <t>N_w-1 &gt;= 1</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Broadcast </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="8" tint="-0.249977111117893"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>unblock</t>
+      <t>signal to wake all threads that called wait() if any</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Transition Mode and then broadcast to all waiting threads the </t>
     </r>
     <r>
       <rPr>
@@ -1053,7 +1083,7 @@
         <color theme="8" tint="-0.249977111117893"/>
         <rFont val="Calibri (Body)_x0000_"/>
       </rPr>
-      <t>WaitThread</t>
+      <t>transitionThread</t>
     </r>
     <r>
       <rPr>
@@ -1063,23 +1093,21 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> signal to wake all threads that called wait() if any</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Broadcast </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="8" tint="-0.249977111117893"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>unblock</t>
+      <t xml:space="preserve"> signal</t>
+    </r>
+  </si>
+  <si>
+    <t>0 &lt; N_i &lt; N_max</t>
+  </si>
+  <si>
+    <t>0 &lt;= N_i &lt; N_max</t>
+  </si>
+  <si>
+    <t>N_i+1 &lt; N_max</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Increment N_to_activate by i and emit </t>
     </r>
     <r>
       <rPr>
@@ -1088,7 +1116,7 @@
         <color theme="8" tint="-0.249977111117893"/>
         <rFont val="Calibri (Body)_x0000_"/>
       </rPr>
-      <t xml:space="preserve">WaitThread </t>
+      <t>activateThread</t>
     </r>
     <r>
       <rPr>
@@ -1098,21 +1126,75 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>signal to wake all threads that called wait() if any</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Transition Mode and then broadcast to all waiting threads the </t>
+      <t xml:space="preserve"> event i times</t>
+    </r>
+  </si>
+  <si>
+    <t>Test name</t>
+  </si>
+  <si>
+    <t>TestInitialState</t>
+  </si>
+  <si>
+    <t>Internally</t>
+  </si>
+  <si>
+    <t>TestNoWorkNoThreads</t>
+  </si>
+  <si>
+    <t>TestIdleErrors</t>
+  </si>
+  <si>
+    <t>Many</t>
+  </si>
+  <si>
+    <t>TestIdleForwardsThreads</t>
+  </si>
+  <si>
+    <t>TestNoWork</t>
+  </si>
+  <si>
+    <t>TestRunningOpenErrors</t>
+  </si>
+  <si>
+    <t>TestRunningOpenIncreaseThreads</t>
+  </si>
+  <si>
+    <t>Nothing to test</t>
+  </si>
+  <si>
+    <t>TestRunningOpenEnqueue</t>
+  </si>
+  <si>
+    <t>TestRunningClosedErrors</t>
+  </si>
+  <si>
+    <t>TestRunningNoMoreWorkErrors</t>
+  </si>
+  <si>
+    <t>TestRunningClosedActivation</t>
+  </si>
+  <si>
+    <t>TestRunningClosedWorkPub</t>
+  </si>
+  <si>
+    <t>TestRunningNoMoreWorkForward</t>
+  </si>
+  <si>
+    <t>Do not know how to test directly</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Call </t>
     </r>
     <r>
       <rPr>
         <b/>
         <sz val="12"/>
-        <color theme="8" tint="-0.249977111117893"/>
+        <color theme="9" tint="-0.249977111117893"/>
         <rFont val="Calibri (Body)_x0000_"/>
       </rPr>
-      <t>transitionThread</t>
+      <t>increaseThreadCount</t>
     </r>
     <r>
       <rPr>
@@ -1122,54 +1204,35 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> signal</t>
-    </r>
-  </si>
-  <si>
-    <t>0 &lt; N_i &lt; N_max</t>
-  </si>
-  <si>
-    <t>0 &lt;= N_i &lt; N_max</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">We are assuming that any threads that are Waiting have yet to receive the </t>
-    </r>
+      <t>(i) of Thread Subscriber if exists</t>
+    </r>
+  </si>
+  <si>
+    <t>TestRunningNoMoreWorkTransition</t>
+  </si>
+  <si>
+    <t>N_i &lt; N_max-1</t>
+  </si>
+  <si>
+    <t>N_i = N_max</t>
+  </si>
+  <si>
+    <t>THIS WOULD LEAD TO DEADLOCK.  Not allowed by specifications.</t>
+  </si>
+  <si>
+    <t>THIS WOULD LEAD TO THREAD RESOURCE LOSS!  Not allowed by specifications.</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
-        <sz val="12"/>
-        <color theme="8" tint="-0.249977111117893"/>
-        <rFont val="Calibri (Body)_x0000_"/>
-      </rPr>
-      <t>transitionThread</t>
-    </r>
-    <r>
-      <rPr>
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> signal, but will.</t>
-    </r>
-  </si>
-  <si>
-    <t>N_i+1 &lt; N_max</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Increment N_to_activate by i and emit </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="8" tint="-0.249977111117893"/>
-        <rFont val="Calibri (Body)_x0000_"/>
-      </rPr>
-      <t>activateThread</t>
+      <t>IMPOSSIBLE:</t>
     </r>
     <r>
       <rPr>
@@ -1179,113 +1242,41 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> event i times</t>
-    </r>
-  </si>
-  <si>
-    <t>Test name</t>
-  </si>
-  <si>
-    <t>TestInitialState</t>
-  </si>
-  <si>
-    <t>Internally</t>
-  </si>
-  <si>
-    <t>TestNoWorkNoThreads</t>
-  </si>
-  <si>
-    <t>TestIdleErrors</t>
-  </si>
-  <si>
-    <t>Many</t>
-  </si>
-  <si>
-    <t>TestIdleForwardsThreads</t>
-  </si>
-  <si>
-    <t>TestNoWork</t>
-  </si>
-  <si>
-    <t>TestRunningOpenErrors</t>
-  </si>
-  <si>
-    <t>TestRunningOpenIncreaseThreads</t>
-  </si>
-  <si>
-    <t>Nothing to test</t>
-  </si>
-  <si>
-    <t>TestRunningOpenEnqueue</t>
-  </si>
-  <si>
-    <t>TestRunningClosedErrors</t>
-  </si>
-  <si>
-    <t>TestRunningNoMoreWorkErrors</t>
-  </si>
-  <si>
-    <t>TestRunningClosedActivation</t>
-  </si>
-  <si>
-    <t>TestRunningClosedWorkPub</t>
-  </si>
-  <si>
-    <t>TestRunningNoMoreWorkForward</t>
-  </si>
-  <si>
-    <t>Do not know how to test directly</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Call </t>
-    </r>
+      <t xml:space="preserve"> this event is triggered by a computing thread =&gt; N_c &gt; 0</t>
+    </r>
+  </si>
+  <si>
+    <t>N_c+1 &gt; 0</t>
+  </si>
+  <si>
+    <t>NEED AT LEAST ONE THREAD TO TRANSITION TO IDLE. Not allowed by specifications.</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
-        <sz val="12"/>
-        <color theme="9" tint="-0.249977111117893"/>
-        <rFont val="Calibri (Body)_x0000_"/>
-      </rPr>
-      <t>increaseThreadCount</t>
-    </r>
-    <r>
-      <rPr>
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>(i) of Thread Subscriber if exists</t>
-    </r>
-  </si>
-  <si>
-    <t>TestRunningNoMoreWorkTransition</t>
-  </si>
-  <si>
-    <t>N_i &lt; N_max-1</t>
-  </si>
-  <si>
-    <t>N_i = N_max</t>
-  </si>
-  <si>
-    <t>THIS WOULD LEAD TO DEADLOCK.  Not allowed by specifications.</t>
-  </si>
-  <si>
-    <t>THIS WOULD LEAD TO THREAD RESOURCE LOSS!  Not allowed by specifications.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
+      <t>Throw error</t>
+    </r>
+    <r>
+      <rPr>
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>IMPOSSIBLE:</t>
+      <t xml:space="preserve"> - By specifications</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Throw error -</t>
     </r>
     <r>
       <rPr>
@@ -1295,14 +1286,35 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> this event is triggered by a computing thread =&gt; N_c &gt; 0</t>
-    </r>
-  </si>
-  <si>
-    <t>N_c+1 &gt; 0</t>
-  </si>
-  <si>
-    <t>NEED AT LEAST ONE THREAD TO TRANSITION TO IDLE. Not allowed by specifications.</t>
+      <t xml:space="preserve"> By specifications</t>
+    </r>
+  </si>
+  <si>
+    <t>Not yet tested!</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Call </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>increaseThreadCount</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(1) of Thread Subscriber if exists</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1394,10 +1406,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Menlo"/>
-      <family val="2"/>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri (Body)_x0000_"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1561,7 +1573,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1587,14 +1599,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1632,9 +1638,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1642,9 +1645,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1659,9 +1659,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1687,7 +1689,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2004,11 +2030,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98772F20-44FC-FE45-839B-70D0417F8C61}">
-  <dimension ref="A1:Q99"/>
+  <dimension ref="A1:Q105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O92" sqref="O92"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P96" sqref="P96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2027,71 +2053,71 @@
     <col min="12" max="12" width="12.1640625" style="1" customWidth="1"/>
     <col min="13" max="13" width="14.5" style="1" customWidth="1"/>
     <col min="14" max="14" width="11.1640625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="103.33203125" style="3" customWidth="1"/>
-    <col min="16" max="16" width="38.5" style="1" customWidth="1"/>
+    <col min="15" max="15" width="59.5" style="39" customWidth="1"/>
+    <col min="16" max="16" width="31.83203125" style="1" customWidth="1"/>
     <col min="17" max="17" width="99.6640625" style="3" customWidth="1"/>
     <col min="18" max="18" width="72.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="16" customHeight="1">
-      <c r="B1" s="30"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
-      <c r="K1" s="42"/>
-      <c r="L1" s="42"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
     </row>
     <row r="2" spans="1:17" ht="17" thickBot="1">
-      <c r="B2" s="30"/>
+      <c r="B2" s="26"/>
     </row>
     <row r="3" spans="1:17" ht="17" thickBot="1">
-      <c r="B3" s="30"/>
-      <c r="C3" s="35" t="s">
+      <c r="B3" s="26"/>
+      <c r="C3" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="34"/>
+      <c r="J3" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="38"/>
-      <c r="J3" s="35" t="s">
-        <v>37</v>
-      </c>
-      <c r="K3" s="36"/>
-      <c r="L3" s="36"/>
-      <c r="M3" s="37"/>
-      <c r="N3" s="38"/>
+      <c r="K3" s="32"/>
+      <c r="L3" s="32"/>
+      <c r="M3" s="33"/>
+      <c r="N3" s="34"/>
     </row>
     <row r="4" spans="1:17" ht="17" thickBot="1">
-      <c r="B4" s="30"/>
+      <c r="B4" s="26"/>
       <c r="C4" s="5"/>
-      <c r="D4" s="39" t="s">
+      <c r="D4" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="41"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="37"/>
       <c r="J4" s="5"/>
-      <c r="K4" s="39" t="s">
+      <c r="K4" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="L4" s="40"/>
-      <c r="M4" s="40"/>
-      <c r="N4" s="41"/>
-    </row>
-    <row r="5" spans="1:17" ht="17" thickBot="1">
-      <c r="B5" s="30"/>
+      <c r="L4" s="36"/>
+      <c r="M4" s="36"/>
+      <c r="N4" s="37"/>
+    </row>
+    <row r="5" spans="1:17" ht="18" thickBot="1">
+      <c r="B5" s="26"/>
       <c r="C5" s="5" t="s">
         <v>0</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="E5" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="E5" s="9" t="s">
         <v>13</v>
       </c>
       <c r="F5" s="8" t="s">
@@ -2110,9 +2136,9 @@
         <v>0</v>
       </c>
       <c r="K5" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="L5" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="L5" s="9" t="s">
         <v>13</v>
       </c>
       <c r="M5" s="8" t="s">
@@ -2121,66 +2147,64 @@
       <c r="N5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="O5" s="9" t="s">
+      <c r="O5" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="P5" s="23" t="s">
-        <v>115</v>
-      </c>
-      <c r="Q5" s="12" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17">
-      <c r="B6" s="29" t="s">
+      <c r="P5" s="46" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q5" s="10"/>
+    </row>
+    <row r="6" spans="1:17" ht="17">
+      <c r="B6" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="21">
+        <v>0</v>
+      </c>
+      <c r="F6" s="21">
+        <v>0</v>
+      </c>
+      <c r="G6" s="21">
+        <v>0</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="O6" s="41" t="s">
         <v>82</v>
       </c>
-      <c r="C6" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="23" t="s">
-        <v>39</v>
-      </c>
-      <c r="E6" s="23">
-        <v>0</v>
-      </c>
-      <c r="F6" s="23">
-        <v>0</v>
-      </c>
-      <c r="G6" s="23">
-        <v>0</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="O6" s="24" t="s">
-        <v>83</v>
-      </c>
-      <c r="P6" s="28" t="s">
-        <v>116</v>
-      </c>
-      <c r="Q6" s="12"/>
-    </row>
-    <row r="7" spans="1:17">
-      <c r="B7" s="21"/>
+      <c r="P6" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q6" s="10"/>
+    </row>
+    <row r="7" spans="1:17" ht="17">
+      <c r="B7" s="19"/>
       <c r="C7" s="1" t="s">
         <v>4</v>
       </c>
@@ -2194,7 +2218,7 @@
         <v>27</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>27</v>
@@ -2217,18 +2241,15 @@
       <c r="N7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="O7" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="P7" s="15" t="s">
-        <v>117</v>
-      </c>
-      <c r="Q7" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17">
-      <c r="B8" s="21"/>
+      <c r="O7" s="42" t="s">
+        <v>138</v>
+      </c>
+      <c r="P7" s="13" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="17">
+      <c r="B8" s="19"/>
       <c r="C8" s="1" t="s">
         <v>4</v>
       </c>
@@ -2265,24 +2286,22 @@
       <c r="N8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="O8" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="P8" s="15" t="s">
-        <v>117</v>
-      </c>
-      <c r="Q8" s="13" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17">
+      <c r="O8" s="45" t="s">
+        <v>139</v>
+      </c>
+      <c r="P8" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q8" s="11"/>
+    </row>
+    <row r="9" spans="1:17" ht="17">
       <c r="A9" s="2"/>
-      <c r="B9" s="19"/>
+      <c r="B9" s="17"/>
       <c r="C9" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E9" s="1">
         <v>0</v>
@@ -2293,7 +2312,7 @@
       <c r="G9" s="1">
         <v>0</v>
       </c>
-      <c r="H9" s="16" t="s">
+      <c r="H9" s="14" t="s">
         <v>9</v>
       </c>
       <c r="I9" s="1" t="s">
@@ -2314,20 +2333,20 @@
       <c r="N9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="O9" s="3" t="s">
+      <c r="O9" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="P9" s="28" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17">
-      <c r="B10" s="18"/>
+      <c r="P9" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="17">
+      <c r="B10" s="16"/>
       <c r="C10" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E10" s="1">
         <v>0</v>
@@ -2338,17 +2357,17 @@
       <c r="G10" s="1">
         <v>0</v>
       </c>
-      <c r="H10" s="16" t="s">
+      <c r="H10" s="14" t="s">
         <v>9</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>5</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L10" s="1">
         <v>0</v>
@@ -2359,20 +2378,20 @@
       <c r="N10" s="1">
         <v>0</v>
       </c>
-      <c r="O10" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="P10" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17">
-      <c r="B11" s="18"/>
+      <c r="O10" s="39" t="s">
+        <v>89</v>
+      </c>
+      <c r="P10" s="13" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" ht="17">
+      <c r="B11" s="16"/>
       <c r="C11" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E11" s="1">
         <v>0</v>
@@ -2383,7 +2402,7 @@
       <c r="G11" s="1">
         <v>0</v>
       </c>
-      <c r="H11" s="16" t="s">
+      <c r="H11" s="14" t="s">
         <v>11</v>
       </c>
       <c r="I11" s="1" t="s">
@@ -2404,21 +2423,21 @@
       <c r="N11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="O11" s="13" t="s">
+      <c r="O11" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="P11" s="28" t="s">
-        <v>119</v>
-      </c>
-      <c r="Q11" s="13"/>
-    </row>
-    <row r="12" spans="1:17">
-      <c r="B12" s="18"/>
+      <c r="P11" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q11" s="11"/>
+    </row>
+    <row r="12" spans="1:17" ht="17">
+      <c r="B12" s="16"/>
       <c r="C12" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E12" s="1">
         <v>0</v>
@@ -2429,7 +2448,7 @@
       <c r="G12" s="1">
         <v>0</v>
       </c>
-      <c r="H12" s="16" t="s">
+      <c r="H12" s="14" t="s">
         <v>11</v>
       </c>
       <c r="I12" s="1" t="s">
@@ -2450,21 +2469,21 @@
       <c r="N12" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="O12" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="P12" s="28" t="s">
-        <v>119</v>
-      </c>
-      <c r="Q12" s="13"/>
-    </row>
-    <row r="13" spans="1:17">
-      <c r="B13" s="22"/>
+      <c r="O12" s="39" t="s">
+        <v>88</v>
+      </c>
+      <c r="P12" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q12" s="11"/>
+    </row>
+    <row r="13" spans="1:17" ht="17">
+      <c r="B13" s="20"/>
       <c r="C13" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E13" s="1">
         <v>0</v>
@@ -2475,7 +2494,7 @@
       <c r="G13" s="1">
         <v>0</v>
       </c>
-      <c r="H13" s="16" t="s">
+      <c r="H13" s="14" t="s">
         <v>11</v>
       </c>
       <c r="I13" s="1" t="s">
@@ -2485,7 +2504,7 @@
         <v>4</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L13" s="1">
         <v>0</v>
@@ -2496,20 +2515,20 @@
       <c r="N13" s="1">
         <v>0</v>
       </c>
-      <c r="O13" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="P13" s="28" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17">
-      <c r="B14" s="22"/>
+      <c r="O13" s="39" t="s">
+        <v>64</v>
+      </c>
+      <c r="P13" s="4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="17">
+      <c r="B14" s="20"/>
       <c r="C14" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E14" s="1">
         <v>0</v>
@@ -2520,7 +2539,7 @@
       <c r="G14" s="1">
         <v>0</v>
       </c>
-      <c r="H14" s="16" t="s">
+      <c r="H14" s="14" t="s">
         <v>22</v>
       </c>
       <c r="I14" s="1" t="s">
@@ -2541,21 +2560,21 @@
       <c r="N14" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="O14" s="3" t="s">
+      <c r="O14" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="P14" s="28" t="s">
-        <v>119</v>
-      </c>
-      <c r="Q14" s="13"/>
-    </row>
-    <row r="15" spans="1:17">
-      <c r="B15" s="22"/>
+      <c r="P14" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q14" s="11"/>
+    </row>
+    <row r="15" spans="1:17" ht="17">
+      <c r="B15" s="20"/>
       <c r="C15" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E15" s="1">
         <v>0</v>
@@ -2566,7 +2585,7 @@
       <c r="G15" s="1">
         <v>0</v>
       </c>
-      <c r="H15" s="16" t="s">
+      <c r="H15" s="14" t="s">
         <v>28</v>
       </c>
       <c r="I15" s="1" t="s">
@@ -2587,20 +2606,20 @@
       <c r="N15" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="O15" s="3" t="s">
+      <c r="O15" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="P15" s="28" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17">
-      <c r="B16" s="22"/>
+      <c r="P15" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" ht="34">
+      <c r="B16" s="20"/>
       <c r="C16" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E16" s="1">
         <v>0</v>
@@ -2611,7 +2630,7 @@
       <c r="G16" s="1">
         <v>0</v>
       </c>
-      <c r="H16" s="14" t="s">
+      <c r="H16" s="12" t="s">
         <v>7</v>
       </c>
       <c r="I16" s="1" t="s">
@@ -2621,7 +2640,7 @@
         <v>4</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L16" s="1">
         <v>0</v>
@@ -2632,20 +2651,20 @@
       <c r="N16" s="1">
         <v>0</v>
       </c>
-      <c r="O16" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="P16" s="31" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="17" spans="2:17">
-      <c r="B17" s="22"/>
+      <c r="O16" s="39" t="s">
+        <v>84</v>
+      </c>
+      <c r="P16" s="27" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="17" spans="2:17" ht="17">
+      <c r="B17" s="20"/>
       <c r="C17" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E17" s="1">
         <v>0</v>
@@ -2656,8 +2675,8 @@
       <c r="G17" s="1">
         <v>0</v>
       </c>
-      <c r="H17" s="14" t="s">
-        <v>54</v>
+      <c r="H17" s="12" t="s">
+        <v>53</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>8</v>
@@ -2666,7 +2685,7 @@
         <v>4</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L17" s="1">
         <v>0</v>
@@ -2677,20 +2696,20 @@
       <c r="N17" s="1">
         <v>0</v>
       </c>
-      <c r="O17" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="P17" s="31" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="18" spans="2:17">
-      <c r="B18" s="22"/>
+      <c r="O17" s="39" t="s">
+        <v>85</v>
+      </c>
+      <c r="P17" s="27" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="18" spans="2:17" ht="17">
+      <c r="B18" s="20"/>
       <c r="C18" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E18" s="1">
         <v>0</v>
@@ -2701,8 +2720,8 @@
       <c r="G18" s="1">
         <v>0</v>
       </c>
-      <c r="H18" s="14" t="s">
-        <v>88</v>
+      <c r="H18" s="12" t="s">
+        <v>86</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>8</v>
@@ -2711,7 +2730,7 @@
         <v>4</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L18" s="1">
         <v>0</v>
@@ -2722,16 +2741,16 @@
       <c r="N18" s="1">
         <v>0</v>
       </c>
-      <c r="O18" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="P18" s="31" t="s">
-        <v>132</v>
-      </c>
-      <c r="Q18" s="13"/>
-    </row>
-    <row r="19" spans="2:17">
-      <c r="B19" s="18"/>
+      <c r="O18" s="39" t="s">
+        <v>85</v>
+      </c>
+      <c r="P18" s="27" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q18" s="11"/>
+    </row>
+    <row r="19" spans="2:17" ht="17">
+      <c r="B19" s="16"/>
       <c r="C19" s="1" t="s">
         <v>5</v>
       </c>
@@ -2747,7 +2766,7 @@
       <c r="G19" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H19" s="16" t="s">
+      <c r="H19" s="14" t="s">
         <v>9</v>
       </c>
       <c r="I19" s="4" t="s">
@@ -2768,15 +2787,15 @@
       <c r="N19" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="O19" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="P19" s="28" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="20" spans="2:17">
-      <c r="B20" s="18"/>
+      <c r="O19" s="39" t="s">
+        <v>45</v>
+      </c>
+      <c r="P19" s="4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="20" spans="2:17" ht="17">
+      <c r="B20" s="16"/>
       <c r="C20" s="1" t="s">
         <v>5</v>
       </c>
@@ -2792,7 +2811,7 @@
       <c r="G20" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H20" s="16" t="s">
+      <c r="H20" s="14" t="s">
         <v>11</v>
       </c>
       <c r="I20" s="1" t="s">
@@ -2813,15 +2832,15 @@
       <c r="N20" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="O20" s="3" t="s">
+      <c r="O20" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="P20" s="28" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="21" spans="2:17">
-      <c r="B21" s="18"/>
+      <c r="P20" s="4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="21" spans="2:17" ht="17">
+      <c r="B21" s="16"/>
       <c r="C21" s="1" t="s">
         <v>5</v>
       </c>
@@ -2837,11 +2856,11 @@
       <c r="G21" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H21" s="16" t="s">
+      <c r="H21" s="14" t="s">
         <v>11</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="J21" s="1" t="s">
         <v>8</v>
@@ -2858,15 +2877,15 @@
       <c r="N21" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="O21" s="3" t="s">
+      <c r="O21" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="P21" s="28" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="22" spans="2:17">
-      <c r="B22" s="18"/>
+      <c r="P21" s="4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="22" spans="2:17" ht="34">
+      <c r="B22" s="16"/>
       <c r="C22" s="1" t="s">
         <v>5</v>
       </c>
@@ -2880,38 +2899,38 @@
         <v>18</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="H22" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="H22" s="14" t="s">
         <v>11</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J22" s="1" t="s">
         <v>5</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="O22" s="13" t="s">
-        <v>114</v>
-      </c>
-      <c r="P22" s="28" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="23" spans="2:17">
-      <c r="B23" s="18"/>
+        <v>92</v>
+      </c>
+      <c r="O22" s="39" t="s">
+        <v>110</v>
+      </c>
+      <c r="P22" s="4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="23" spans="2:17" ht="17">
+      <c r="B23" s="16"/>
       <c r="C23" s="1" t="s">
         <v>5</v>
       </c>
@@ -2925,9 +2944,9 @@
         <v>18</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="H23" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="H23" s="14" t="s">
         <v>22</v>
       </c>
       <c r="I23" s="4" t="s">
@@ -2937,31 +2956,31 @@
         <v>5</v>
       </c>
       <c r="K23" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L23" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M23" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N23" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="O23" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="P23" s="28" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="24" spans="2:17">
-      <c r="B24" s="18"/>
+        <v>96</v>
+      </c>
+      <c r="O23" s="42" t="s">
+        <v>95</v>
+      </c>
+      <c r="P23" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="24" spans="2:17" ht="17">
+      <c r="B24" s="16"/>
       <c r="C24" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E24" s="1">
         <v>0</v>
@@ -2972,7 +2991,7 @@
       <c r="G24" s="1">
         <v>0</v>
       </c>
-      <c r="H24" s="16" t="s">
+      <c r="H24" s="14" t="s">
         <v>28</v>
       </c>
       <c r="I24" s="4" t="s">
@@ -2982,7 +3001,7 @@
         <v>4</v>
       </c>
       <c r="K24" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L24" s="4">
         <v>0</v>
@@ -2993,21 +3012,21 @@
       <c r="N24" s="4">
         <v>0</v>
       </c>
-      <c r="O24" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="P24" s="28" t="s">
-        <v>118</v>
-      </c>
-      <c r="Q24" s="13"/>
-    </row>
-    <row r="25" spans="2:17">
-      <c r="B25" s="18"/>
+      <c r="O24" s="42" t="s">
+        <v>62</v>
+      </c>
+      <c r="P24" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q24" s="11"/>
+    </row>
+    <row r="25" spans="2:17" ht="34">
+      <c r="B25" s="16"/>
       <c r="C25" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>17</v>
@@ -3018,36 +3037,36 @@
       <c r="G25" s="1">
         <v>0</v>
       </c>
-      <c r="H25" s="16" t="s">
+      <c r="H25" s="14" t="s">
         <v>28</v>
       </c>
       <c r="I25" s="4" t="s">
         <v>8</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K25" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L25" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M25" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N25" s="4">
         <v>0</v>
       </c>
-      <c r="O25" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="P25" s="28" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="26" spans="2:17">
-      <c r="B26" s="18"/>
+      <c r="O25" s="42" t="s">
+        <v>106</v>
+      </c>
+      <c r="P25" s="4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="26" spans="2:17" ht="17">
+      <c r="B26" s="16"/>
       <c r="C26" s="1" t="s">
         <v>5</v>
       </c>
@@ -3061,39 +3080,39 @@
         <v>18</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="H26" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="H26" s="14" t="s">
         <v>28</v>
       </c>
       <c r="I26" s="4" t="s">
         <v>8</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K26" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L26" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M26" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N26" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="O26" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="O26" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="P26" s="15" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q26" s="13"/>
-    </row>
-    <row r="27" spans="2:17">
-      <c r="B27" s="18"/>
+      <c r="P26" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q26" s="11"/>
+    </row>
+    <row r="27" spans="2:17" ht="34">
+      <c r="B27" s="16"/>
       <c r="C27" s="1" t="s">
         <v>5</v>
       </c>
@@ -3109,7 +3128,7 @@
       <c r="G27" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H27" s="14" t="s">
+      <c r="H27" s="12" t="s">
         <v>7</v>
       </c>
       <c r="I27" s="1" t="s">
@@ -3130,15 +3149,15 @@
       <c r="N27" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="O27" s="34" t="s">
-        <v>138</v>
-      </c>
-      <c r="P27" s="31" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="28" spans="2:17">
-      <c r="B28" s="18"/>
+      <c r="O27" s="43" t="s">
+        <v>134</v>
+      </c>
+      <c r="P27" s="27" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="28" spans="2:17" ht="17">
+      <c r="B28" s="16"/>
       <c r="C28" s="1" t="s">
         <v>5</v>
       </c>
@@ -3154,7 +3173,7 @@
       <c r="G28" s="1">
         <v>0</v>
       </c>
-      <c r="H28" s="14" t="s">
+      <c r="H28" s="12" t="s">
         <v>7</v>
       </c>
       <c r="I28" s="1" t="s">
@@ -3164,26 +3183,26 @@
         <v>5</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L28" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="M28" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="N28" s="1">
+        <v>0</v>
+      </c>
+      <c r="O28" s="39" t="s">
         <v>51</v>
       </c>
-      <c r="M28" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="N28" s="1">
-        <v>0</v>
-      </c>
-      <c r="O28" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="P28" s="28" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="29" spans="2:17">
-      <c r="B29" s="18"/>
+      <c r="P28" s="4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="29" spans="2:17" ht="17">
+      <c r="B29" s="16"/>
       <c r="C29" s="1" t="s">
         <v>5</v>
       </c>
@@ -3197,9 +3216,9 @@
         <v>18</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="H29" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="H29" s="12" t="s">
         <v>7</v>
       </c>
       <c r="I29" s="1" t="s">
@@ -3209,35 +3228,35 @@
         <v>5</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L29" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M29" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N29" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="O29" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="P29" s="28" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="30" spans="2:17">
-      <c r="B30" s="20"/>
-      <c r="O30" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="P30" s="28" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="31" spans="2:17">
-      <c r="B31" s="18"/>
+        <v>93</v>
+      </c>
+      <c r="O29" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="P29" s="4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="30" spans="2:17" ht="34">
+      <c r="B30" s="18"/>
+      <c r="O30" s="39" t="s">
+        <v>56</v>
+      </c>
+      <c r="P30" s="4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="31" spans="2:17" ht="17">
+      <c r="B31" s="16"/>
       <c r="C31" s="1" t="s">
         <v>5</v>
       </c>
@@ -3251,10 +3270,10 @@
         <v>18</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="H31" s="14" t="s">
-        <v>54</v>
+        <v>91</v>
+      </c>
+      <c r="H31" s="12" t="s">
+        <v>53</v>
       </c>
       <c r="I31" s="1" t="s">
         <v>8</v>
@@ -3263,26 +3282,26 @@
         <v>5</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L31" s="1">
         <v>0</v>
       </c>
       <c r="M31" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N31" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="O31" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="O31" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="P31" s="1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="32" spans="2:17">
-      <c r="B32" s="18"/>
+      <c r="P31" s="13" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="32" spans="2:17" ht="17">
+      <c r="B32" s="16"/>
       <c r="C32" s="1" t="s">
         <v>5</v>
       </c>
@@ -3298,8 +3317,8 @@
       <c r="G32" s="1">
         <v>0</v>
       </c>
-      <c r="H32" s="14" t="s">
-        <v>54</v>
+      <c r="H32" s="12" t="s">
+        <v>53</v>
       </c>
       <c r="I32" s="1" t="s">
         <v>8</v>
@@ -3308,26 +3327,26 @@
         <v>5</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L32" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M32" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N32" s="1">
         <v>0</v>
       </c>
-      <c r="O32" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="P32" s="31" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="33" spans="1:17">
-      <c r="B33" s="18"/>
+      <c r="O32" s="39" t="s">
+        <v>59</v>
+      </c>
+      <c r="P32" s="27" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" ht="17">
+      <c r="B33" s="16"/>
       <c r="C33" s="1" t="s">
         <v>5</v>
       </c>
@@ -3341,10 +3360,10 @@
         <v>18</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="H33" s="14" t="s">
-        <v>54</v>
+        <v>83</v>
+      </c>
+      <c r="H33" s="12" t="s">
+        <v>53</v>
       </c>
       <c r="I33" s="1" t="s">
         <v>8</v>
@@ -3353,36 +3372,36 @@
         <v>5</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L33" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M33" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N33" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="O33" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="O33" s="39" t="s">
+        <v>66</v>
+      </c>
+      <c r="P33" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" ht="34">
+      <c r="B34" s="18"/>
+      <c r="H34" s="12"/>
+      <c r="O34" s="39" t="s">
         <v>67</v>
       </c>
-      <c r="P33" s="28" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="34" spans="1:17">
-      <c r="B34" s="20"/>
-      <c r="H34" s="14"/>
-      <c r="O34" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="P34" s="28" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="35" spans="1:17">
-      <c r="B35" s="18"/>
+      <c r="P34" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" ht="34">
+      <c r="B35" s="16"/>
       <c r="C35" s="1" t="s">
         <v>5</v>
       </c>
@@ -3398,8 +3417,8 @@
       <c r="G35" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H35" s="14" t="s">
-        <v>88</v>
+      <c r="H35" s="12" t="s">
+        <v>86</v>
       </c>
       <c r="I35" s="1" t="s">
         <v>8</v>
@@ -3419,15 +3438,15 @@
       <c r="N35" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="O35" s="32" t="s">
-        <v>139</v>
-      </c>
-      <c r="P35" s="1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="36" spans="1:17">
-      <c r="B36" s="18"/>
+      <c r="O35" s="39" t="s">
+        <v>135</v>
+      </c>
+      <c r="P35" s="13" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" ht="34">
+      <c r="B36" s="16"/>
       <c r="C36" s="1" t="s">
         <v>5</v>
       </c>
@@ -3443,8 +3462,8 @@
       <c r="G36" s="1">
         <v>0</v>
       </c>
-      <c r="H36" s="14" t="s">
-        <v>88</v>
+      <c r="H36" s="12" t="s">
+        <v>86</v>
       </c>
       <c r="I36" s="1" t="s">
         <v>8</v>
@@ -3453,37 +3472,37 @@
         <v>5</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L36" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M36" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N36" s="1">
         <v>0</v>
       </c>
-      <c r="O36" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="P36" s="28" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="37" spans="1:17">
-      <c r="A37" s="13"/>
-      <c r="B37" s="20"/>
-      <c r="H37" s="17"/>
-      <c r="O37" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="P37" s="28" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="38" spans="1:17">
-      <c r="B38" s="18"/>
+      <c r="O36" s="39" t="s">
+        <v>63</v>
+      </c>
+      <c r="P36" s="47" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" ht="17">
+      <c r="A37" s="11"/>
+      <c r="B37" s="18"/>
+      <c r="H37" s="15"/>
+      <c r="O37" s="39" t="s">
+        <v>59</v>
+      </c>
+      <c r="P37" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" ht="34">
+      <c r="B38" s="16"/>
       <c r="C38" s="1" t="s">
         <v>5</v>
       </c>
@@ -3497,10 +3516,10 @@
         <v>32</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="H38" s="14" t="s">
-        <v>88</v>
+        <v>83</v>
+      </c>
+      <c r="H38" s="12" t="s">
+        <v>86</v>
       </c>
       <c r="I38" s="1" t="s">
         <v>8</v>
@@ -3509,48 +3528,48 @@
         <v>5</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L38" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M38" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N38" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="O38" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="O38" s="39" t="s">
+        <v>68</v>
+      </c>
+      <c r="P38" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" ht="17">
+      <c r="B39" s="18"/>
+      <c r="H39" s="13"/>
+      <c r="O39" s="39" t="s">
         <v>69</v>
       </c>
-      <c r="P38" s="28" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="39" spans="1:17">
-      <c r="B39" s="20"/>
-      <c r="H39" s="15"/>
-      <c r="O39" s="3" t="s">
+      <c r="P39" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" ht="34">
+      <c r="B40" s="18"/>
+      <c r="H40" s="13"/>
+      <c r="O40" s="39" t="s">
         <v>70</v>
       </c>
-      <c r="P39" s="28" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="40" spans="1:17">
-      <c r="B40" s="20"/>
-      <c r="H40" s="15"/>
-      <c r="O40" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="P40" s="28" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="41" spans="1:17">
-      <c r="B41" s="18"/>
+      <c r="P40" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" ht="17">
+      <c r="B41" s="16"/>
       <c r="C41" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>27</v>
@@ -3564,7 +3583,7 @@
       <c r="G41" s="1">
         <v>0</v>
       </c>
-      <c r="H41" s="15" t="s">
+      <c r="H41" s="13" t="s">
         <v>27</v>
       </c>
       <c r="I41" s="1" t="s">
@@ -3585,18 +3604,18 @@
       <c r="N41" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="O41" s="34" t="s">
-        <v>137</v>
-      </c>
-      <c r="P41" s="28" t="s">
-        <v>117</v>
-      </c>
-      <c r="Q41" s="32"/>
-    </row>
-    <row r="42" spans="1:17">
-      <c r="B42" s="18"/>
+      <c r="O41" s="43" t="s">
+        <v>133</v>
+      </c>
+      <c r="P41" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q41" s="28"/>
+    </row>
+    <row r="42" spans="1:17" ht="17">
+      <c r="B42" s="16"/>
       <c r="C42" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>27</v>
@@ -3608,9 +3627,9 @@
         <v>27</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="H42" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="H42" s="14" t="s">
         <v>9</v>
       </c>
       <c r="I42" s="1" t="s">
@@ -3631,17 +3650,17 @@
       <c r="N42" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="O42" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="P42" s="28" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="43" spans="1:17">
-      <c r="B43" s="18"/>
+      <c r="O42" s="39" t="s">
+        <v>45</v>
+      </c>
+      <c r="P42" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" ht="17">
+      <c r="B43" s="16"/>
       <c r="C43" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>27</v>
@@ -3653,9 +3672,9 @@
         <v>27</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="H43" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="H43" s="14" t="s">
         <v>11</v>
       </c>
       <c r="I43" s="1" t="s">
@@ -3676,17 +3695,17 @@
       <c r="N43" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="O43" s="3" t="s">
+      <c r="O43" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="P43" s="28" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="44" spans="1:17">
-      <c r="B44" s="18"/>
+      <c r="P43" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" ht="17">
+      <c r="B44" s="16"/>
       <c r="C44" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>19</v>
@@ -3698,13 +3717,13 @@
         <v>27</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="H44" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="H44" s="14" t="s">
         <v>11</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="J44" s="1" t="s">
         <v>8</v>
@@ -3721,17 +3740,17 @@
       <c r="N44" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="O44" s="3" t="s">
+      <c r="O44" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="P44" s="28" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="45" spans="1:17">
-      <c r="B45" s="18"/>
+      <c r="P44" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" ht="34">
+      <c r="B45" s="16"/>
       <c r="C45" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>19</v>
@@ -3743,40 +3762,40 @@
         <v>18</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="H45" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="H45" s="14" t="s">
         <v>11</v>
       </c>
       <c r="I45" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J45" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="J45" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="K45" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L45" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M45" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N45" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="O45" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="P45" s="28" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="46" spans="1:17">
-      <c r="B46" s="18"/>
+        <v>92</v>
+      </c>
+      <c r="O45" s="39" t="s">
+        <v>99</v>
+      </c>
+      <c r="P45" s="4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" ht="17">
+      <c r="B46" s="16"/>
       <c r="C46" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>27</v>
@@ -3788,9 +3807,9 @@
         <v>27</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="H46" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="H46" s="14" t="s">
         <v>22</v>
       </c>
       <c r="I46" s="1" t="s">
@@ -3811,17 +3830,17 @@
       <c r="N46" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="O46" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="P46" s="28" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="47" spans="1:17">
-      <c r="B47" s="18"/>
+      <c r="O46" s="39" t="s">
+        <v>43</v>
+      </c>
+      <c r="P46" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" ht="17">
+      <c r="B47" s="16"/>
       <c r="C47" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>27</v>
@@ -3833,9 +3852,9 @@
         <v>27</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="H47" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="H47" s="14" t="s">
         <v>28</v>
       </c>
       <c r="I47" s="1" t="s">
@@ -3856,17 +3875,17 @@
       <c r="N47" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="O47" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="P47" s="28" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="48" spans="1:17">
-      <c r="B48" s="18"/>
+      <c r="O47" s="39" t="s">
+        <v>46</v>
+      </c>
+      <c r="P47" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" ht="34">
+      <c r="B48" s="16"/>
       <c r="C48" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D48" s="1">
         <v>0</v>
@@ -3878,9 +3897,9 @@
         <v>27</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="H48" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="H48" s="12" t="s">
         <v>7</v>
       </c>
       <c r="I48" s="1" t="s">
@@ -3901,18 +3920,18 @@
       <c r="N48" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="O48" s="34" t="s">
-        <v>138</v>
-      </c>
-      <c r="P48" s="31" t="s">
-        <v>132</v>
-      </c>
-      <c r="Q48" s="13"/>
-    </row>
-    <row r="49" spans="2:16">
-      <c r="B49" s="18"/>
+      <c r="O48" s="43" t="s">
+        <v>134</v>
+      </c>
+      <c r="P48" s="27" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q48" s="11"/>
+    </row>
+    <row r="49" spans="2:16" ht="17">
+      <c r="B49" s="16"/>
       <c r="C49" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>16</v>
@@ -3926,56 +3945,56 @@
       <c r="G49" s="1">
         <v>1</v>
       </c>
-      <c r="H49" s="14" t="s">
+      <c r="H49" s="12" t="s">
         <v>7</v>
       </c>
       <c r="I49" s="1" t="s">
         <v>8</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K49" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L49" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M49" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N49" s="1">
         <v>0</v>
       </c>
-      <c r="O49" s="3" t="s">
+      <c r="O49" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="P49" s="4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="50" spans="2:16" ht="34">
+      <c r="B50" s="18"/>
+      <c r="O50" s="39" t="s">
+        <v>72</v>
+      </c>
+      <c r="P50" s="4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="51" spans="2:16" ht="34">
+      <c r="B51" s="18"/>
+      <c r="O51" s="39" t="s">
         <v>55</v>
       </c>
-      <c r="P49" s="28" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="50" spans="2:16">
-      <c r="B50" s="20"/>
-      <c r="O50" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="P50" s="31" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="51" spans="2:16">
-      <c r="B51" s="20"/>
-      <c r="O51" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="P51" s="28" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="52" spans="2:16">
-      <c r="B52" s="18"/>
+      <c r="P51" s="4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="52" spans="2:16" ht="17">
+      <c r="B52" s="16"/>
       <c r="C52" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>16</v>
@@ -3987,50 +4006,50 @@
         <v>18</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="H52" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="H52" s="12" t="s">
         <v>7</v>
       </c>
       <c r="I52" s="1" t="s">
         <v>8</v>
       </c>
       <c r="J52" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K52" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L52" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M52" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N52" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="O52" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="O52" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="P52" s="4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="53" spans="2:16" ht="34">
+      <c r="B53" s="18"/>
+      <c r="H53" s="12"/>
+      <c r="O53" s="39" t="s">
         <v>55</v>
       </c>
-      <c r="P52" s="28" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="53" spans="2:16">
-      <c r="B53" s="20"/>
-      <c r="H53" s="14"/>
-      <c r="O53" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="P53" s="28" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="54" spans="2:16">
-      <c r="B54" s="18"/>
+      <c r="P53" s="4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="54" spans="2:16" ht="17">
+      <c r="B54" s="16"/>
       <c r="C54" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>19</v>
@@ -4042,40 +4061,40 @@
         <v>18</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="H54" s="14" t="s">
-        <v>54</v>
+        <v>83</v>
+      </c>
+      <c r="H54" s="12" t="s">
+        <v>53</v>
       </c>
       <c r="I54" s="1" t="s">
         <v>8</v>
       </c>
       <c r="J54" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K54" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L54" s="1">
         <v>0</v>
       </c>
       <c r="M54" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N54" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="O54" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="O54" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="P54" s="1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="55" spans="2:16">
-      <c r="B55" s="18"/>
+      <c r="P54" s="13" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="55" spans="2:16" ht="17">
+      <c r="B55" s="16"/>
       <c r="C55" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>19</v>
@@ -4089,58 +4108,58 @@
       <c r="G55" s="1">
         <v>1</v>
       </c>
-      <c r="H55" s="14" t="s">
-        <v>54</v>
+      <c r="H55" s="12" t="s">
+        <v>53</v>
       </c>
       <c r="I55" s="1" t="s">
         <v>8</v>
       </c>
       <c r="J55" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K55" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L55" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="M55" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="N55" s="1">
+        <v>0</v>
+      </c>
+      <c r="O55" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="M55" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="N55" s="1">
-        <v>0</v>
-      </c>
-      <c r="O55" s="3" t="s">
+      <c r="P55" s="27" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="56" spans="2:16" ht="34">
+      <c r="B56" s="18"/>
+      <c r="H56" s="12"/>
+      <c r="O56" s="39" t="s">
         <v>75</v>
       </c>
-      <c r="P55" s="31" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="56" spans="2:16">
-      <c r="B56" s="20"/>
-      <c r="H56" s="14"/>
-      <c r="O56" s="3" t="s">
+      <c r="P56" s="27" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="57" spans="2:16" ht="34">
+      <c r="B57" s="18"/>
+      <c r="H57" s="12"/>
+      <c r="O57" s="39" t="s">
         <v>76</v>
       </c>
-      <c r="P56" s="31" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="57" spans="2:16">
-      <c r="B57" s="20"/>
-      <c r="H57" s="14"/>
-      <c r="O57" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="P57" s="31" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="58" spans="2:16">
-      <c r="B58" s="18"/>
+      <c r="P57" s="27" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="58" spans="2:16" ht="17">
+      <c r="B58" s="16"/>
       <c r="C58" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>19</v>
@@ -4152,50 +4171,50 @@
         <v>18</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="H58" s="14" t="s">
-        <v>54</v>
+        <v>97</v>
+      </c>
+      <c r="H58" s="12" t="s">
+        <v>53</v>
       </c>
       <c r="I58" s="1" t="s">
         <v>8</v>
       </c>
       <c r="J58" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K58" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L58" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="M58" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="N58" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="O58" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="M58" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="N58" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="O58" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="P58" s="31" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="59" spans="2:16">
-      <c r="B59" s="20"/>
-      <c r="H59" s="14"/>
-      <c r="O59" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="P59" s="31" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="60" spans="2:16">
-      <c r="B60" s="18"/>
+      <c r="P58" s="27" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="59" spans="2:16" ht="34">
+      <c r="B59" s="18"/>
+      <c r="H59" s="12"/>
+      <c r="O59" s="39" t="s">
+        <v>76</v>
+      </c>
+      <c r="P59" s="27" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="60" spans="2:16" ht="34">
+      <c r="B60" s="16"/>
       <c r="C60" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>27</v>
@@ -4207,10 +4226,10 @@
         <v>0</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="H60" s="14" t="s">
-        <v>88</v>
+        <v>83</v>
+      </c>
+      <c r="H60" s="12" t="s">
+        <v>86</v>
       </c>
       <c r="I60" s="1" t="s">
         <v>8</v>
@@ -4230,20 +4249,20 @@
       <c r="N60" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="O60" s="13" t="s">
-        <v>139</v>
-      </c>
-      <c r="P60" s="1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="61" spans="2:16">
-      <c r="B61" s="18"/>
+      <c r="O60" s="39" t="s">
+        <v>135</v>
+      </c>
+      <c r="P60" s="13" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="61" spans="2:16" ht="34">
+      <c r="B61" s="16"/>
       <c r="C61" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>17</v>
@@ -4254,20 +4273,20 @@
       <c r="G61" s="1">
         <v>1</v>
       </c>
-      <c r="H61" s="14" t="s">
-        <v>88</v>
+      <c r="H61" s="12" t="s">
+        <v>86</v>
       </c>
       <c r="I61" s="1" t="s">
         <v>8</v>
       </c>
       <c r="J61" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K61" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L61" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M61" s="1" t="s">
         <v>32</v>
@@ -4275,50 +4294,50 @@
       <c r="N61" s="1">
         <v>0</v>
       </c>
-      <c r="O61" s="3" t="s">
+      <c r="O61" s="39" t="s">
+        <v>68</v>
+      </c>
+      <c r="P61" s="4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="62" spans="2:16" ht="17">
+      <c r="B62" s="18"/>
+      <c r="H62" s="13"/>
+      <c r="O62" s="39" t="s">
         <v>69</v>
       </c>
-      <c r="P61" s="28" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="62" spans="2:16">
-      <c r="B62" s="20"/>
-      <c r="H62" s="15"/>
-      <c r="O62" s="3" t="s">
+      <c r="P62" s="4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="63" spans="2:16" ht="34">
+      <c r="B63" s="18"/>
+      <c r="H63" s="13"/>
+      <c r="O63" s="39" t="s">
+        <v>79</v>
+      </c>
+      <c r="P63" s="27" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="64" spans="2:16" ht="34">
+      <c r="B64" s="18"/>
+      <c r="H64" s="13"/>
+      <c r="O64" s="39" t="s">
         <v>70</v>
       </c>
-      <c r="P62" s="28" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="63" spans="2:16">
-      <c r="B63" s="20"/>
-      <c r="H63" s="15"/>
-      <c r="O63" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="P63" s="31" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="64" spans="2:16">
-      <c r="B64" s="20"/>
-      <c r="H64" s="15"/>
-      <c r="O64" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="P64" s="28" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="65" spans="2:17">
-      <c r="B65" s="18"/>
+      <c r="P64" s="4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="65" spans="2:17" ht="34">
+      <c r="B65" s="16"/>
       <c r="C65" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E65" s="1" t="s">
         <v>17</v>
@@ -4327,63 +4346,63 @@
         <v>32</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="H65" s="14" t="s">
-        <v>88</v>
+        <v>97</v>
+      </c>
+      <c r="H65" s="12" t="s">
+        <v>86</v>
       </c>
       <c r="I65" s="1" t="s">
         <v>8</v>
       </c>
       <c r="J65" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K65" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L65" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M65" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N65" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="O65" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="O65" s="39" t="s">
+        <v>68</v>
+      </c>
+      <c r="P65" s="4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="66" spans="2:17" ht="17">
+      <c r="B66" s="23"/>
+      <c r="H66" s="15"/>
+      <c r="O66" s="39" t="s">
         <v>69</v>
       </c>
-      <c r="P65" s="28" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="66" spans="2:17">
-      <c r="B66" s="26"/>
-      <c r="H66" s="17"/>
-      <c r="O66" s="3" t="s">
+      <c r="P66" s="4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="67" spans="2:17" ht="34">
+      <c r="B67" s="24"/>
+      <c r="H67" s="15"/>
+      <c r="O67" s="39" t="s">
         <v>70</v>
       </c>
-      <c r="P66" s="28" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="67" spans="2:17">
-      <c r="B67" s="27"/>
-      <c r="H67" s="17"/>
-      <c r="O67" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="P67" s="28" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="68" spans="2:17">
-      <c r="B68" s="43"/>
+      <c r="P67" s="4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="68" spans="2:17" ht="34">
+      <c r="B68" s="30"/>
       <c r="C68" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="E68" s="1" t="s">
         <v>27</v>
@@ -4415,18 +4434,18 @@
       <c r="N68" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="O68" s="34" t="s">
-        <v>141</v>
-      </c>
-      <c r="P68" s="28" t="s">
-        <v>117</v>
-      </c>
-      <c r="Q68" s="32"/>
-    </row>
-    <row r="69" spans="2:17">
-      <c r="B69" s="18"/>
+      <c r="O68" s="43" t="s">
+        <v>137</v>
+      </c>
+      <c r="P68" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q68" s="28"/>
+    </row>
+    <row r="69" spans="2:17" ht="17">
+      <c r="B69" s="16"/>
       <c r="C69" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D69" s="4" t="s">
         <v>15</v>
@@ -4438,7 +4457,7 @@
         <v>27</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H69" s="1" t="s">
         <v>27</v>
@@ -4461,17 +4480,17 @@
       <c r="N69" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="O69" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="P69" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="70" spans="2:17">
-      <c r="B70" s="18"/>
+      <c r="O69" s="39" t="s">
+        <v>100</v>
+      </c>
+      <c r="P69" s="13" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="70" spans="2:17" ht="17">
+      <c r="B70" s="16"/>
       <c r="C70" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D70" s="4" t="s">
         <v>15</v>
@@ -4485,7 +4504,7 @@
       <c r="G70" s="1">
         <v>0</v>
       </c>
-      <c r="H70" s="16" t="s">
+      <c r="H70" s="14" t="s">
         <v>9</v>
       </c>
       <c r="I70" s="1" t="s">
@@ -4506,17 +4525,17 @@
       <c r="N70" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="O70" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="P70" s="28" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="71" spans="2:17">
-      <c r="B71" s="18"/>
+      <c r="O70" s="39" t="s">
+        <v>45</v>
+      </c>
+      <c r="P70" s="4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="71" spans="2:17" ht="17">
+      <c r="B71" s="16"/>
       <c r="C71" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D71" s="4" t="s">
         <v>15</v>
@@ -4530,7 +4549,7 @@
       <c r="G71" s="1">
         <v>0</v>
       </c>
-      <c r="H71" s="16" t="s">
+      <c r="H71" s="14" t="s">
         <v>11</v>
       </c>
       <c r="I71" s="1" t="s">
@@ -4551,18 +4570,18 @@
       <c r="N71" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="O71" s="13" t="s">
+      <c r="O71" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="P71" s="28" t="s">
-        <v>128</v>
-      </c>
-      <c r="Q71" s="13"/>
-    </row>
-    <row r="72" spans="2:17">
-      <c r="B72" s="18"/>
+      <c r="P71" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q71" s="11"/>
+    </row>
+    <row r="72" spans="2:17" ht="17">
+      <c r="B72" s="16"/>
       <c r="C72" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>15</v>
@@ -4576,11 +4595,11 @@
       <c r="G72" s="1">
         <v>0</v>
       </c>
-      <c r="H72" s="16" t="s">
+      <c r="H72" s="14" t="s">
         <v>11</v>
       </c>
       <c r="I72" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="J72" s="1" t="s">
         <v>8</v>
@@ -4597,17 +4616,17 @@
       <c r="N72" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="O72" s="13" t="s">
+      <c r="O72" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="P72" s="28" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="73" spans="2:17">
-      <c r="B73" s="18"/>
+      <c r="P72" s="4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="73" spans="2:17" ht="17">
+      <c r="B73" s="16"/>
       <c r="C73" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>15</v>
@@ -4621,39 +4640,39 @@
       <c r="G73" s="1">
         <v>0</v>
       </c>
-      <c r="H73" s="16" t="s">
+      <c r="H73" s="14" t="s">
         <v>11</v>
       </c>
       <c r="I73" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J73" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K73" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L73" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M73" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N73" s="1">
         <v>0</v>
       </c>
-      <c r="O73" s="13" t="s">
-        <v>133</v>
-      </c>
-      <c r="P73" s="28" t="s">
-        <v>131</v>
-      </c>
-      <c r="Q73" s="13"/>
-    </row>
-    <row r="74" spans="2:17">
-      <c r="B74" s="18"/>
+      <c r="O73" s="39" t="s">
+        <v>129</v>
+      </c>
+      <c r="P73" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q73" s="11"/>
+    </row>
+    <row r="74" spans="2:17" ht="17">
+      <c r="B74" s="16"/>
       <c r="C74" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D74" s="4" t="s">
         <v>15</v>
@@ -4667,7 +4686,7 @@
       <c r="G74" s="1">
         <v>0</v>
       </c>
-      <c r="H74" s="16" t="s">
+      <c r="H74" s="14" t="s">
         <v>22</v>
       </c>
       <c r="I74" s="1" t="s">
@@ -4688,17 +4707,17 @@
       <c r="N74" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="O74" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="P74" s="28" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="75" spans="2:17">
-      <c r="B75" s="18"/>
+      <c r="O74" s="39" t="s">
+        <v>43</v>
+      </c>
+      <c r="P74" s="4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="75" spans="2:17" ht="17">
+      <c r="B75" s="16"/>
       <c r="C75" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D75" s="4" t="s">
         <v>15</v>
@@ -4712,7 +4731,7 @@
       <c r="G75" s="1">
         <v>0</v>
       </c>
-      <c r="H75" s="16" t="s">
+      <c r="H75" s="14" t="s">
         <v>28</v>
       </c>
       <c r="I75" s="1" t="s">
@@ -4733,66 +4752,66 @@
       <c r="N75" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="O75" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="P75" s="28" t="s">
+      <c r="O75" s="39" t="s">
+        <v>46</v>
+      </c>
+      <c r="P75" s="4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="76" spans="2:17" ht="34">
+      <c r="B76" s="16"/>
+      <c r="C76" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D76" s="1">
+        <v>0</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G76" s="1">
+        <v>0</v>
+      </c>
+      <c r="H76" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="I76" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J76" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K76" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L76" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M76" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N76" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="O76" s="43" t="s">
+        <v>134</v>
+      </c>
+      <c r="P76" s="27" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="76" spans="2:17">
-      <c r="B76" s="18"/>
-      <c r="C76" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D76" s="1">
-        <v>0</v>
-      </c>
-      <c r="E76" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F76" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G76" s="1">
-        <v>0</v>
-      </c>
-      <c r="H76" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="I76" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J76" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K76" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L76" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="M76" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="N76" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="O76" s="34" t="s">
-        <v>138</v>
-      </c>
-      <c r="P76" s="31" t="s">
-        <v>132</v>
-      </c>
-      <c r="Q76" s="25"/>
-    </row>
-    <row r="77" spans="2:17">
-      <c r="B77" s="18"/>
+      <c r="Q76" s="22"/>
+    </row>
+    <row r="77" spans="2:17" ht="34">
+      <c r="B77" s="16"/>
       <c r="C77" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E77" s="1" t="s">
         <v>17</v>
@@ -4803,41 +4822,38 @@
       <c r="G77" s="1">
         <v>0</v>
       </c>
-      <c r="H77" s="14" t="s">
+      <c r="H77" s="12" t="s">
         <v>7</v>
       </c>
       <c r="I77" s="1" t="s">
         <v>8</v>
       </c>
       <c r="J77" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K77" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L77" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M77" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N77" s="1">
         <v>0</v>
       </c>
-      <c r="O77" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="P77" s="31" t="s">
-        <v>132</v>
-      </c>
-      <c r="Q77" s="3" t="s">
-        <v>112</v>
+      <c r="O77" s="39" t="s">
+        <v>71</v>
+      </c>
+      <c r="P77" s="27" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="78" spans="2:17" ht="17" customHeight="1">
-      <c r="B78" s="18"/>
+      <c r="B78" s="16"/>
       <c r="C78" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>15</v>
@@ -4851,41 +4867,41 @@
       <c r="G78" s="1">
         <v>0</v>
       </c>
-      <c r="H78" s="14" t="s">
-        <v>54</v>
+      <c r="H78" s="12" t="s">
+        <v>53</v>
       </c>
       <c r="I78" s="1" t="s">
         <v>8</v>
       </c>
       <c r="J78" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K78" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L78" s="1">
         <v>0</v>
       </c>
       <c r="M78" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N78" s="1">
         <v>0</v>
       </c>
-      <c r="O78" s="3" t="s">
+      <c r="O78" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="P78" s="1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="79" spans="2:17">
-      <c r="B79" s="18"/>
+      <c r="P78" s="13" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="79" spans="2:17" ht="17">
+      <c r="B79" s="16"/>
       <c r="C79" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="E79" s="1">
         <v>1</v>
@@ -4896,402 +4912,468 @@
       <c r="G79" s="1">
         <v>0</v>
       </c>
-      <c r="H79" s="14" t="s">
-        <v>54</v>
+      <c r="H79" s="12" t="s">
+        <v>53</v>
       </c>
       <c r="I79" s="1" t="s">
         <v>8</v>
       </c>
       <c r="J79" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K79" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="L79" s="1">
+        <v>0</v>
+      </c>
+      <c r="M79" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="N79" s="1">
+        <v>0</v>
+      </c>
+      <c r="O79" s="39" t="s">
+        <v>141</v>
+      </c>
+      <c r="P79" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q79" s="11"/>
+    </row>
+    <row r="80" spans="2:17" ht="17">
+      <c r="B80" s="18"/>
+      <c r="H80" s="12"/>
+      <c r="O80" s="39" t="s">
+        <v>61</v>
+      </c>
+      <c r="P80" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q80" s="29"/>
+    </row>
+    <row r="81" spans="2:17" ht="17">
+      <c r="B81" s="16"/>
+      <c r="C81" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E81" s="1">
+        <v>1</v>
+      </c>
+      <c r="F81" s="1">
+        <v>0</v>
+      </c>
+      <c r="G81" s="1">
+        <v>0</v>
+      </c>
+      <c r="H81" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="I81" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J81" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K81" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="K79" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="L79" s="1">
-        <v>0</v>
-      </c>
-      <c r="M79" s="1" t="s">
+      <c r="L81" s="1">
+        <v>0</v>
+      </c>
+      <c r="M81" s="1">
+        <v>0</v>
+      </c>
+      <c r="N81" s="1">
+        <v>0</v>
+      </c>
+      <c r="O81" s="42" t="s">
+        <v>62</v>
+      </c>
+      <c r="P81" s="27" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="82" spans="2:17" ht="17">
+      <c r="B82" s="18"/>
+      <c r="H82" s="12"/>
+      <c r="O82" s="39" t="s">
+        <v>141</v>
+      </c>
+      <c r="P82" s="27" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="83" spans="2:17" ht="34">
+      <c r="B83" s="18"/>
+      <c r="H83" s="12"/>
+      <c r="O83" s="39" t="s">
+        <v>105</v>
+      </c>
+      <c r="P83" s="27" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="84" spans="2:17" ht="17">
+      <c r="B84" s="18"/>
+      <c r="H84" s="12"/>
+      <c r="O84" s="39" t="s">
+        <v>80</v>
+      </c>
+      <c r="P84" s="27" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q84" s="29"/>
+    </row>
+    <row r="85" spans="2:17" ht="17">
+      <c r="B85" s="16"/>
+      <c r="C85" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G85" s="1">
+        <v>0</v>
+      </c>
+      <c r="H85" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="I85" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J85" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K85" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="L85" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="M85" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="N85" s="1">
+        <v>0</v>
+      </c>
+      <c r="O85" s="39" t="s">
+        <v>141</v>
+      </c>
+      <c r="P85" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="86" spans="2:17" ht="17">
+      <c r="B86" s="18"/>
+      <c r="H86" s="12"/>
+      <c r="O86" s="39" t="s">
+        <v>61</v>
+      </c>
+      <c r="P86" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q86" s="29"/>
+    </row>
+    <row r="87" spans="2:17" ht="18" customHeight="1">
+      <c r="B87" s="16"/>
+      <c r="C87" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F87" s="1">
+        <v>0</v>
+      </c>
+      <c r="G87" s="1">
+        <v>0</v>
+      </c>
+      <c r="H87" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="I87" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J87" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K87" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L87" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M87" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N87" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="O87" s="39" t="s">
+        <v>135</v>
+      </c>
+      <c r="P87" s="13" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="88" spans="2:17" ht="34">
+      <c r="B88" s="16"/>
+      <c r="C88" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F88" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G88" s="1">
+        <v>0</v>
+      </c>
+      <c r="H88" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="I88" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J88" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K88" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="L88" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="N79" s="1">
-        <v>0</v>
-      </c>
-      <c r="O79" s="13" t="s">
+      <c r="M88" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="N88" s="1">
+        <v>0</v>
+      </c>
+      <c r="O88" s="39" t="s">
+        <v>78</v>
+      </c>
+      <c r="P88" s="27" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="89" spans="2:17" ht="17">
+      <c r="B89" s="18"/>
+      <c r="H89" s="12"/>
+      <c r="O89" s="39" t="s">
+        <v>141</v>
+      </c>
+      <c r="P89" s="27" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q89" s="29"/>
+    </row>
+    <row r="90" spans="2:17" ht="17">
+      <c r="B90" s="18"/>
+      <c r="H90" s="12"/>
+      <c r="O90" s="39" t="s">
+        <v>60</v>
+      </c>
+      <c r="P90" s="27" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q90" s="11"/>
+    </row>
+    <row r="91" spans="2:17" ht="34">
+      <c r="B91" s="16"/>
+      <c r="C91" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E91" s="1">
+        <v>0</v>
+      </c>
+      <c r="F91" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G91" s="1">
+        <v>0</v>
+      </c>
+      <c r="H91" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="I91" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J91" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K91" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="L91" s="1">
+        <v>0</v>
+      </c>
+      <c r="M91" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="N91" s="1">
+        <v>0</v>
+      </c>
+      <c r="O91" s="39" t="s">
+        <v>78</v>
+      </c>
+      <c r="P91" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="92" spans="2:17" ht="17">
+      <c r="B92" s="18"/>
+      <c r="H92" s="12"/>
+      <c r="O92" s="39" t="s">
+        <v>141</v>
+      </c>
+      <c r="P92" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q92" s="29"/>
+    </row>
+    <row r="93" spans="2:17" ht="17">
+      <c r="B93" s="18"/>
+      <c r="H93" s="12"/>
+      <c r="O93" s="39" t="s">
+        <v>60</v>
+      </c>
+      <c r="P93" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q93" s="11"/>
+    </row>
+    <row r="94" spans="2:17" ht="34">
+      <c r="B94" s="16"/>
+      <c r="C94" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E94" s="1">
+        <v>0</v>
+      </c>
+      <c r="F94" s="1">
+        <v>1</v>
+      </c>
+      <c r="G94" s="1">
+        <v>0</v>
+      </c>
+      <c r="H94" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="I94" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J94" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K94" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L94" s="1">
+        <v>0</v>
+      </c>
+      <c r="M94" s="1">
+        <v>0</v>
+      </c>
+      <c r="N94" s="1">
+        <v>0</v>
+      </c>
+      <c r="O94" s="39" t="s">
+        <v>78</v>
+      </c>
+      <c r="P94" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="95" spans="2:17" ht="17">
+      <c r="B95" s="18"/>
+      <c r="H95" s="15"/>
+      <c r="O95" s="42" t="s">
         <v>62</v>
       </c>
-      <c r="P79" s="33" t="s">
-        <v>134</v>
-      </c>
-      <c r="Q79" s="13"/>
-    </row>
-    <row r="80" spans="2:17">
-      <c r="B80" s="18"/>
-      <c r="C80" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D80" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E80" s="1">
-        <v>1</v>
-      </c>
-      <c r="F80" s="1">
-        <v>0</v>
-      </c>
-      <c r="G80" s="1">
-        <v>0</v>
-      </c>
-      <c r="H80" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="I80" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J80" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="K80" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="L80" s="1">
-        <v>0</v>
-      </c>
-      <c r="M80" s="1">
-        <v>0</v>
-      </c>
-      <c r="N80" s="1">
-        <v>0</v>
-      </c>
-      <c r="O80" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="P80" s="31" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="81" spans="2:17">
-      <c r="B81" s="20"/>
-      <c r="H81" s="14"/>
-      <c r="O81" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="P81" s="31" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="82" spans="2:17">
-      <c r="B82" s="20"/>
-      <c r="H82" s="14"/>
-      <c r="O82" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="P82" s="31" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="83" spans="2:17">
-      <c r="B83" s="18"/>
-      <c r="C83" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D83" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="E83" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="F83" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G83" s="1">
-        <v>0</v>
-      </c>
-      <c r="H83" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="I83" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J83" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="K83" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="L83" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="M83" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="N83" s="1">
-        <v>0</v>
-      </c>
-      <c r="O83" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="P83" s="33" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="84" spans="2:17">
-      <c r="B84" s="18"/>
-      <c r="C84" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D84" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="E84" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F84" s="1">
-        <v>0</v>
-      </c>
-      <c r="G84" s="1">
-        <v>0</v>
-      </c>
-      <c r="H84" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="I84" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J84" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K84" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L84" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="M84" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="N84" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="O84" s="32" t="s">
-        <v>139</v>
-      </c>
-      <c r="P84" s="1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="85" spans="2:17">
-      <c r="B85" s="18"/>
-      <c r="C85" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D85" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="E85" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F85" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G85" s="1">
-        <v>0</v>
-      </c>
-      <c r="H85" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="I85" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J85" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="K85" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="L85" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="M85" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="N85" s="1">
-        <v>0</v>
-      </c>
-      <c r="O85" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="P85" s="31" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="86" spans="2:17">
-      <c r="B86" s="20"/>
-      <c r="H86" s="14"/>
-      <c r="O86" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="P86" s="31" t="s">
-        <v>132</v>
-      </c>
-      <c r="Q86" s="13"/>
-    </row>
-    <row r="87" spans="2:17">
-      <c r="B87" s="18"/>
-      <c r="C87" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D87" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="E87" s="1">
-        <v>0</v>
-      </c>
-      <c r="F87" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="G87" s="1">
-        <v>0</v>
-      </c>
-      <c r="H87" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="I87" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J87" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="K87" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="L87" s="1">
-        <v>0</v>
-      </c>
-      <c r="M87" s="1" t="s">
+      <c r="P95" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="96" spans="2:17" ht="17">
+      <c r="B96" s="18"/>
+      <c r="H96" s="15"/>
+      <c r="O96" s="39" t="s">
+        <v>141</v>
+      </c>
+      <c r="P96" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q96" s="29"/>
+    </row>
+    <row r="97" spans="2:17" ht="34">
+      <c r="B97" s="18"/>
+      <c r="H97" s="15"/>
+      <c r="O97" s="39" t="s">
         <v>104</v>
       </c>
-      <c r="N87" s="1">
-        <v>0</v>
-      </c>
-      <c r="O87" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="P87" s="33" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="88" spans="2:17">
-      <c r="B88" s="20"/>
-      <c r="H88" s="14"/>
-      <c r="O88" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="P88" s="33" t="s">
-        <v>134</v>
-      </c>
-      <c r="Q88" s="13"/>
-    </row>
-    <row r="89" spans="2:17">
-      <c r="B89" s="18"/>
-      <c r="C89" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D89" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E89" s="1">
-        <v>0</v>
-      </c>
-      <c r="F89" s="1">
-        <v>1</v>
-      </c>
-      <c r="G89" s="1">
-        <v>0</v>
-      </c>
-      <c r="H89" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="I89" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J89" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="K89" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="L89" s="1">
-        <v>0</v>
-      </c>
-      <c r="M89" s="1">
-        <v>0</v>
-      </c>
-      <c r="N89" s="1">
-        <v>0</v>
-      </c>
-      <c r="O89" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="P89" s="33" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="90" spans="2:17">
-      <c r="B90" s="20"/>
-      <c r="H90" s="17"/>
-      <c r="O90" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="P90" s="33" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="91" spans="2:17">
-      <c r="B91" s="20"/>
-      <c r="H91" s="17"/>
-      <c r="O91" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="P91" s="33" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="92" spans="2:17">
-      <c r="B92" s="20"/>
-      <c r="H92" s="17"/>
-      <c r="O92" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="P92" s="33" t="s">
-        <v>134</v>
-      </c>
-      <c r="Q92" s="13"/>
-    </row>
-    <row r="93" spans="2:17">
-      <c r="H93" s="15"/>
-      <c r="O93"/>
-      <c r="Q93"/>
-    </row>
-    <row r="94" spans="2:17">
-      <c r="H94" s="15"/>
-      <c r="O94"/>
-      <c r="Q94"/>
-    </row>
-    <row r="95" spans="2:17">
-      <c r="H95" s="14"/>
-    </row>
-    <row r="96" spans="2:17">
-      <c r="H96" s="14"/>
-    </row>
-    <row r="97" spans="8:8">
-      <c r="H97" s="14"/>
-    </row>
-    <row r="98" spans="8:8">
-      <c r="H98" s="14"/>
-    </row>
-    <row r="99" spans="8:8">
-      <c r="H99" s="15"/>
+      <c r="P97" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="98" spans="2:17" ht="17">
+      <c r="B98" s="18"/>
+      <c r="H98" s="15"/>
+      <c r="O98" s="39" t="s">
+        <v>80</v>
+      </c>
+      <c r="P98" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q98" s="11"/>
+    </row>
+    <row r="99" spans="2:17">
+      <c r="H99" s="13"/>
+      <c r="O99" s="44"/>
+      <c r="Q99"/>
+    </row>
+    <row r="100" spans="2:17">
+      <c r="H100" s="13"/>
+      <c r="O100" s="44"/>
+      <c r="Q100"/>
+    </row>
+    <row r="101" spans="2:17">
+      <c r="H101" s="12"/>
+    </row>
+    <row r="102" spans="2:17">
+      <c r="H102" s="12"/>
+    </row>
+    <row r="103" spans="2:17">
+      <c r="H103" s="12"/>
+    </row>
+    <row r="104" spans="2:17">
+      <c r="H104" s="12"/>
+    </row>
+    <row r="105" spans="2:17">
+      <c r="H105" s="13"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0"/>

</xml_diff>

<commit_message>
Reviewed/cleaned the code to confirm that the implementation satisfies the EFSM design as per the spreadsheet.  One of the timings tests is failing with no logging very infrequently.  Need to figure out where the error is.
</commit_message>
<xml_diff>
--- a/docs/RuntimeDesign.xlsx
+++ b/docs/RuntimeDesign.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jared/Projects/OrchestrationRuntime/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9439BD9-9834-5A4A-8E32-A941DF76F145}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82816A65-3637-E941-B21C-E2CCC19555BA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="17560" xr2:uid="{9B8D0C4A-3FF1-A04E-B8F8-B86CE3BC2D78}"/>
   </bookViews>
@@ -804,20 +804,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Wait for </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="8" tint="-0.249977111117893"/>
-        <rFont val="Calibri (Body)_x0000_"/>
-      </rPr>
-      <t>activateThread</t>
-    </r>
-  </si>
-  <si>
     <t>computationFinished</t>
   </si>
   <si>
@@ -1379,6 +1365,9 @@
       </rPr>
       <t>: THIS WOULD LEAD TO DEADLOCK.  See specifications.</t>
     </r>
+  </si>
+  <si>
+    <t>N_i &lt;= N_max</t>
   </si>
 </sst>
 </file>
@@ -1649,7 +1638,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1693,19 +1682,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1725,33 +1702,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1783,16 +1733,49 @@
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2109,11 +2092,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98772F20-44FC-FE45-839B-70D0417F8C61}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="B1:R107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1:B5"/>
+      <pane ySplit="5" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C96" sqref="C96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2122,7 +2108,7 @@
     <col min="2" max="2" width="3.1640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="3" style="1" customWidth="1"/>
     <col min="4" max="4" width="20.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.1640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="18.1640625" style="1" customWidth="1"/>
     <col min="6" max="6" width="10.33203125" style="1" customWidth="1"/>
     <col min="7" max="7" width="13.5" style="1" customWidth="1"/>
     <col min="8" max="8" width="11.5" style="1" customWidth="1"/>
@@ -2133,78 +2119,78 @@
     <col min="13" max="13" width="12.1640625" style="1" customWidth="1"/>
     <col min="14" max="14" width="14.5" style="1" customWidth="1"/>
     <col min="15" max="15" width="11.1640625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="59.5" style="36" customWidth="1"/>
+    <col min="16" max="16" width="59.5" style="23" customWidth="1"/>
     <col min="17" max="17" width="31.83203125" style="1" customWidth="1"/>
     <col min="18" max="18" width="99.6640625" style="2" customWidth="1"/>
     <col min="19" max="19" width="72.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:18" ht="16" customHeight="1">
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="34" t="s">
+        <v>135</v>
+      </c>
+      <c r="C1" s="34" t="s">
         <v>136</v>
       </c>
-      <c r="C1" s="45" t="s">
-        <v>137</v>
-      </c>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="35"/>
-      <c r="L1" s="35"/>
-      <c r="M1" s="35"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="43"/>
+      <c r="L1" s="43"/>
+      <c r="M1" s="43"/>
     </row>
     <row r="2" spans="2:18" ht="17" thickBot="1">
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
     </row>
     <row r="3" spans="2:18" ht="17" thickBot="1">
-      <c r="B3" s="45"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="28" t="s">
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="36" t="s">
         <v>35</v>
       </c>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="31"/>
-      <c r="K3" s="28" t="s">
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="39"/>
+      <c r="K3" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="L3" s="29"/>
-      <c r="M3" s="29"/>
-      <c r="N3" s="30"/>
-      <c r="O3" s="31"/>
+      <c r="L3" s="37"/>
+      <c r="M3" s="37"/>
+      <c r="N3" s="38"/>
+      <c r="O3" s="39"/>
     </row>
     <row r="4" spans="2:18" ht="17" thickBot="1">
-      <c r="B4" s="45"/>
-      <c r="C4" s="45"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="34"/>
       <c r="D4" s="4"/>
-      <c r="E4" s="32" t="s">
+      <c r="E4" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="34"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="41"/>
+      <c r="H4" s="42"/>
       <c r="K4" s="4"/>
-      <c r="L4" s="32" t="s">
+      <c r="L4" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="M4" s="33"/>
-      <c r="N4" s="33"/>
-      <c r="O4" s="34"/>
+      <c r="M4" s="41"/>
+      <c r="N4" s="41"/>
+      <c r="O4" s="42"/>
     </row>
     <row r="5" spans="2:18" ht="18" thickBot="1">
-      <c r="B5" s="45"/>
-      <c r="C5" s="45"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="34"/>
       <c r="D5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F5" s="8" t="s">
         <v>13</v>
@@ -2225,7 +2211,7 @@
         <v>0</v>
       </c>
       <c r="L5" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="M5" s="8" t="s">
         <v>13</v>
@@ -2236,66 +2222,66 @@
       <c r="O5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="P5" s="37" t="s">
+      <c r="P5" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="Q5" s="43" t="s">
+      <c r="Q5" s="30" t="s">
+        <v>106</v>
+      </c>
+      <c r="R5" s="9"/>
+    </row>
+    <row r="6" spans="2:18" ht="17">
+      <c r="B6" s="35" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" s="35"/>
+      <c r="D6" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" s="16">
+        <v>0</v>
+      </c>
+      <c r="G6" s="16">
+        <v>0</v>
+      </c>
+      <c r="H6" s="16">
+        <v>0</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="P6" s="25" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q6" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="R5" s="9"/>
-    </row>
-    <row r="6" spans="2:18" ht="17">
-      <c r="B6" s="46" t="s">
-        <v>78</v>
-      </c>
-      <c r="C6" s="46"/>
-      <c r="D6" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="E6" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="F6" s="20">
-        <v>0</v>
-      </c>
-      <c r="G6" s="20">
-        <v>0</v>
-      </c>
-      <c r="H6" s="20">
-        <v>0</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="O6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="P6" s="38" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q6" s="3" t="s">
-        <v>108</v>
-      </c>
       <c r="R6" s="9"/>
     </row>
     <row r="7" spans="2:18" ht="17">
-      <c r="B7" s="47"/>
-      <c r="C7" s="18"/>
+      <c r="B7" s="32"/>
+      <c r="C7" s="44"/>
       <c r="D7" s="1" t="s">
         <v>4</v>
       </c>
@@ -2332,16 +2318,16 @@
       <c r="O7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="P7" s="39" t="s">
-        <v>131</v>
+      <c r="P7" s="26" t="s">
+        <v>130</v>
       </c>
       <c r="Q7" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="8" spans="2:18" ht="17">
-      <c r="B8" s="47"/>
-      <c r="C8" s="18"/>
+      <c r="B8" s="32"/>
+      <c r="C8" s="44"/>
       <c r="D8" s="1" t="s">
         <v>4</v>
       </c>
@@ -2378,17 +2364,17 @@
       <c r="O8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="P8" s="42" t="s">
-        <v>132</v>
+      <c r="P8" s="29" t="s">
+        <v>131</v>
       </c>
       <c r="Q8" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="R8" s="10"/>
     </row>
     <row r="9" spans="2:18" ht="17">
-      <c r="B9" s="48"/>
-      <c r="C9" s="16"/>
+      <c r="B9" s="33"/>
+      <c r="C9" s="33"/>
       <c r="D9" s="1" t="s">
         <v>4</v>
       </c>
@@ -2425,16 +2411,16 @@
       <c r="O9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="P9" s="36" t="s">
+      <c r="P9" s="23" t="s">
         <v>23</v>
       </c>
       <c r="Q9" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="10" spans="2:18" ht="17">
-      <c r="B10" s="47"/>
-      <c r="C10" s="15"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="32"/>
       <c r="D10" s="1" t="s">
         <v>4</v>
       </c>
@@ -2454,7 +2440,7 @@
         <v>9</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>5</v>
@@ -2471,16 +2457,16 @@
       <c r="O10" s="1">
         <v>0</v>
       </c>
-      <c r="P10" s="36" t="s">
-        <v>86</v>
+      <c r="P10" s="23" t="s">
+        <v>85</v>
       </c>
       <c r="Q10" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="11" spans="2:18" ht="17">
-      <c r="B11" s="47"/>
-      <c r="C11" s="15"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
       <c r="D11" s="1" t="s">
         <v>4</v>
       </c>
@@ -2517,17 +2503,17 @@
       <c r="O11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="P11" s="36" t="s">
+      <c r="P11" s="23" t="s">
         <v>23</v>
       </c>
       <c r="Q11" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="R11" s="10"/>
     </row>
     <row r="12" spans="2:18" ht="17">
-      <c r="B12" s="47"/>
-      <c r="C12" s="15"/>
+      <c r="B12" s="32"/>
+      <c r="C12" s="32"/>
       <c r="D12" s="1" t="s">
         <v>4</v>
       </c>
@@ -2564,17 +2550,17 @@
       <c r="O12" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="P12" s="36" t="s">
-        <v>85</v>
+      <c r="P12" s="23" t="s">
+        <v>84</v>
       </c>
       <c r="Q12" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="R12" s="10"/>
     </row>
     <row r="13" spans="2:18" ht="17">
-      <c r="B13" s="47"/>
-      <c r="C13" s="19"/>
+      <c r="B13" s="32"/>
+      <c r="C13" s="45"/>
       <c r="D13" s="1" t="s">
         <v>4</v>
       </c>
@@ -2611,16 +2597,16 @@
       <c r="O13" s="1">
         <v>0</v>
       </c>
-      <c r="P13" s="36" t="s">
+      <c r="P13" s="23" t="s">
         <v>61</v>
       </c>
       <c r="Q13" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="14" spans="2:18" ht="17">
-      <c r="B14" s="47"/>
-      <c r="C14" s="19"/>
+      <c r="B14" s="32"/>
+      <c r="C14" s="45"/>
       <c r="D14" s="1" t="s">
         <v>4</v>
       </c>
@@ -2657,17 +2643,17 @@
       <c r="O14" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="P14" s="36" t="s">
+      <c r="P14" s="23" t="s">
         <v>24</v>
       </c>
       <c r="Q14" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="R14" s="10"/>
     </row>
     <row r="15" spans="2:18" ht="17">
-      <c r="B15" s="47"/>
-      <c r="C15" s="19"/>
+      <c r="B15" s="32"/>
+      <c r="C15" s="45"/>
       <c r="D15" s="1" t="s">
         <v>4</v>
       </c>
@@ -2704,16 +2690,16 @@
       <c r="O15" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="P15" s="36" t="s">
+      <c r="P15" s="23" t="s">
         <v>26</v>
       </c>
       <c r="Q15" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="16" spans="2:18" ht="34">
-      <c r="B16" s="47"/>
-      <c r="C16" s="19"/>
+      <c r="B16" s="32"/>
+      <c r="C16" s="45"/>
       <c r="D16" s="1" t="s">
         <v>4</v>
       </c>
@@ -2750,16 +2736,16 @@
       <c r="O16" s="1">
         <v>0</v>
       </c>
-      <c r="P16" s="36" t="s">
+      <c r="P16" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="Q16" s="24" t="s">
-        <v>124</v>
+      <c r="Q16" s="20" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="17" spans="2:18" ht="17">
-      <c r="B17" s="47"/>
-      <c r="C17" s="19"/>
+      <c r="B17" s="32"/>
+      <c r="C17" s="45"/>
       <c r="D17" s="1" t="s">
         <v>4</v>
       </c>
@@ -2796,16 +2782,16 @@
       <c r="O17" s="1">
         <v>0</v>
       </c>
-      <c r="P17" s="36" t="s">
-        <v>82</v>
-      </c>
-      <c r="Q17" s="24" t="s">
-        <v>124</v>
+      <c r="P17" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q17" s="20" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="18" spans="2:18" ht="17">
-      <c r="B18" s="47"/>
-      <c r="C18" s="19"/>
+      <c r="B18" s="32"/>
+      <c r="C18" s="45"/>
       <c r="D18" s="1" t="s">
         <v>4</v>
       </c>
@@ -2822,7 +2808,7 @@
         <v>0</v>
       </c>
       <c r="I18" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J18" s="1" t="s">
         <v>8</v>
@@ -2842,17 +2828,17 @@
       <c r="O18" s="1">
         <v>0</v>
       </c>
-      <c r="P18" s="36" t="s">
-        <v>129</v>
-      </c>
-      <c r="Q18" s="24" t="s">
-        <v>124</v>
+      <c r="P18" s="23" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q18" s="20" t="s">
+        <v>123</v>
       </c>
       <c r="R18" s="10"/>
     </row>
     <row r="19" spans="2:18" ht="17">
-      <c r="B19" s="47"/>
-      <c r="C19" s="15"/>
+      <c r="B19" s="32"/>
+      <c r="C19" s="32"/>
       <c r="D19" s="1" t="s">
         <v>5</v>
       </c>
@@ -2889,16 +2875,16 @@
       <c r="O19" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="P19" s="36" t="s">
+      <c r="P19" s="23" t="s">
         <v>43</v>
       </c>
       <c r="Q19" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="20" spans="2:18" ht="17">
-      <c r="B20" s="47"/>
-      <c r="C20" s="15"/>
+      <c r="B20" s="32"/>
+      <c r="C20" s="32"/>
       <c r="D20" s="1" t="s">
         <v>5</v>
       </c>
@@ -2935,16 +2921,16 @@
       <c r="O20" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="P20" s="36" t="s">
+      <c r="P20" s="23" t="s">
         <v>25</v>
       </c>
       <c r="Q20" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="21" spans="2:18" ht="17">
-      <c r="B21" s="47"/>
-      <c r="C21" s="15"/>
+      <c r="B21" s="32"/>
+      <c r="C21" s="32"/>
       <c r="D21" s="1" t="s">
         <v>5</v>
       </c>
@@ -2964,7 +2950,7 @@
         <v>11</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="K21" s="1" t="s">
         <v>8</v>
@@ -2981,16 +2967,16 @@
       <c r="O21" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="P21" s="36" t="s">
+      <c r="P21" s="23" t="s">
         <v>23</v>
       </c>
       <c r="Q21" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="22" spans="2:18" ht="17">
-      <c r="B22" s="47"/>
-      <c r="C22" s="15"/>
+      <c r="B22" s="32"/>
+      <c r="C22" s="32"/>
       <c r="D22" s="1" t="s">
         <v>5</v>
       </c>
@@ -3004,7 +2990,7 @@
         <v>18</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I22" s="13" t="s">
         <v>11</v>
@@ -3025,18 +3011,18 @@
         <v>39</v>
       </c>
       <c r="O22" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="P22" s="36" t="s">
-        <v>106</v>
+        <v>88</v>
+      </c>
+      <c r="P22" s="23" t="s">
+        <v>105</v>
       </c>
       <c r="Q22" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="23" spans="2:18" ht="17">
-      <c r="B23" s="47"/>
-      <c r="C23" s="15"/>
+      <c r="B23" s="32"/>
+      <c r="C23" s="32"/>
       <c r="D23" s="1" t="s">
         <v>5</v>
       </c>
@@ -3050,7 +3036,7 @@
         <v>18</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I23" s="13" t="s">
         <v>22</v>
@@ -3071,18 +3057,18 @@
         <v>39</v>
       </c>
       <c r="O23" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="P23" s="39" t="s">
         <v>92</v>
       </c>
+      <c r="P23" s="26" t="s">
+        <v>91</v>
+      </c>
       <c r="Q23" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="24" spans="2:18" ht="17">
-      <c r="B24" s="47"/>
-      <c r="C24" s="15"/>
+      <c r="B24" s="32"/>
+      <c r="C24" s="32"/>
       <c r="D24" s="1" t="s">
         <v>5</v>
       </c>
@@ -3119,38 +3105,38 @@
       <c r="O24" s="3">
         <v>0</v>
       </c>
-      <c r="P24" s="39" t="s">
+      <c r="P24" s="26" t="s">
         <v>59</v>
       </c>
       <c r="Q24" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="R24" s="10"/>
     </row>
     <row r="25" spans="2:18" ht="34">
-      <c r="C25" s="17"/>
+      <c r="C25" s="15"/>
       <c r="I25" s="13"/>
       <c r="J25" s="3"/>
       <c r="L25" s="3"/>
       <c r="M25" s="3"/>
       <c r="N25" s="3"/>
       <c r="O25" s="3"/>
-      <c r="P25" s="36" t="s">
-        <v>101</v>
-      </c>
-      <c r="Q25" s="24" t="s">
-        <v>135</v>
-      </c>
-      <c r="R25" s="26"/>
+      <c r="P25" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q25" s="20" t="s">
+        <v>134</v>
+      </c>
+      <c r="R25" s="22"/>
     </row>
     <row r="26" spans="2:18" ht="34">
-      <c r="B26" s="47"/>
-      <c r="C26" s="15"/>
+      <c r="B26" s="32"/>
+      <c r="C26" s="32"/>
       <c r="D26" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>104</v>
+        <v>15</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>17</v>
@@ -3182,21 +3168,21 @@
       <c r="O26" s="3">
         <v>0</v>
       </c>
-      <c r="P26" s="39" t="s">
-        <v>102</v>
+      <c r="P26" s="26" t="s">
+        <v>101</v>
       </c>
       <c r="Q26" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="27" spans="2:18" ht="17">
-      <c r="B27" s="47"/>
-      <c r="C27" s="15"/>
+      <c r="B27" s="32"/>
+      <c r="C27" s="32"/>
       <c r="D27" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>104</v>
+        <v>143</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>17</v>
@@ -3226,19 +3212,19 @@
         <v>39</v>
       </c>
       <c r="O27" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="P27" s="39" t="s">
+        <v>88</v>
+      </c>
+      <c r="P27" s="26" t="s">
         <v>20</v>
       </c>
       <c r="Q27" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="R27" s="10"/>
     </row>
     <row r="28" spans="2:18" ht="34">
-      <c r="B28" s="47"/>
-      <c r="C28" s="15"/>
+      <c r="B28" s="32"/>
+      <c r="C28" s="32"/>
       <c r="D28" s="1" t="s">
         <v>5</v>
       </c>
@@ -3275,16 +3261,16 @@
       <c r="O28" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="P28" s="40" t="s">
-        <v>138</v>
-      </c>
-      <c r="Q28" s="24" t="s">
-        <v>124</v>
+      <c r="P28" s="27" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q28" s="20" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="29" spans="2:18" ht="17">
-      <c r="B29" s="47"/>
-      <c r="C29" s="15"/>
+      <c r="B29" s="32"/>
+      <c r="C29" s="32"/>
       <c r="D29" s="1" t="s">
         <v>5</v>
       </c>
@@ -3321,16 +3307,16 @@
       <c r="O29" s="1">
         <v>0</v>
       </c>
-      <c r="P29" s="36" t="s">
+      <c r="P29" s="23" t="s">
         <v>48</v>
       </c>
       <c r="Q29" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="30" spans="2:18" ht="17">
-      <c r="B30" s="47"/>
-      <c r="C30" s="15"/>
+      <c r="B30" s="32"/>
+      <c r="C30" s="32"/>
       <c r="D30" s="1" t="s">
         <v>5</v>
       </c>
@@ -3365,27 +3351,27 @@
         <v>55</v>
       </c>
       <c r="O30" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="P30" s="36" t="s">
+        <v>89</v>
+      </c>
+      <c r="P30" s="23" t="s">
         <v>49</v>
       </c>
       <c r="Q30" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="31" spans="2:18" ht="34">
-      <c r="C31" s="17"/>
-      <c r="P31" s="36" t="s">
+      <c r="C31" s="15"/>
+      <c r="P31" s="23" t="s">
         <v>53</v>
       </c>
       <c r="Q31" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="32" spans="2:18" ht="17">
-      <c r="B32" s="47"/>
-      <c r="C32" s="15"/>
+      <c r="B32" s="32"/>
+      <c r="C32" s="32"/>
       <c r="D32" s="1" t="s">
         <v>5</v>
       </c>
@@ -3399,7 +3385,7 @@
         <v>18</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I32" s="11" t="s">
         <v>50</v>
@@ -3420,18 +3406,18 @@
         <v>39</v>
       </c>
       <c r="O32" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="P32" s="36" t="s">
+        <v>88</v>
+      </c>
+      <c r="P32" s="23" t="s">
         <v>20</v>
       </c>
       <c r="Q32" s="12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="33" spans="2:18" ht="17">
-      <c r="B33" s="47"/>
-      <c r="C33" s="15"/>
+      <c r="B33" s="32"/>
+      <c r="C33" s="32"/>
       <c r="D33" s="1" t="s">
         <v>5</v>
       </c>
@@ -3468,16 +3454,16 @@
       <c r="O33" s="1">
         <v>0</v>
       </c>
-      <c r="P33" s="36" t="s">
+      <c r="P33" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="Q33" s="24" t="s">
-        <v>124</v>
+      <c r="Q33" s="20" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="34" spans="2:18" ht="17">
-      <c r="B34" s="47"/>
-      <c r="C34" s="15"/>
+      <c r="B34" s="32"/>
+      <c r="C34" s="32"/>
       <c r="D34" s="1" t="s">
         <v>5</v>
       </c>
@@ -3509,31 +3495,31 @@
         <v>70</v>
       </c>
       <c r="N34" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="O34" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="P34" s="36" t="s">
+        <v>89</v>
+      </c>
+      <c r="P34" s="23" t="s">
         <v>63</v>
       </c>
       <c r="Q34" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="35" spans="2:18" ht="34">
-      <c r="C35" s="17"/>
+      <c r="C35" s="15"/>
       <c r="I35" s="11"/>
-      <c r="P35" s="36" t="s">
+      <c r="P35" s="23" t="s">
         <v>64</v>
       </c>
       <c r="Q35" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="36" spans="2:18" ht="17">
-      <c r="B36" s="47"/>
-      <c r="C36" s="15"/>
+      <c r="B36" s="32"/>
+      <c r="C36" s="32"/>
       <c r="D36" s="1" t="s">
         <v>5</v>
       </c>
@@ -3550,7 +3536,7 @@
         <v>27</v>
       </c>
       <c r="I36" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J36" s="1" t="s">
         <v>8</v>
@@ -3570,16 +3556,16 @@
       <c r="O36" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="P36" s="36" t="s">
-        <v>129</v>
+      <c r="P36" s="23" t="s">
+        <v>128</v>
       </c>
       <c r="Q36" s="12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="37" spans="2:18" ht="17">
-      <c r="B37" s="47"/>
-      <c r="C37" s="15"/>
+      <c r="B37" s="32"/>
+      <c r="C37" s="32"/>
       <c r="D37" s="1" t="s">
         <v>5</v>
       </c>
@@ -3596,7 +3582,7 @@
         <v>0</v>
       </c>
       <c r="I37" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J37" s="1" t="s">
         <v>8</v>
@@ -3608,7 +3594,7 @@
         <v>42</v>
       </c>
       <c r="M37" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="N37" s="1" t="s">
         <v>74</v>
@@ -3616,27 +3602,27 @@
       <c r="O37" s="1">
         <v>0</v>
       </c>
-      <c r="P37" s="36" t="s">
+      <c r="P37" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="Q37" s="44" t="s">
-        <v>133</v>
+      <c r="Q37" s="31" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="38" spans="2:18" ht="17">
       <c r="B38" s="10"/>
-      <c r="C38" s="17"/>
+      <c r="C38" s="15"/>
       <c r="I38" s="14"/>
-      <c r="P38" s="36" t="s">
+      <c r="P38" s="23" t="s">
         <v>56</v>
       </c>
       <c r="Q38" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="39" spans="2:18" ht="34">
-      <c r="B39" s="47"/>
-      <c r="C39" s="15"/>
+      <c r="B39" s="32"/>
+      <c r="C39" s="32"/>
       <c r="D39" s="1" t="s">
         <v>5</v>
       </c>
@@ -3653,7 +3639,7 @@
         <v>80</v>
       </c>
       <c r="I39" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J39" s="1" t="s">
         <v>8</v>
@@ -3671,38 +3657,38 @@
         <v>39</v>
       </c>
       <c r="O39" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="P39" s="36" t="s">
+        <v>89</v>
+      </c>
+      <c r="P39" s="23" t="s">
         <v>65</v>
       </c>
       <c r="Q39" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="40" spans="2:18" ht="17">
-      <c r="C40" s="17"/>
+      <c r="C40" s="15"/>
       <c r="I40" s="12"/>
-      <c r="P40" s="36" t="s">
+      <c r="P40" s="23" t="s">
         <v>66</v>
       </c>
       <c r="Q40" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="41" spans="2:18" ht="34">
-      <c r="C41" s="17"/>
+      <c r="C41" s="15"/>
       <c r="I41" s="12"/>
-      <c r="P41" s="36" t="s">
+      <c r="P41" s="23" t="s">
         <v>67</v>
       </c>
       <c r="Q41" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="42" spans="2:18" ht="17">
-      <c r="B42" s="47"/>
-      <c r="C42" s="15"/>
+      <c r="B42" s="32"/>
+      <c r="C42" s="32"/>
       <c r="D42" s="1" t="s">
         <v>46</v>
       </c>
@@ -3739,17 +3725,17 @@
       <c r="O42" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="P42" s="40" t="s">
-        <v>143</v>
+      <c r="P42" s="27" t="s">
+        <v>142</v>
       </c>
       <c r="Q42" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="R42" s="25"/>
+        <v>108</v>
+      </c>
+      <c r="R42" s="21"/>
     </row>
     <row r="43" spans="2:18" ht="17">
-      <c r="B43" s="47"/>
-      <c r="C43" s="15"/>
+      <c r="B43" s="32"/>
+      <c r="C43" s="32"/>
       <c r="D43" s="1" t="s">
         <v>46</v>
       </c>
@@ -3786,16 +3772,16 @@
       <c r="O43" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="P43" s="36" t="s">
+      <c r="P43" s="23" t="s">
         <v>43</v>
       </c>
       <c r="Q43" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="44" spans="2:18" ht="17">
-      <c r="B44" s="47"/>
-      <c r="C44" s="15"/>
+      <c r="B44" s="32"/>
+      <c r="C44" s="32"/>
       <c r="D44" s="1" t="s">
         <v>46</v>
       </c>
@@ -3832,16 +3818,16 @@
       <c r="O44" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="P44" s="36" t="s">
+      <c r="P44" s="23" t="s">
         <v>25</v>
       </c>
       <c r="Q44" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="45" spans="2:18" ht="17">
-      <c r="B45" s="47"/>
-      <c r="C45" s="15"/>
+      <c r="B45" s="32"/>
+      <c r="C45" s="32"/>
       <c r="D45" s="1" t="s">
         <v>46</v>
       </c>
@@ -3861,7 +3847,7 @@
         <v>11</v>
       </c>
       <c r="J45" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="K45" s="1" t="s">
         <v>8</v>
@@ -3878,16 +3864,16 @@
       <c r="O45" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="P45" s="36" t="s">
+      <c r="P45" s="23" t="s">
         <v>23</v>
       </c>
       <c r="Q45" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="46" spans="2:18" ht="34">
-      <c r="B46" s="47"/>
-      <c r="C46" s="15"/>
+      <c r="B46" s="32"/>
+      <c r="C46" s="32"/>
       <c r="D46" s="1" t="s">
         <v>46</v>
       </c>
@@ -3922,30 +3908,30 @@
         <v>39</v>
       </c>
       <c r="O46" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="P46" s="36" t="s">
+        <v>88</v>
+      </c>
+      <c r="P46" s="23" t="s">
+        <v>139</v>
+      </c>
+      <c r="Q46" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="47" spans="2:18" ht="34">
+      <c r="B47" s="15"/>
+      <c r="C47" s="15"/>
+      <c r="I47" s="13"/>
+      <c r="P47" s="23" t="s">
         <v>140</v>
       </c>
-      <c r="Q46" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="47" spans="2:18" ht="34">
-      <c r="B47" s="17"/>
-      <c r="C47" s="17"/>
-      <c r="I47" s="13"/>
-      <c r="P47" s="36" t="s">
-        <v>141</v>
-      </c>
       <c r="Q47" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="R47" s="26"/>
+        <v>112</v>
+      </c>
+      <c r="R47" s="22"/>
     </row>
     <row r="48" spans="2:18" ht="17">
-      <c r="B48" s="47"/>
-      <c r="C48" s="15"/>
+      <c r="B48" s="32"/>
+      <c r="C48" s="32"/>
       <c r="D48" s="1" t="s">
         <v>46</v>
       </c>
@@ -3982,16 +3968,16 @@
       <c r="O48" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="P48" s="36" t="s">
+      <c r="P48" s="23" t="s">
         <v>41</v>
       </c>
       <c r="Q48" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="49" spans="2:18" ht="17">
-      <c r="B49" s="47"/>
-      <c r="C49" s="15"/>
+      <c r="B49" s="32"/>
+      <c r="C49" s="32"/>
       <c r="D49" s="1" t="s">
         <v>46</v>
       </c>
@@ -4028,16 +4014,16 @@
       <c r="O49" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="P49" s="36" t="s">
+      <c r="P49" s="23" t="s">
         <v>44</v>
       </c>
       <c r="Q49" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="50" spans="2:18" ht="34">
-      <c r="B50" s="47"/>
-      <c r="C50" s="15"/>
+      <c r="B50" s="32"/>
+      <c r="C50" s="32"/>
       <c r="D50" s="1" t="s">
         <v>46</v>
       </c>
@@ -4074,17 +4060,17 @@
       <c r="O50" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="P50" s="40" t="s">
-        <v>138</v>
-      </c>
-      <c r="Q50" s="24" t="s">
-        <v>124</v>
+      <c r="P50" s="27" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q50" s="20" t="s">
+        <v>123</v>
       </c>
       <c r="R50" s="10"/>
     </row>
     <row r="51" spans="2:18" ht="17">
-      <c r="B51" s="47"/>
-      <c r="C51" s="15"/>
+      <c r="B51" s="32"/>
+      <c r="C51" s="32"/>
       <c r="D51" s="1" t="s">
         <v>46</v>
       </c>
@@ -4116,39 +4102,39 @@
         <v>40</v>
       </c>
       <c r="N51" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="O51" s="1">
         <v>0</v>
       </c>
-      <c r="P51" s="36" t="s">
+      <c r="P51" s="23" t="s">
         <v>51</v>
       </c>
       <c r="Q51" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="52" spans="2:18" ht="34">
-      <c r="C52" s="17"/>
-      <c r="P52" s="36" t="s">
+      <c r="C52" s="15"/>
+      <c r="P52" s="23" t="s">
         <v>69</v>
       </c>
       <c r="Q52" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="53" spans="2:18" ht="34">
-      <c r="C53" s="17"/>
-      <c r="P53" s="36" t="s">
+      <c r="C53" s="15"/>
+      <c r="P53" s="23" t="s">
         <v>52</v>
       </c>
       <c r="Q53" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="54" spans="2:18" ht="17">
-      <c r="B54" s="47"/>
-      <c r="C54" s="15"/>
+      <c r="B54" s="32"/>
+      <c r="C54" s="32"/>
       <c r="D54" s="1" t="s">
         <v>46</v>
       </c>
@@ -4162,7 +4148,7 @@
         <v>18</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I54" s="11" t="s">
         <v>7</v>
@@ -4180,31 +4166,31 @@
         <v>40</v>
       </c>
       <c r="N54" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="O54" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="P54" s="36" t="s">
+        <v>94</v>
+      </c>
+      <c r="P54" s="23" t="s">
         <v>51</v>
       </c>
       <c r="Q54" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="55" spans="2:18" ht="34">
-      <c r="C55" s="17"/>
+      <c r="C55" s="15"/>
       <c r="I55" s="11"/>
-      <c r="P55" s="36" t="s">
+      <c r="P55" s="23" t="s">
         <v>52</v>
       </c>
       <c r="Q55" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="56" spans="2:18" ht="17">
-      <c r="B56" s="47"/>
-      <c r="C56" s="15"/>
+      <c r="B56" s="32"/>
+      <c r="C56" s="32"/>
       <c r="D56" s="1" t="s">
         <v>46</v>
       </c>
@@ -4239,18 +4225,18 @@
         <v>39</v>
       </c>
       <c r="O56" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="P56" s="36" t="s">
+        <v>88</v>
+      </c>
+      <c r="P56" s="23" t="s">
         <v>20</v>
       </c>
       <c r="Q56" s="12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="57" spans="2:18" ht="17">
-      <c r="B57" s="47"/>
-      <c r="C57" s="15"/>
+      <c r="B57" s="32"/>
+      <c r="C57" s="32"/>
       <c r="D57" s="1" t="s">
         <v>46</v>
       </c>
@@ -4282,41 +4268,41 @@
         <v>70</v>
       </c>
       <c r="N57" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="O57" s="1">
         <v>0</v>
       </c>
-      <c r="P57" s="36" t="s">
+      <c r="P57" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="Q57" s="24" t="s">
-        <v>124</v>
+      <c r="Q57" s="20" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="58" spans="2:18" ht="34">
-      <c r="C58" s="17"/>
+      <c r="C58" s="15"/>
       <c r="I58" s="11"/>
-      <c r="P58" s="36" t="s">
+      <c r="P58" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="Q58" s="24" t="s">
-        <v>124</v>
+      <c r="Q58" s="20" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="59" spans="2:18" ht="34">
-      <c r="C59" s="17"/>
+      <c r="C59" s="15"/>
       <c r="I59" s="11"/>
-      <c r="P59" s="36" t="s">
+      <c r="P59" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="Q59" s="24" t="s">
-        <v>124</v>
+      <c r="Q59" s="20" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="60" spans="2:18" ht="17">
-      <c r="B60" s="47"/>
-      <c r="C60" s="15"/>
+      <c r="B60" s="32"/>
+      <c r="C60" s="32"/>
       <c r="D60" s="1" t="s">
         <v>46</v>
       </c>
@@ -4330,7 +4316,7 @@
         <v>18</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I60" s="11" t="s">
         <v>50</v>
@@ -4348,31 +4334,31 @@
         <v>70</v>
       </c>
       <c r="N60" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="O60" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="P60" s="36" t="s">
+        <v>94</v>
+      </c>
+      <c r="P60" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="Q60" s="24" t="s">
-        <v>124</v>
+      <c r="Q60" s="20" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="61" spans="2:18" ht="34">
-      <c r="C61" s="17"/>
+      <c r="C61" s="15"/>
       <c r="I61" s="11"/>
-      <c r="P61" s="36" t="s">
+      <c r="P61" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="Q61" s="24" t="s">
-        <v>124</v>
+      <c r="Q61" s="20" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="62" spans="2:18" ht="17">
-      <c r="B62" s="47"/>
-      <c r="C62" s="15"/>
+      <c r="B62" s="32"/>
+      <c r="C62" s="32"/>
       <c r="D62" s="1" t="s">
         <v>46</v>
       </c>
@@ -4389,7 +4375,7 @@
         <v>80</v>
       </c>
       <c r="I62" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J62" s="1" t="s">
         <v>8</v>
@@ -4409,21 +4395,21 @@
       <c r="O62" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="P62" s="36" t="s">
-        <v>129</v>
+      <c r="P62" s="23" t="s">
+        <v>128</v>
       </c>
       <c r="Q62" s="12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="63" spans="2:18" ht="34">
-      <c r="B63" s="47"/>
-      <c r="C63" s="15"/>
+      <c r="B63" s="32"/>
+      <c r="C63" s="32"/>
       <c r="D63" s="1" t="s">
         <v>46</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F63" s="1" t="s">
         <v>17</v>
@@ -4435,7 +4421,7 @@
         <v>1</v>
       </c>
       <c r="I63" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J63" s="1" t="s">
         <v>8</v>
@@ -4455,51 +4441,51 @@
       <c r="O63" s="1">
         <v>0</v>
       </c>
-      <c r="P63" s="36" t="s">
+      <c r="P63" s="23" t="s">
         <v>65</v>
       </c>
       <c r="Q63" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="64" spans="2:18" ht="17">
-      <c r="C64" s="17"/>
+      <c r="C64" s="15"/>
       <c r="I64" s="12"/>
-      <c r="P64" s="36" t="s">
+      <c r="P64" s="23" t="s">
         <v>66</v>
       </c>
       <c r="Q64" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="65" spans="2:18" ht="34">
-      <c r="C65" s="17"/>
+      <c r="C65" s="15"/>
       <c r="I65" s="12"/>
-      <c r="P65" s="36" t="s">
+      <c r="P65" s="23" t="s">
         <v>76</v>
       </c>
-      <c r="Q65" s="24" t="s">
-        <v>124</v>
+      <c r="Q65" s="20" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="66" spans="2:18" ht="34">
-      <c r="C66" s="17"/>
+      <c r="C66" s="15"/>
       <c r="I66" s="12"/>
-      <c r="P66" s="36" t="s">
+      <c r="P66" s="23" t="s">
         <v>67</v>
       </c>
       <c r="Q66" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="67" spans="2:18" ht="34">
-      <c r="B67" s="47"/>
-      <c r="C67" s="15"/>
+      <c r="B67" s="32"/>
+      <c r="C67" s="32"/>
       <c r="D67" s="1" t="s">
         <v>46</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F67" s="1" t="s">
         <v>17</v>
@@ -4508,10 +4494,10 @@
         <v>32</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I67" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J67" s="1" t="s">
         <v>8</v>
@@ -4529,43 +4515,43 @@
         <v>39</v>
       </c>
       <c r="O67" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="P67" s="36" t="s">
+        <v>94</v>
+      </c>
+      <c r="P67" s="23" t="s">
         <v>65</v>
       </c>
       <c r="Q67" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="68" spans="2:18" ht="17">
-      <c r="C68" s="22"/>
+      <c r="C68" s="18"/>
       <c r="I68" s="14"/>
-      <c r="P68" s="36" t="s">
+      <c r="P68" s="23" t="s">
         <v>66</v>
       </c>
       <c r="Q68" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="69" spans="2:18" ht="34">
-      <c r="C69" s="23"/>
+      <c r="C69" s="19"/>
       <c r="I69" s="14"/>
-      <c r="P69" s="36" t="s">
+      <c r="P69" s="23" t="s">
         <v>67</v>
       </c>
       <c r="Q69" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="70" spans="2:18" ht="34">
-      <c r="B70" s="47"/>
-      <c r="C70" s="27"/>
+      <c r="B70" s="32"/>
+      <c r="C70" s="46"/>
       <c r="D70" s="1" t="s">
         <v>37</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F70" s="1" t="s">
         <v>27</v>
@@ -4597,17 +4583,17 @@
       <c r="O70" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="P70" s="40" t="s">
-        <v>142</v>
+      <c r="P70" s="27" t="s">
+        <v>141</v>
       </c>
       <c r="Q70" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="R70" s="25"/>
+        <v>108</v>
+      </c>
+      <c r="R70" s="21"/>
     </row>
     <row r="71" spans="2:18" ht="17">
-      <c r="B71" s="47"/>
-      <c r="C71" s="15"/>
+      <c r="B71" s="32"/>
+      <c r="C71" s="32"/>
       <c r="D71" s="1" t="s">
         <v>37</v>
       </c>
@@ -4644,16 +4630,16 @@
       <c r="O71" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="P71" s="36" t="s">
-        <v>96</v>
+      <c r="P71" s="23" t="s">
+        <v>95</v>
       </c>
       <c r="Q71" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="72" spans="2:18" ht="17">
-      <c r="B72" s="47"/>
-      <c r="C72" s="15"/>
+      <c r="B72" s="32"/>
+      <c r="C72" s="32"/>
       <c r="D72" s="1" t="s">
         <v>37</v>
       </c>
@@ -4690,16 +4676,16 @@
       <c r="O72" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="P72" s="36" t="s">
+      <c r="P72" s="23" t="s">
         <v>43</v>
       </c>
       <c r="Q72" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="73" spans="2:18" ht="17">
-      <c r="B73" s="47"/>
-      <c r="C73" s="15"/>
+      <c r="B73" s="32"/>
+      <c r="C73" s="32"/>
       <c r="D73" s="1" t="s">
         <v>37</v>
       </c>
@@ -4736,17 +4722,17 @@
       <c r="O73" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="P73" s="36" t="s">
+      <c r="P73" s="23" t="s">
         <v>25</v>
       </c>
       <c r="Q73" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="R73" s="10"/>
     </row>
     <row r="74" spans="2:18" ht="17">
-      <c r="B74" s="47"/>
-      <c r="C74" s="15"/>
+      <c r="B74" s="32"/>
+      <c r="C74" s="32"/>
       <c r="D74" s="1" t="s">
         <v>37</v>
       </c>
@@ -4766,7 +4752,7 @@
         <v>11</v>
       </c>
       <c r="J74" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="K74" s="1" t="s">
         <v>8</v>
@@ -4783,21 +4769,21 @@
       <c r="O74" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="P74" s="36" t="s">
+      <c r="P74" s="23" t="s">
         <v>23</v>
       </c>
       <c r="Q74" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="75" spans="2:18" ht="17">
-      <c r="B75" s="47"/>
-      <c r="C75" s="15"/>
+      <c r="B75" s="32"/>
+      <c r="C75" s="32"/>
       <c r="D75" s="1" t="s">
         <v>37</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F75" s="1" t="s">
         <v>17</v>
@@ -4829,17 +4815,17 @@
       <c r="O75" s="1">
         <v>0</v>
       </c>
-      <c r="P75" s="36" t="s">
-        <v>125</v>
+      <c r="P75" s="23" t="s">
+        <v>124</v>
       </c>
       <c r="Q75" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="R75" s="10"/>
     </row>
     <row r="76" spans="2:18" ht="17">
-      <c r="B76" s="47"/>
-      <c r="C76" s="15"/>
+      <c r="B76" s="32"/>
+      <c r="C76" s="32"/>
       <c r="D76" s="1" t="s">
         <v>37</v>
       </c>
@@ -4876,16 +4862,16 @@
       <c r="O76" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="P76" s="36" t="s">
+      <c r="P76" s="23" t="s">
         <v>41</v>
       </c>
       <c r="Q76" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="77" spans="2:18" ht="17">
-      <c r="B77" s="47"/>
-      <c r="C77" s="15"/>
+      <c r="B77" s="32"/>
+      <c r="C77" s="32"/>
       <c r="D77" s="1" t="s">
         <v>37</v>
       </c>
@@ -4922,16 +4908,16 @@
       <c r="O77" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="P77" s="36" t="s">
+      <c r="P77" s="23" t="s">
         <v>44</v>
       </c>
       <c r="Q77" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="78" spans="2:18" ht="34">
-      <c r="B78" s="47"/>
-      <c r="C78" s="15"/>
+      <c r="B78" s="32"/>
+      <c r="C78" s="32"/>
       <c r="D78" s="1" t="s">
         <v>37</v>
       </c>
@@ -4968,22 +4954,22 @@
       <c r="O78" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="P78" s="40" t="s">
-        <v>138</v>
-      </c>
-      <c r="Q78" s="24" t="s">
-        <v>124</v>
-      </c>
-      <c r="R78" s="21"/>
+      <c r="P78" s="27" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q78" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="R78" s="17"/>
     </row>
     <row r="79" spans="2:18" ht="34">
-      <c r="B79" s="47"/>
-      <c r="C79" s="15"/>
+      <c r="B79" s="32"/>
+      <c r="C79" s="32"/>
       <c r="D79" s="1" t="s">
         <v>37</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F79" s="1" t="s">
         <v>17</v>
@@ -5015,16 +5001,16 @@
       <c r="O79" s="1">
         <v>0</v>
       </c>
-      <c r="P79" s="36" t="s">
+      <c r="P79" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="Q79" s="24" t="s">
-        <v>124</v>
+      <c r="Q79" s="20" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="80" spans="2:18" ht="17" customHeight="1">
-      <c r="B80" s="47"/>
-      <c r="C80" s="15"/>
+      <c r="B80" s="32"/>
+      <c r="C80" s="32"/>
       <c r="D80" s="1" t="s">
         <v>37</v>
       </c>
@@ -5061,21 +5047,21 @@
       <c r="O80" s="1">
         <v>0</v>
       </c>
-      <c r="P80" s="36" t="s">
+      <c r="P80" s="23" t="s">
         <v>20</v>
       </c>
       <c r="Q80" s="12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="81" spans="2:18" ht="17">
-      <c r="B81" s="47"/>
-      <c r="C81" s="15"/>
+      <c r="B81" s="32"/>
+      <c r="C81" s="32"/>
       <c r="D81" s="1" t="s">
         <v>37</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F81" s="1">
         <v>1</v>
@@ -5096,7 +5082,7 @@
         <v>37</v>
       </c>
       <c r="L81" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="M81" s="1">
         <v>0</v>
@@ -5107,28 +5093,28 @@
       <c r="O81" s="1">
         <v>0</v>
       </c>
-      <c r="P81" s="36" t="s">
-        <v>134</v>
+      <c r="P81" s="23" t="s">
+        <v>133</v>
       </c>
       <c r="Q81" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="R81" s="10"/>
     </row>
     <row r="82" spans="2:18" ht="17">
-      <c r="C82" s="17"/>
+      <c r="C82" s="15"/>
       <c r="I82" s="11"/>
-      <c r="P82" s="36" t="s">
+      <c r="P82" s="23" t="s">
         <v>58</v>
       </c>
       <c r="Q82" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="R82" s="26"/>
+        <v>125</v>
+      </c>
+      <c r="R82" s="22"/>
     </row>
     <row r="83" spans="2:18" ht="17">
-      <c r="B83" s="47"/>
-      <c r="C83" s="15"/>
+      <c r="B83" s="32"/>
+      <c r="C83" s="32"/>
       <c r="D83" s="1" t="s">
         <v>37</v>
       </c>
@@ -5165,55 +5151,55 @@
       <c r="O83" s="1">
         <v>0</v>
       </c>
-      <c r="P83" s="39" t="s">
+      <c r="P83" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="Q83" s="24" t="s">
-        <v>124</v>
+      <c r="Q83" s="20" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="84" spans="2:18" ht="17">
-      <c r="C84" s="17"/>
+      <c r="C84" s="15"/>
       <c r="I84" s="11"/>
-      <c r="P84" s="36" t="s">
-        <v>134</v>
-      </c>
-      <c r="Q84" s="24" t="s">
-        <v>124</v>
+      <c r="P84" s="23" t="s">
+        <v>133</v>
+      </c>
+      <c r="Q84" s="20" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="85" spans="2:18" ht="34">
-      <c r="C85" s="17"/>
+      <c r="C85" s="15"/>
       <c r="I85" s="11"/>
-      <c r="P85" s="36" t="s">
-        <v>101</v>
-      </c>
-      <c r="Q85" s="24" t="s">
-        <v>124</v>
+      <c r="P85" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q85" s="20" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="86" spans="2:18" ht="17">
-      <c r="C86" s="17"/>
+      <c r="C86" s="15"/>
       <c r="I86" s="11"/>
-      <c r="P86" s="36" t="s">
+      <c r="P86" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="Q86" s="24" t="s">
-        <v>124</v>
-      </c>
-      <c r="R86" s="26"/>
+      <c r="Q86" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="R86" s="22"/>
     </row>
     <row r="87" spans="2:18" ht="17">
-      <c r="B87" s="47"/>
-      <c r="C87" s="15"/>
+      <c r="B87" s="32"/>
+      <c r="C87" s="32"/>
       <c r="D87" s="1" t="s">
         <v>37</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G87" s="1" t="s">
         <v>18</v>
@@ -5231,10 +5217,10 @@
         <v>37</v>
       </c>
       <c r="L87" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="M87" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="N87" s="1" t="s">
         <v>39</v>
@@ -5242,27 +5228,27 @@
       <c r="O87" s="1">
         <v>0</v>
       </c>
-      <c r="P87" s="36" t="s">
-        <v>134</v>
+      <c r="P87" s="23" t="s">
+        <v>133</v>
       </c>
       <c r="Q87" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="88" spans="2:18" ht="17">
-      <c r="C88" s="17"/>
+      <c r="C88" s="15"/>
       <c r="I88" s="11"/>
-      <c r="P88" s="36" t="s">
+      <c r="P88" s="23" t="s">
         <v>58</v>
       </c>
       <c r="Q88" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="R88" s="26"/>
+        <v>125</v>
+      </c>
+      <c r="R88" s="22"/>
     </row>
     <row r="89" spans="2:18" ht="18" customHeight="1">
-      <c r="B89" s="47"/>
-      <c r="C89" s="15"/>
+      <c r="B89" s="32"/>
+      <c r="C89" s="32"/>
       <c r="D89" s="1" t="s">
         <v>37</v>
       </c>
@@ -5279,7 +5265,7 @@
         <v>0</v>
       </c>
       <c r="I89" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J89" s="1" t="s">
         <v>8</v>
@@ -5299,21 +5285,21 @@
       <c r="O89" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="P89" s="36" t="s">
-        <v>129</v>
+      <c r="P89" s="23" t="s">
+        <v>128</v>
       </c>
       <c r="Q89" s="12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="90" spans="2:18" ht="34">
-      <c r="B90" s="47"/>
-      <c r="C90" s="15"/>
+      <c r="B90" s="32"/>
+      <c r="C90" s="32"/>
       <c r="D90" s="1" t="s">
         <v>37</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F90" s="1" t="s">
         <v>31</v>
@@ -5325,7 +5311,7 @@
         <v>0</v>
       </c>
       <c r="I90" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J90" s="1" t="s">
         <v>8</v>
@@ -5334,7 +5320,7 @@
         <v>37</v>
       </c>
       <c r="L90" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="M90" s="1" t="s">
         <v>40</v>
@@ -5345,43 +5331,43 @@
       <c r="O90" s="1">
         <v>0</v>
       </c>
-      <c r="P90" s="36" t="s">
+      <c r="P90" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="Q90" s="24" t="s">
-        <v>124</v>
+      <c r="Q90" s="20" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="91" spans="2:18" ht="17">
-      <c r="C91" s="17"/>
+      <c r="C91" s="15"/>
       <c r="I91" s="11"/>
-      <c r="P91" s="36" t="s">
-        <v>134</v>
-      </c>
-      <c r="Q91" s="24" t="s">
-        <v>124</v>
-      </c>
-      <c r="R91" s="26"/>
+      <c r="P91" s="23" t="s">
+        <v>133</v>
+      </c>
+      <c r="Q91" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="R91" s="22"/>
     </row>
     <row r="92" spans="2:18" ht="17">
-      <c r="C92" s="17"/>
+      <c r="C92" s="15"/>
       <c r="I92" s="11"/>
-      <c r="P92" s="36" t="s">
+      <c r="P92" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="Q92" s="24" t="s">
-        <v>124</v>
+      <c r="Q92" s="20" t="s">
+        <v>123</v>
       </c>
       <c r="R92" s="10"/>
     </row>
     <row r="93" spans="2:18" ht="34">
-      <c r="B93" s="47"/>
-      <c r="C93" s="15"/>
+      <c r="B93" s="32"/>
+      <c r="C93" s="32"/>
       <c r="D93" s="1" t="s">
         <v>37</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F93" s="1">
         <v>0</v>
@@ -5393,7 +5379,7 @@
         <v>0</v>
       </c>
       <c r="I93" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J93" s="1" t="s">
         <v>8</v>
@@ -5402,49 +5388,49 @@
         <v>37</v>
       </c>
       <c r="L93" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="M93" s="1">
         <v>0</v>
       </c>
       <c r="N93" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="O93" s="1">
         <v>0</v>
       </c>
-      <c r="P93" s="36" t="s">
+      <c r="P93" s="23" t="s">
         <v>75</v>
       </c>
       <c r="Q93" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="94" spans="2:18" ht="17">
-      <c r="C94" s="17"/>
+      <c r="C94" s="15"/>
       <c r="I94" s="11"/>
-      <c r="P94" s="36" t="s">
-        <v>134</v>
+      <c r="P94" s="23" t="s">
+        <v>133</v>
       </c>
       <c r="Q94" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="R94" s="26"/>
+        <v>125</v>
+      </c>
+      <c r="R94" s="22"/>
     </row>
     <row r="95" spans="2:18" ht="17">
-      <c r="C95" s="17"/>
+      <c r="C95" s="15"/>
       <c r="I95" s="11"/>
-      <c r="P95" s="36" t="s">
+      <c r="P95" s="23" t="s">
         <v>57</v>
       </c>
       <c r="Q95" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="R95" s="10"/>
     </row>
     <row r="96" spans="2:18" ht="34">
-      <c r="B96" s="47"/>
-      <c r="C96" s="15"/>
+      <c r="B96" s="32"/>
+      <c r="C96" s="32"/>
       <c r="D96" s="1" t="s">
         <v>37</v>
       </c>
@@ -5461,7 +5447,7 @@
         <v>0</v>
       </c>
       <c r="I96" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J96" s="1" t="s">
         <v>8</v>
@@ -5481,63 +5467,63 @@
       <c r="O96" s="1">
         <v>0</v>
       </c>
-      <c r="P96" s="36" t="s">
+      <c r="P96" s="23" t="s">
         <v>75</v>
       </c>
       <c r="Q96" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="97" spans="3:18" ht="17">
-      <c r="C97" s="17"/>
+      <c r="C97" s="15"/>
       <c r="I97" s="14"/>
-      <c r="P97" s="39" t="s">
+      <c r="P97" s="26" t="s">
         <v>59</v>
       </c>
       <c r="Q97" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="98" spans="3:18" ht="17">
-      <c r="C98" s="17"/>
+      <c r="C98" s="15"/>
       <c r="I98" s="14"/>
-      <c r="P98" s="36" t="s">
-        <v>134</v>
+      <c r="P98" s="23" t="s">
+        <v>133</v>
       </c>
       <c r="Q98" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="R98" s="26"/>
+        <v>125</v>
+      </c>
+      <c r="R98" s="22"/>
     </row>
     <row r="99" spans="3:18" ht="34">
-      <c r="C99" s="17"/>
+      <c r="C99" s="15"/>
       <c r="I99" s="14"/>
-      <c r="P99" s="36" t="s">
-        <v>100</v>
+      <c r="P99" s="23" t="s">
+        <v>99</v>
       </c>
       <c r="Q99" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="100" spans="3:18" ht="17">
-      <c r="C100" s="17"/>
+      <c r="C100" s="15"/>
       <c r="I100" s="14"/>
-      <c r="P100" s="36" t="s">
+      <c r="P100" s="23" t="s">
         <v>77</v>
       </c>
       <c r="Q100" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="R100" s="10"/>
     </row>
     <row r="101" spans="3:18">
       <c r="I101" s="12"/>
-      <c r="P101" s="41"/>
+      <c r="P101" s="28"/>
       <c r="R101"/>
     </row>
     <row r="102" spans="3:18">
       <c r="I102" s="12"/>
-      <c r="P102" s="41"/>
+      <c r="P102" s="28"/>
       <c r="R102"/>
     </row>
     <row r="103" spans="3:18">
@@ -5568,5 +5554,6 @@
     <mergeCell ref="D1:M1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="30" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
WIP: The ThreadTeam test was originally constructed on hello.  However, when tested on other platforms, some of the wait loops were not adequate as they were only waiting on one piece of information while the test after the loop were checking multiple changes.  Based on this experience, reviewed the tests and attempted to make them more robust.  Improved timings as well.
These have only been tested on hello, so pending testing on other platforms.
</commit_message>
<xml_diff>
--- a/docs/RuntimeDesign.xlsx
+++ b/docs/RuntimeDesign.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10307"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jared/Projects/OrchestrationRuntime/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82816A65-3637-E941-B21C-E2CCC19555BA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{056FA51E-6D64-1748-B765-55AD5E646C19}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="17560" xr2:uid="{9B8D0C4A-3FF1-A04E-B8F8-B86CE3BC2D78}"/>
+    <workbookView xWindow="14180" yWindow="440" windowWidth="35820" windowHeight="27600" xr2:uid="{9B8D0C4A-3FF1-A04E-B8F8-B86CE3BC2D78}"/>
   </bookViews>
   <sheets>
     <sheet name="Design_1.0" sheetId="1" r:id="rId1"/>
@@ -1739,6 +1739,15 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
@@ -1768,15 +1777,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2098,8 +2098,8 @@
   <dimension ref="B1:R107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C96" sqref="C96"/>
+      <pane ySplit="5" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q52" sqref="Q52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2126,66 +2126,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" ht="16" customHeight="1">
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="37" t="s">
         <v>135</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="37" t="s">
         <v>136</v>
       </c>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="43"/>
-      <c r="K1" s="43"/>
-      <c r="L1" s="43"/>
-      <c r="M1" s="43"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
     </row>
     <row r="2" spans="2:18" ht="17" thickBot="1">
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
     </row>
     <row r="3" spans="2:18" ht="17" thickBot="1">
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="36" t="s">
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="39"/>
-      <c r="K3" s="36" t="s">
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="42"/>
+      <c r="K3" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="L3" s="37"/>
-      <c r="M3" s="37"/>
-      <c r="N3" s="38"/>
-      <c r="O3" s="39"/>
+      <c r="L3" s="40"/>
+      <c r="M3" s="40"/>
+      <c r="N3" s="41"/>
+      <c r="O3" s="42"/>
     </row>
     <row r="4" spans="2:18" ht="17" thickBot="1">
-      <c r="B4" s="34"/>
-      <c r="C4" s="34"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="37"/>
       <c r="D4" s="4"/>
-      <c r="E4" s="40" t="s">
+      <c r="E4" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="41"/>
-      <c r="G4" s="41"/>
-      <c r="H4" s="42"/>
+      <c r="F4" s="44"/>
+      <c r="G4" s="44"/>
+      <c r="H4" s="45"/>
       <c r="K4" s="4"/>
-      <c r="L4" s="40" t="s">
+      <c r="L4" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="M4" s="41"/>
-      <c r="N4" s="41"/>
-      <c r="O4" s="42"/>
+      <c r="M4" s="44"/>
+      <c r="N4" s="44"/>
+      <c r="O4" s="45"/>
     </row>
     <row r="5" spans="2:18" ht="18" thickBot="1">
-      <c r="B5" s="34"/>
-      <c r="C5" s="34"/>
+      <c r="B5" s="37"/>
+      <c r="C5" s="37"/>
       <c r="D5" s="4" t="s">
         <v>0</v>
       </c>
@@ -2231,10 +2231,10 @@
       <c r="R5" s="9"/>
     </row>
     <row r="6" spans="2:18" ht="17">
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="38" t="s">
         <v>78</v>
       </c>
-      <c r="C6" s="35"/>
+      <c r="C6" s="38"/>
       <c r="D6" s="16" t="s">
         <v>4</v>
       </c>
@@ -2281,7 +2281,7 @@
     </row>
     <row r="7" spans="2:18" ht="17">
       <c r="B7" s="32"/>
-      <c r="C7" s="44"/>
+      <c r="C7" s="34"/>
       <c r="D7" s="1" t="s">
         <v>4</v>
       </c>
@@ -2327,7 +2327,7 @@
     </row>
     <row r="8" spans="2:18" ht="17">
       <c r="B8" s="32"/>
-      <c r="C8" s="44"/>
+      <c r="C8" s="34"/>
       <c r="D8" s="1" t="s">
         <v>4</v>
       </c>
@@ -2560,7 +2560,7 @@
     </row>
     <row r="13" spans="2:18" ht="17">
       <c r="B13" s="32"/>
-      <c r="C13" s="45"/>
+      <c r="C13" s="35"/>
       <c r="D13" s="1" t="s">
         <v>4</v>
       </c>
@@ -2606,7 +2606,7 @@
     </row>
     <row r="14" spans="2:18" ht="17">
       <c r="B14" s="32"/>
-      <c r="C14" s="45"/>
+      <c r="C14" s="35"/>
       <c r="D14" s="1" t="s">
         <v>4</v>
       </c>
@@ -2653,7 +2653,7 @@
     </row>
     <row r="15" spans="2:18" ht="17">
       <c r="B15" s="32"/>
-      <c r="C15" s="45"/>
+      <c r="C15" s="35"/>
       <c r="D15" s="1" t="s">
         <v>4</v>
       </c>
@@ -2699,7 +2699,7 @@
     </row>
     <row r="16" spans="2:18" ht="34">
       <c r="B16" s="32"/>
-      <c r="C16" s="45"/>
+      <c r="C16" s="35"/>
       <c r="D16" s="1" t="s">
         <v>4</v>
       </c>
@@ -2745,7 +2745,7 @@
     </row>
     <row r="17" spans="2:18" ht="17">
       <c r="B17" s="32"/>
-      <c r="C17" s="45"/>
+      <c r="C17" s="35"/>
       <c r="D17" s="1" t="s">
         <v>4</v>
       </c>
@@ -2791,7 +2791,7 @@
     </row>
     <row r="18" spans="2:18" ht="17">
       <c r="B18" s="32"/>
-      <c r="C18" s="45"/>
+      <c r="C18" s="35"/>
       <c r="D18" s="1" t="s">
         <v>4</v>
       </c>
@@ -4119,8 +4119,8 @@
       <c r="P52" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="Q52" s="3" t="s">
-        <v>120</v>
+      <c r="Q52" s="20" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="53" spans="2:18" ht="34">
@@ -4546,7 +4546,7 @@
     </row>
     <row r="70" spans="2:18" ht="34">
       <c r="B70" s="32"/>
-      <c r="C70" s="46"/>
+      <c r="C70" s="36"/>
       <c r="D70" s="1" t="s">
         <v>37</v>
       </c>

</xml_diff>